<commit_message>
Add new table from Li, Zhang et al
</commit_message>
<xml_diff>
--- a/MUSCShield_form.xlsx
+++ b/MUSCShield_form.xlsx
@@ -720,7 +720,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="309">
   <si>
     <t>Shielding Calculations</t>
   </si>
@@ -1660,106 +1660,6 @@
   </si>
   <si>
     <t>Mean DAP/pt</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Table 1: Fitted results of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">, and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>g</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> for broad tungste-anode, aluminum-filter x-ray beams. Units of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> in mm^-1</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1868,6 +1768,71 @@
     <t>W/Al</t>
   </si>
   <si>
+    <t>W/Ag</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table V: Fitting parameters </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>g</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> for the transmission of the primary radiation generated by the combined workload distribution [Table IV(c).</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Table 1: Fitted results of </t>
     </r>
@@ -1926,7 +1891,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> for broad tungste-anode, silver-filter x-ray beams. Units of </t>
+      <t xml:space="preserve"> for broad tungsten-anode, silver-filter x-ray beams. Units of </t>
     </r>
     <r>
       <rPr>
@@ -1968,7 +1933,107 @@
     </r>
   </si>
   <si>
-    <t>W/Ag</t>
+    <r>
+      <t xml:space="preserve">Table 1: Fitted results of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>g</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> for broad tungsten-anode, aluminum-filter x-ray beams. Units of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in mm^-1</t>
+    </r>
+  </si>
+  <si>
+    <t>W/Rh, W/Ag, W/Al</t>
   </si>
 </sst>
 </file>
@@ -3551,6 +3616,9 @@
     <xf numFmtId="0" fontId="24" fillId="9" borderId="24" xfId="4" applyFill="1" applyBorder="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3595,9 +3663,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -13541,13 +13606,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E6" s="334" t="s">
+      <c r="E6" s="335" t="s">
         <v>263</v>
       </c>
-      <c r="F6" s="334"/>
-      <c r="G6" s="334"/>
-      <c r="H6" s="334"/>
-      <c r="I6" s="334"/>
+      <c r="F6" s="335"/>
+      <c r="G6" s="335"/>
+      <c r="H6" s="335"/>
+      <c r="I6" s="335"/>
     </row>
     <row r="7" spans="1:9" s="308" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="314" t="s">
@@ -13996,48 +14061,48 @@
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="B4" s="334" t="s">
+      <c r="B4" s="335" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="334"/>
-      <c r="D4" s="334"/>
-      <c r="E4" s="334"/>
-      <c r="F4" s="334"/>
-      <c r="G4" s="334" t="s">
+      <c r="C4" s="335"/>
+      <c r="D4" s="335"/>
+      <c r="E4" s="335"/>
+      <c r="F4" s="335"/>
+      <c r="G4" s="335" t="s">
         <v>95</v>
       </c>
-      <c r="H4" s="334"/>
-      <c r="I4" s="334"/>
-      <c r="J4" s="334"/>
-      <c r="K4" s="334"/>
-      <c r="L4" s="334" t="s">
+      <c r="H4" s="335"/>
+      <c r="I4" s="335"/>
+      <c r="J4" s="335"/>
+      <c r="K4" s="335"/>
+      <c r="L4" s="335" t="s">
         <v>52</v>
       </c>
-      <c r="M4" s="334"/>
-      <c r="N4" s="334"/>
-      <c r="O4" s="334"/>
-      <c r="P4" s="334"/>
-      <c r="Q4" s="334" t="s">
+      <c r="M4" s="335"/>
+      <c r="N4" s="335"/>
+      <c r="O4" s="335"/>
+      <c r="P4" s="335"/>
+      <c r="Q4" s="335" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="334"/>
-      <c r="S4" s="334"/>
-      <c r="T4" s="334"/>
-      <c r="U4" s="334"/>
-      <c r="V4" s="334" t="s">
+      <c r="R4" s="335"/>
+      <c r="S4" s="335"/>
+      <c r="T4" s="335"/>
+      <c r="U4" s="335"/>
+      <c r="V4" s="335" t="s">
         <v>96</v>
       </c>
-      <c r="W4" s="334"/>
-      <c r="X4" s="334"/>
-      <c r="Y4" s="334"/>
-      <c r="Z4" s="334"/>
-      <c r="AA4" s="334" t="s">
+      <c r="W4" s="335"/>
+      <c r="X4" s="335"/>
+      <c r="Y4" s="335"/>
+      <c r="Z4" s="335"/>
+      <c r="AA4" s="335" t="s">
         <v>58</v>
       </c>
-      <c r="AB4" s="334"/>
-      <c r="AC4" s="334"/>
-      <c r="AD4" s="334"/>
-      <c r="AE4" s="334"/>
+      <c r="AB4" s="335"/>
+      <c r="AC4" s="335"/>
+      <c r="AD4" s="335"/>
+      <c r="AE4" s="335"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -16793,42 +16858,42 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="336" t="s">
+      <c r="A3" s="337" t="s">
         <v>264</v>
       </c>
-      <c r="B3" s="334" t="s">
+      <c r="B3" s="335" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="334"/>
-      <c r="D3" s="334"/>
-      <c r="E3" s="334" t="s">
+      <c r="C3" s="335"/>
+      <c r="D3" s="335"/>
+      <c r="E3" s="335" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="334"/>
-      <c r="G3" s="334"/>
-      <c r="H3" s="334" t="s">
+      <c r="F3" s="335"/>
+      <c r="G3" s="335"/>
+      <c r="H3" s="335" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="334"/>
-      <c r="J3" s="334"/>
-      <c r="K3" s="334" t="s">
+      <c r="I3" s="335"/>
+      <c r="J3" s="335"/>
+      <c r="K3" s="335" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="334"/>
-      <c r="M3" s="334"/>
-      <c r="N3" s="334" t="s">
+      <c r="L3" s="335"/>
+      <c r="M3" s="335"/>
+      <c r="N3" s="335" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="334"/>
-      <c r="P3" s="334"/>
-      <c r="Q3" s="334" t="s">
+      <c r="O3" s="335"/>
+      <c r="P3" s="335"/>
+      <c r="Q3" s="335" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="334"/>
-      <c r="S3" s="334"/>
+      <c r="R3" s="335"/>
+      <c r="S3" s="335"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="336"/>
+      <c r="A4" s="337"/>
       <c r="B4" s="313" t="s">
         <v>40</v>
       </c>
@@ -17448,42 +17513,42 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="336" t="s">
+      <c r="A3" s="337" t="s">
         <v>264</v>
       </c>
-      <c r="B3" s="334" t="s">
+      <c r="B3" s="335" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="334"/>
-      <c r="D3" s="334"/>
-      <c r="E3" s="334" t="s">
+      <c r="C3" s="335"/>
+      <c r="D3" s="335"/>
+      <c r="E3" s="335" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="334"/>
-      <c r="G3" s="334"/>
-      <c r="H3" s="334" t="s">
+      <c r="F3" s="335"/>
+      <c r="G3" s="335"/>
+      <c r="H3" s="335" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="334"/>
-      <c r="J3" s="334"/>
-      <c r="K3" s="334" t="s">
+      <c r="I3" s="335"/>
+      <c r="J3" s="335"/>
+      <c r="K3" s="335" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="334"/>
-      <c r="M3" s="334"/>
-      <c r="N3" s="334" t="s">
+      <c r="L3" s="335"/>
+      <c r="M3" s="335"/>
+      <c r="N3" s="335" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="334"/>
-      <c r="P3" s="334"/>
-      <c r="Q3" s="334" t="s">
+      <c r="O3" s="335"/>
+      <c r="P3" s="335"/>
+      <c r="Q3" s="335" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="334"/>
-      <c r="S3" s="334"/>
+      <c r="R3" s="335"/>
+      <c r="S3" s="335"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="336"/>
+      <c r="A4" s="337"/>
       <c r="B4" s="313" t="s">
         <v>40</v>
       </c>
@@ -18440,53 +18505,53 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="309" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="337" t="s">
-        <v>306</v>
-      </c>
-      <c r="B2" s="334" t="s">
+      <c r="A2" s="322" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" s="335" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="334"/>
-      <c r="D2" s="334"/>
-      <c r="E2" s="334" t="s">
+      <c r="C2" s="335"/>
+      <c r="D2" s="335"/>
+      <c r="E2" s="335" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="334"/>
-      <c r="G2" s="334"/>
-      <c r="H2" s="334" t="s">
+      <c r="F2" s="335"/>
+      <c r="G2" s="335"/>
+      <c r="H2" s="335" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="334"/>
-      <c r="J2" s="334"/>
-      <c r="K2" s="334" t="s">
+      <c r="I2" s="335"/>
+      <c r="J2" s="335"/>
+      <c r="K2" s="335" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="334"/>
-      <c r="M2" s="334"/>
-      <c r="N2" s="334" t="s">
+      <c r="L2" s="335"/>
+      <c r="M2" s="335"/>
+      <c r="N2" s="335" t="s">
         <v>96</v>
       </c>
-      <c r="O2" s="334"/>
-      <c r="P2" s="334"/>
-      <c r="Q2" s="334" t="s">
+      <c r="O2" s="335"/>
+      <c r="P2" s="335"/>
+      <c r="Q2" s="335" t="s">
         <v>58</v>
       </c>
-      <c r="R2" s="334"/>
-      <c r="S2" s="334"/>
+      <c r="R2" s="335"/>
+      <c r="S2" s="335"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -18784,7 +18849,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="337" t="s">
+      <c r="A9" s="322" t="s">
         <v>296</v>
       </c>
       <c r="B9" s="309" t="s">
@@ -18793,43 +18858,43 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="309" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="337" t="s">
-        <v>304</v>
-      </c>
-      <c r="B12" s="334" t="s">
+      <c r="A12" s="322" t="s">
+        <v>303</v>
+      </c>
+      <c r="B12" s="335" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="334"/>
-      <c r="D12" s="334"/>
-      <c r="E12" s="334" t="s">
+      <c r="C12" s="335"/>
+      <c r="D12" s="335"/>
+      <c r="E12" s="335" t="s">
         <v>95</v>
       </c>
-      <c r="F12" s="334"/>
-      <c r="G12" s="334"/>
-      <c r="H12" s="334" t="s">
+      <c r="F12" s="335"/>
+      <c r="G12" s="335"/>
+      <c r="H12" s="335" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="334"/>
-      <c r="J12" s="334"/>
-      <c r="K12" s="334" t="s">
+      <c r="I12" s="335"/>
+      <c r="J12" s="335"/>
+      <c r="K12" s="335" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="334"/>
-      <c r="M12" s="334"/>
-      <c r="N12" s="334" t="s">
+      <c r="L12" s="335"/>
+      <c r="M12" s="335"/>
+      <c r="N12" s="335" t="s">
         <v>96</v>
       </c>
-      <c r="O12" s="334"/>
-      <c r="P12" s="334"/>
-      <c r="Q12" s="334" t="s">
+      <c r="O12" s="335"/>
+      <c r="P12" s="335"/>
+      <c r="Q12" s="335" t="s">
         <v>58</v>
       </c>
-      <c r="R12" s="334"/>
-      <c r="S12" s="334"/>
+      <c r="R12" s="335"/>
+      <c r="S12" s="335"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -19245,7 +19310,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A21" s="337" t="s">
+      <c r="A21" s="322" t="s">
         <v>296</v>
       </c>
       <c r="B21" s="309" t="s">
@@ -19254,43 +19319,43 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="309" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A24" s="322" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A24" s="337" t="s">
-        <v>303</v>
-      </c>
-      <c r="B24" s="334" t="s">
+      <c r="B24" s="335" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="334"/>
-      <c r="D24" s="334"/>
-      <c r="E24" s="334" t="s">
+      <c r="C24" s="335"/>
+      <c r="D24" s="335"/>
+      <c r="E24" s="335" t="s">
         <v>95</v>
       </c>
-      <c r="F24" s="334"/>
-      <c r="G24" s="334"/>
-      <c r="H24" s="334" t="s">
+      <c r="F24" s="335"/>
+      <c r="G24" s="335"/>
+      <c r="H24" s="335" t="s">
         <v>52</v>
       </c>
-      <c r="I24" s="334"/>
-      <c r="J24" s="334"/>
-      <c r="K24" s="334" t="s">
+      <c r="I24" s="335"/>
+      <c r="J24" s="335"/>
+      <c r="K24" s="335" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="334"/>
-      <c r="M24" s="334"/>
-      <c r="N24" s="334" t="s">
+      <c r="L24" s="335"/>
+      <c r="M24" s="335"/>
+      <c r="N24" s="335" t="s">
         <v>96</v>
       </c>
-      <c r="O24" s="334"/>
-      <c r="P24" s="334"/>
-      <c r="Q24" s="334" t="s">
+      <c r="O24" s="335"/>
+      <c r="P24" s="335"/>
+      <c r="Q24" s="335" t="s">
         <v>58</v>
       </c>
-      <c r="R24" s="334"/>
-      <c r="S24" s="334"/>
+      <c r="R24" s="335"/>
+      <c r="S24" s="335"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -19588,15 +19653,246 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A31" s="337" t="s">
+      <c r="A31" s="322" t="s">
         <v>296</v>
       </c>
       <c r="B31" s="309" t="s">
         <v>298</v>
       </c>
     </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A33" s="309" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C34" s="335" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="335"/>
+      <c r="E34" s="335"/>
+      <c r="F34" s="335" t="s">
+        <v>95</v>
+      </c>
+      <c r="G34" s="335"/>
+      <c r="H34" s="335"/>
+      <c r="I34" s="335" t="s">
+        <v>52</v>
+      </c>
+      <c r="J34" s="335"/>
+      <c r="K34" s="335"/>
+      <c r="L34" s="335" t="s">
+        <v>54</v>
+      </c>
+      <c r="M34" s="335"/>
+      <c r="N34" s="335"/>
+      <c r="O34" s="335" t="s">
+        <v>96</v>
+      </c>
+      <c r="P34" s="335"/>
+      <c r="Q34" s="335"/>
+      <c r="R34" s="335" t="s">
+        <v>58</v>
+      </c>
+      <c r="S34" s="335"/>
+      <c r="T34" s="335"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C35" s="313" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="313" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="313" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="313" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="313" t="s">
+        <v>41</v>
+      </c>
+      <c r="H35" s="313" t="s">
+        <v>42</v>
+      </c>
+      <c r="I35" s="313" t="s">
+        <v>40</v>
+      </c>
+      <c r="J35" s="313" t="s">
+        <v>41</v>
+      </c>
+      <c r="K35" s="313" t="s">
+        <v>42</v>
+      </c>
+      <c r="L35" s="313" t="s">
+        <v>40</v>
+      </c>
+      <c r="M35" s="313" t="s">
+        <v>41</v>
+      </c>
+      <c r="N35" s="313" t="s">
+        <v>42</v>
+      </c>
+      <c r="O35" s="313" t="s">
+        <v>40</v>
+      </c>
+      <c r="P35" s="313" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q35" s="313" t="s">
+        <v>42</v>
+      </c>
+      <c r="R35" s="313" t="s">
+        <v>40</v>
+      </c>
+      <c r="S35" s="313" t="s">
+        <v>41</v>
+      </c>
+      <c r="T35" s="313" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="C36">
+        <v>13.33</v>
+      </c>
+      <c r="D36">
+        <v>65.260000000000005</v>
+      </c>
+      <c r="E36">
+        <v>0.21190000000000001</v>
+      </c>
+      <c r="F36">
+        <v>0.1338</v>
+      </c>
+      <c r="G36">
+        <v>0.63460000000000005</v>
+      </c>
+      <c r="H36">
+        <v>0.37769999999999998</v>
+      </c>
+      <c r="I36">
+        <v>6.343E-2</v>
+      </c>
+      <c r="J36">
+        <v>0.34150000000000003</v>
+      </c>
+      <c r="K36">
+        <v>0.37080000000000002</v>
+      </c>
+      <c r="L36">
+        <v>2.56</v>
+      </c>
+      <c r="M36">
+        <v>13.66</v>
+      </c>
+      <c r="N36">
+        <v>0.27239999999999998</v>
+      </c>
+      <c r="O36">
+        <v>0.1444</v>
+      </c>
+      <c r="P36">
+        <v>0.68579999999999997</v>
+      </c>
+      <c r="Q36">
+        <v>0.37140000000000001</v>
+      </c>
+      <c r="R36">
+        <v>1.285E-2</v>
+      </c>
+      <c r="S36">
+        <v>1.41E-2</v>
+      </c>
+      <c r="T36">
+        <v>0.3422</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>303</v>
+      </c>
+      <c r="C37">
+        <v>12.22</v>
+      </c>
+      <c r="D37">
+        <v>53.6</v>
+      </c>
+      <c r="E37">
+        <v>0.1948</v>
+      </c>
+      <c r="F37">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="G37">
+        <v>0.50849999999999995</v>
+      </c>
+      <c r="H37">
+        <v>0.39279999999999998</v>
+      </c>
+      <c r="I37">
+        <v>6.3539999999999999E-2</v>
+      </c>
+      <c r="J37">
+        <v>0.27439999999999998</v>
+      </c>
+      <c r="K37">
+        <v>0.38429999999999997</v>
+      </c>
+      <c r="L37">
+        <v>2.4220000000000002</v>
+      </c>
+      <c r="M37">
+        <v>10.91</v>
+      </c>
+      <c r="N37">
+        <v>0.2576</v>
+      </c>
+      <c r="O37">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="P37">
+        <v>0.54120000000000001</v>
+      </c>
+      <c r="Q37">
+        <v>0.37990000000000002</v>
+      </c>
+      <c r="R37">
+        <v>1.2970000000000001E-2</v>
+      </c>
+      <c r="S37">
+        <v>1.057E-2</v>
+      </c>
+      <c r="T37">
+        <v>0.40100000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A39" s="322" t="s">
+        <v>296</v>
+      </c>
+      <c r="B39" s="309" t="s">
+        <v>297</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="24">
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
     <mergeCell ref="Q24:S24"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="E12:G12"/>
@@ -19609,12 +19905,6 @@
     <mergeCell ref="H24:J24"/>
     <mergeCell ref="K24:M24"/>
     <mergeCell ref="N24:P24"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19634,20 +19924,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1" s="322" t="s">
+      <c r="B1" s="323" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="322"/>
-      <c r="D1" s="322" t="s">
+      <c r="C1" s="323"/>
+      <c r="D1" s="323" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="322"/>
-      <c r="F1" s="322"/>
-      <c r="H1" s="323" t="s">
+      <c r="E1" s="323"/>
+      <c r="F1" s="323"/>
+      <c r="H1" s="324" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="323"/>
-      <c r="J1" s="323"/>
+      <c r="I1" s="324"/>
+      <c r="J1" s="324"/>
       <c r="K1" s="294"/>
       <c r="M1" s="295"/>
     </row>
@@ -19722,11 +20012,11 @@
       <c r="D5" s="318"/>
       <c r="E5" s="318"/>
       <c r="F5" s="318"/>
-      <c r="H5" s="324" t="s">
+      <c r="H5" s="325" t="s">
         <v>185</v>
       </c>
-      <c r="I5" s="324"/>
-      <c r="J5" s="323"/>
+      <c r="I5" s="325"/>
+      <c r="J5" s="324"/>
       <c r="K5" s="294"/>
       <c r="M5" s="295"/>
     </row>
@@ -21015,14 +21305,14 @@
       <c r="M18" s="265"/>
       <c r="N18" s="264"/>
       <c r="P18" s="279"/>
-      <c r="Q18" s="325" t="s">
+      <c r="Q18" s="326" t="s">
         <v>174</v>
       </c>
-      <c r="R18" s="325"/>
-      <c r="S18" s="325"/>
-      <c r="T18" s="325"/>
-      <c r="U18" s="325"/>
-      <c r="V18" s="326"/>
+      <c r="R18" s="326"/>
+      <c r="S18" s="326"/>
+      <c r="T18" s="326"/>
+      <c r="U18" s="326"/>
+      <c r="V18" s="327"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="215"/>
@@ -21053,16 +21343,16 @@
       </c>
       <c r="N19" s="276"/>
       <c r="P19" s="215"/>
-      <c r="Q19" s="327" t="s">
+      <c r="Q19" s="328" t="s">
         <v>173</v>
       </c>
-      <c r="R19" s="327"/>
-      <c r="S19" s="327"/>
-      <c r="T19" s="328" t="s">
+      <c r="R19" s="328"/>
+      <c r="S19" s="328"/>
+      <c r="T19" s="329" t="s">
         <v>95</v>
       </c>
-      <c r="U19" s="328"/>
-      <c r="V19" s="329"/>
+      <c r="U19" s="329"/>
+      <c r="V19" s="330"/>
     </row>
     <row r="20" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="215"/>
@@ -21259,14 +21549,14 @@
       <c r="N24" s="216"/>
       <c r="O24" s="216"/>
       <c r="P24" s="254"/>
-      <c r="Q24" s="325" t="s">
+      <c r="Q24" s="326" t="s">
         <v>174</v>
       </c>
-      <c r="R24" s="325"/>
-      <c r="S24" s="325"/>
-      <c r="T24" s="325"/>
-      <c r="U24" s="325"/>
-      <c r="V24" s="326"/>
+      <c r="R24" s="326"/>
+      <c r="S24" s="326"/>
+      <c r="T24" s="326"/>
+      <c r="U24" s="326"/>
+      <c r="V24" s="327"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="223" t="s">
@@ -21352,7 +21642,7 @@
       <c r="H27" s="249" t="s">
         <v>48</v>
       </c>
-      <c r="J27" s="330" t="s">
+      <c r="J27" s="331" t="s">
         <v>163</v>
       </c>
       <c r="K27" s="210" t="s">
@@ -21415,7 +21705,7 @@
       <c r="H28" s="246" t="s">
         <v>122</v>
       </c>
-      <c r="J28" s="330"/>
+      <c r="J28" s="331"/>
       <c r="K28" s="210" t="s">
         <v>184</v>
       </c>
@@ -22739,7 +23029,7 @@
       <c r="E18" s="167" t="s">
         <v>120</v>
       </c>
-      <c r="F18" s="331" t="s">
+      <c r="F18" s="332" t="s">
         <v>121</v>
       </c>
       <c r="G18" s="167"/>
@@ -22789,7 +23079,7 @@
       <c r="E19" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="F19" s="331"/>
+      <c r="F19" s="332"/>
       <c r="G19" s="167" t="s">
         <v>48</v>
       </c>
@@ -22822,22 +23112,22 @@
       <c r="E20" s="168" t="s">
         <v>182</v>
       </c>
-      <c r="F20" s="332"/>
+      <c r="F20" s="333"/>
       <c r="G20" s="168" t="s">
         <v>122</v>
       </c>
       <c r="H20" s="168" t="s">
         <v>118</v>
       </c>
-      <c r="L20" s="333" t="s">
+      <c r="L20" s="334" t="s">
         <v>123</v>
       </c>
-      <c r="M20" s="333"/>
-      <c r="N20" s="333"/>
-      <c r="O20" s="333"/>
-      <c r="P20" s="333"/>
-      <c r="Q20" s="333"/>
-      <c r="R20" s="333"/>
+      <c r="M20" s="334"/>
+      <c r="N20" s="334"/>
+      <c r="O20" s="334"/>
+      <c r="P20" s="334"/>
+      <c r="Q20" s="334"/>
+      <c r="R20" s="334"/>
       <c r="T20" s="158">
         <v>1.1906250009999999</v>
       </c>
@@ -26838,16 +27128,16 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="334" t="s">
+      <c r="B3" s="335" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="334"/>
-      <c r="D3" s="334"/>
-      <c r="E3" s="334" t="s">
+      <c r="C3" s="335"/>
+      <c r="D3" s="335"/>
+      <c r="E3" s="335" t="s">
         <v>231</v>
       </c>
-      <c r="F3" s="334"/>
-      <c r="G3" s="334"/>
+      <c r="F3" s="335"/>
+      <c r="G3" s="335"/>
     </row>
     <row r="4" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="314" t="s">
@@ -27694,11 +27984,11 @@
       <c r="A30" t="s">
         <v>242</v>
       </c>
-      <c r="B30" s="334">
+      <c r="B30" s="335">
         <v>110</v>
       </c>
-      <c r="C30" s="334"/>
-      <c r="D30" s="334"/>
+      <c r="C30" s="335"/>
+      <c r="D30" s="335"/>
       <c r="E30">
         <v>18</v>
       </c>
@@ -27753,14 +28043,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="335" t="s">
+      <c r="C3" s="336" t="s">
         <v>245</v>
       </c>
-      <c r="D3" s="335"/>
-      <c r="E3" s="335" t="s">
+      <c r="D3" s="336"/>
+      <c r="E3" s="336" t="s">
         <v>246</v>
       </c>
-      <c r="F3" s="335"/>
+      <c r="F3" s="336"/>
     </row>
     <row r="4" spans="1:6" s="308" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="314" t="s">

</xml_diff>

<commit_message>
Add tab for PET calcs
</commit_message>
<xml_diff>
--- a/MUSCShield_form.xlsx
+++ b/MUSCShield_form.xlsx
@@ -9,55 +9,57 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="9720" windowHeight="3270" tabRatio="688" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="9720" windowHeight="3270" tabRatio="688" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
     <sheet name="RadFluoro" sheetId="5" r:id="rId2"/>
     <sheet name="CT" sheetId="4" r:id="rId3"/>
-    <sheet name="ShieldEvaluation" sheetId="2" r:id="rId4"/>
-    <sheet name="FitParameters" sheetId="3" r:id="rId5"/>
-    <sheet name="NCRP147_4.1" sheetId="16" r:id="rId6"/>
-    <sheet name="NCRP147_4.2" sheetId="17" r:id="rId7"/>
-    <sheet name="NCRP147_4.3" sheetId="18" r:id="rId8"/>
-    <sheet name="NCRP147_4.4" sheetId="19" r:id="rId9"/>
-    <sheet name="NCRP147_4.5" sheetId="26" r:id="rId10"/>
-    <sheet name="NCRP147_4.6" sheetId="27" r:id="rId11"/>
-    <sheet name="NCRP147_4.7" sheetId="20" r:id="rId12"/>
-    <sheet name="NCRP147_5.2" sheetId="21" r:id="rId13"/>
-    <sheet name="NCRP147_A1" sheetId="22" r:id="rId14"/>
-    <sheet name="NCRP147_B1" sheetId="23" r:id="rId15"/>
-    <sheet name="NCRP147_C1" sheetId="24" r:id="rId16"/>
-    <sheet name="W_Rh_Al_Ag" sheetId="25" r:id="rId17"/>
+    <sheet name="PET" sheetId="33" r:id="rId4"/>
+    <sheet name="ShieldEvaluation" sheetId="2" r:id="rId5"/>
+    <sheet name="FitParameters" sheetId="3" r:id="rId6"/>
+    <sheet name="NCRP147_4.1" sheetId="16" r:id="rId7"/>
+    <sheet name="NCRP147_4.2" sheetId="17" r:id="rId8"/>
+    <sheet name="NCRP147_4.3" sheetId="18" r:id="rId9"/>
+    <sheet name="NCRP147_4.4" sheetId="19" r:id="rId10"/>
+    <sheet name="NCRP147_4.5" sheetId="26" r:id="rId11"/>
+    <sheet name="NCRP147_4.6" sheetId="27" r:id="rId12"/>
+    <sheet name="NCRP147_4.7" sheetId="20" r:id="rId13"/>
+    <sheet name="NCRP147_5.2" sheetId="21" r:id="rId14"/>
+    <sheet name="NCRP147_A1" sheetId="22" r:id="rId15"/>
+    <sheet name="NCRP147_B1" sheetId="23" r:id="rId16"/>
+    <sheet name="NCRP147_C1" sheetId="24" r:id="rId17"/>
+    <sheet name="W_Rh_Al_Ag" sheetId="25" r:id="rId18"/>
+    <sheet name="AAPMTG108" sheetId="32" r:id="rId19"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId18"/>
-    <externalReference r:id="rId19"/>
+    <externalReference r:id="rId20"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="FitParams">FitParameters!$A$5:$AF$30</definedName>
     <definedName name="inch_value">Table!$AF$6:$AF$41</definedName>
-    <definedName name="minimum_Pb" localSheetId="9">[1]Table!$AG$6:$AG$41</definedName>
-    <definedName name="minimum_Pb" localSheetId="10">[2]Table!$AG$6:$AG$41</definedName>
+    <definedName name="minimum_Pb" localSheetId="10">[1]Table!$AG$6:$AG$41</definedName>
+    <definedName name="minimum_Pb" localSheetId="11">[2]Table!$AG$6:$AG$41</definedName>
     <definedName name="minimum_Pb">Table!$AG$6:$AG$41</definedName>
-    <definedName name="mm_value" localSheetId="9">[1]Table!$AE$6:$AE$41</definedName>
-    <definedName name="mm_value" localSheetId="10">[2]Table!$AE$6:$AE$41</definedName>
+    <definedName name="mm_value" localSheetId="10">[1]Table!$AE$6:$AE$41</definedName>
+    <definedName name="mm_value" localSheetId="11">[2]Table!$AE$6:$AE$41</definedName>
     <definedName name="mm_value">Table!$AE$6:$AE$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">CT!$A$1:$V$50</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">RadFluoro!$A$1:$J$40</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">ShieldEvaluation!$A$1:$H$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">ShieldEvaluation!$A$1:$H$34</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Table!$A$1:$N$112</definedName>
-    <definedName name="RefDist" localSheetId="9">[1]ShieldEvaluation!$F$16</definedName>
-    <definedName name="RefDist" localSheetId="10">[2]ShieldEvaluation!$F$16</definedName>
+    <definedName name="RefDist" localSheetId="10">[1]ShieldEvaluation!$F$16</definedName>
+    <definedName name="RefDist" localSheetId="11">[2]ShieldEvaluation!$F$16</definedName>
     <definedName name="RefDist">ShieldEvaluation!$F$16</definedName>
-    <definedName name="RefExp" localSheetId="9">[1]ShieldEvaluation!$G$16</definedName>
-    <definedName name="RefExp" localSheetId="10">[2]ShieldEvaluation!$G$16</definedName>
+    <definedName name="RefExp" localSheetId="10">[1]ShieldEvaluation!$G$16</definedName>
+    <definedName name="RefExp" localSheetId="11">[2]ShieldEvaluation!$G$16</definedName>
     <definedName name="RefExp">ShieldEvaluation!$G$16</definedName>
-    <definedName name="RefkV" localSheetId="9">[1]ShieldEvaluation!$C$16</definedName>
-    <definedName name="RefkV" localSheetId="10">[2]ShieldEvaluation!$C$16</definedName>
+    <definedName name="RefkV" localSheetId="10">[1]ShieldEvaluation!$C$16</definedName>
+    <definedName name="RefkV" localSheetId="11">[2]ShieldEvaluation!$C$16</definedName>
     <definedName name="RefkV">ShieldEvaluation!$C$16</definedName>
-    <definedName name="RefOutput" localSheetId="9">[1]ShieldEvaluation!$H$16</definedName>
-    <definedName name="RefOutput" localSheetId="10">[2]ShieldEvaluation!$H$16</definedName>
+    <definedName name="RefOutput" localSheetId="10">[1]ShieldEvaluation!$H$16</definedName>
+    <definedName name="RefOutput" localSheetId="11">[2]ShieldEvaluation!$H$16</definedName>
     <definedName name="RefOutput">ShieldEvaluation!$H$16</definedName>
   </definedNames>
   <calcPr calcId="162913" iterateCount="1"/>
@@ -471,6 +473,136 @@
     <author>Eugene Mah</author>
   </authors>
   <commentList>
+    <comment ref="F11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Average uptake activity while being scanned. Assumes patient transmission factor of 0.64</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Patient activity at the end of the uptake period. Assumes patient transmission factor of 0.64</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Patient activity post-void. Assumes 0.85 activity retention factor.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Average activity during scanning period.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Patient activity after scan completion</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eugene Mah</author>
+  </authors>
+  <commentList>
     <comment ref="L11" authorId="0" shapeId="0">
       <text>
         <r>
@@ -738,7 +870,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="368">
   <si>
     <t>Shielding Calculations</t>
   </si>
@@ -2082,6 +2214,250 @@
   </si>
   <si>
     <t>Steel (mm)</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Table V: Fitting parameter for broad beam 511 keV transmission data.</t>
+  </si>
+  <si>
+    <t>Madsen MT, Anderson JA, et al., "AAPM Task Group 108: PET and PET/CT Shielding Requirements", MedPhys 33(1) 4-15</t>
+  </si>
+  <si>
+    <t>Table I: Physical properties of commonly used PET radionuclides</t>
+  </si>
+  <si>
+    <t>Nuclide</t>
+  </si>
+  <si>
+    <t>Decay mode</t>
+  </si>
+  <si>
+    <t>Max positron energy (MeV)</t>
+  </si>
+  <si>
+    <t>Photon emission (keV)</t>
+  </si>
+  <si>
+    <t>Photons/decay</t>
+  </si>
+  <si>
+    <t>C-11</t>
+  </si>
+  <si>
+    <t>T1/2 (min)</t>
+  </si>
+  <si>
+    <t>N-13</t>
+  </si>
+  <si>
+    <t>O-15</t>
+  </si>
+  <si>
+    <t>F-18</t>
+  </si>
+  <si>
+    <t>Cu-64</t>
+  </si>
+  <si>
+    <t>511, 1346</t>
+  </si>
+  <si>
+    <t>Ga-68</t>
+  </si>
+  <si>
+    <t>Rb-82</t>
+  </si>
+  <si>
+    <t>511, 776</t>
+  </si>
+  <si>
+    <t>1.9, 0.13</t>
+  </si>
+  <si>
+    <t>0.38, 0.005</t>
+  </si>
+  <si>
+    <t>I-124</t>
+  </si>
+  <si>
+    <t>1.54, 2.17</t>
+  </si>
+  <si>
+    <t>511, 603, 1693</t>
+  </si>
+  <si>
+    <t>0.5, 0.62, 0.3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>+, EC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">-, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>+, EC</t>
+    </r>
+  </si>
+  <si>
+    <t>Table II: Effective dose equivalent dose rate constants for commonly used PET radionuclides</t>
+  </si>
+  <si>
+    <t>Dose rate constant</t>
+  </si>
+  <si>
+    <t>1h integrated dose</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Sv-m^2/MBq-h</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Sv-m^2/MBq</t>
+    </r>
+  </si>
+  <si>
+    <t>Shielding Calculation</t>
+  </si>
+  <si>
+    <t>Activity calculations</t>
+  </si>
+  <si>
+    <t>Isotope</t>
+  </si>
+  <si>
+    <t>End scan activity (MBq)</t>
+  </si>
+  <si>
+    <t>Administered activity (MBq)</t>
+  </si>
+  <si>
+    <t>Uptake duration (min)</t>
+  </si>
+  <si>
+    <t>End uptake activity (MBq)</t>
+  </si>
+  <si>
+    <t>Post-void activity (MBq)</t>
+  </si>
+  <si>
+    <t>Avg Uptake activity (MBq)</t>
+  </si>
+  <si>
+    <t>Scan time (min)</t>
+  </si>
+  <si>
+    <t>Half life (min)</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Pts/week</t>
+  </si>
+  <si>
+    <t>Avg scan activity (MBq)</t>
+  </si>
+  <si>
+    <t>Source locations</t>
   </si>
 </sst>
 </file>
@@ -2269,7 +2645,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2321,6 +2697,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2853,7 +3235,7 @@
     </xf>
     <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="340">
+  <cellXfs count="360">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -3667,6 +4049,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3715,7 +4101,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3727,6 +4173,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4529,9 +4981,7 @@
       <sheetData sheetId="3"/>
       <sheetData sheetId="4">
         <row r="16">
-          <cell r="H16" t="str">
-            <v/>
-          </cell>
+          <cell r="H16"/>
         </row>
       </sheetData>
       <sheetData sheetId="5"/>
@@ -4926,7 +5376,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT112"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:J5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14292,6 +14744,70 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="306" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B5">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B6">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>256</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -14367,11 +14883,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -14386,9 +14902,9 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="339"/>
-      <c r="C2" s="339"/>
-      <c r="D2" s="339"/>
+      <c r="B2" s="324"/>
+      <c r="C2" s="324"/>
+      <c r="D2" s="324"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -14437,7 +14953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
@@ -14477,13 +14993,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E6" s="336" t="s">
+      <c r="E6" s="338" t="s">
         <v>262</v>
       </c>
-      <c r="F6" s="336"/>
-      <c r="G6" s="336"/>
-      <c r="H6" s="336"/>
-      <c r="I6" s="336"/>
+      <c r="F6" s="338"/>
+      <c r="G6" s="338"/>
+      <c r="H6" s="338"/>
+      <c r="I6" s="338"/>
     </row>
     <row r="7" spans="1:9" s="305" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="311" t="s">
@@ -14810,7 +15326,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -14916,12 +15432,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="A4" sqref="A4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14932,48 +15448,48 @@
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="B4" s="336" t="s">
+      <c r="B4" s="338" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="336"/>
-      <c r="D4" s="336"/>
-      <c r="E4" s="336"/>
-      <c r="F4" s="336"/>
-      <c r="G4" s="336" t="s">
+      <c r="C4" s="338"/>
+      <c r="D4" s="338"/>
+      <c r="E4" s="338"/>
+      <c r="F4" s="338"/>
+      <c r="G4" s="338" t="s">
         <v>95</v>
       </c>
-      <c r="H4" s="336"/>
-      <c r="I4" s="336"/>
-      <c r="J4" s="336"/>
-      <c r="K4" s="336"/>
-      <c r="L4" s="336" t="s">
+      <c r="H4" s="338"/>
+      <c r="I4" s="338"/>
+      <c r="J4" s="338"/>
+      <c r="K4" s="338"/>
+      <c r="L4" s="338" t="s">
         <v>52</v>
       </c>
-      <c r="M4" s="336"/>
-      <c r="N4" s="336"/>
-      <c r="O4" s="336"/>
-      <c r="P4" s="336"/>
-      <c r="Q4" s="336" t="s">
+      <c r="M4" s="338"/>
+      <c r="N4" s="338"/>
+      <c r="O4" s="338"/>
+      <c r="P4" s="338"/>
+      <c r="Q4" s="338" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="336"/>
-      <c r="S4" s="336"/>
-      <c r="T4" s="336"/>
-      <c r="U4" s="336"/>
-      <c r="V4" s="336" t="s">
+      <c r="R4" s="338"/>
+      <c r="S4" s="338"/>
+      <c r="T4" s="338"/>
+      <c r="U4" s="338"/>
+      <c r="V4" s="338" t="s">
         <v>96</v>
       </c>
-      <c r="W4" s="336"/>
-      <c r="X4" s="336"/>
-      <c r="Y4" s="336"/>
-      <c r="Z4" s="336"/>
-      <c r="AA4" s="336" t="s">
+      <c r="W4" s="338"/>
+      <c r="X4" s="338"/>
+      <c r="Y4" s="338"/>
+      <c r="Z4" s="338"/>
+      <c r="AA4" s="338" t="s">
         <v>58</v>
       </c>
-      <c r="AB4" s="336"/>
-      <c r="AC4" s="336"/>
-      <c r="AD4" s="336"/>
-      <c r="AE4" s="336"/>
+      <c r="AB4" s="338"/>
+      <c r="AC4" s="338"/>
+      <c r="AD4" s="338"/>
+      <c r="AE4" s="338"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -17710,7 +18226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S13"/>
   <sheetViews>
@@ -17729,42 +18245,42 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="338" t="s">
+      <c r="A3" s="340" t="s">
         <v>263</v>
       </c>
-      <c r="B3" s="336" t="s">
+      <c r="B3" s="338" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="336"/>
-      <c r="D3" s="336"/>
-      <c r="E3" s="336" t="s">
+      <c r="C3" s="338"/>
+      <c r="D3" s="338"/>
+      <c r="E3" s="338" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="336"/>
-      <c r="G3" s="336"/>
-      <c r="H3" s="336" t="s">
+      <c r="F3" s="338"/>
+      <c r="G3" s="338"/>
+      <c r="H3" s="338" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="336"/>
-      <c r="J3" s="336"/>
-      <c r="K3" s="336" t="s">
+      <c r="I3" s="338"/>
+      <c r="J3" s="338"/>
+      <c r="K3" s="338" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="336"/>
-      <c r="M3" s="336"/>
-      <c r="N3" s="336" t="s">
+      <c r="L3" s="338"/>
+      <c r="M3" s="338"/>
+      <c r="N3" s="338" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="336"/>
-      <c r="P3" s="336"/>
-      <c r="Q3" s="336" t="s">
+      <c r="O3" s="338"/>
+      <c r="P3" s="338"/>
+      <c r="Q3" s="338" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="336"/>
-      <c r="S3" s="336"/>
+      <c r="R3" s="338"/>
+      <c r="S3" s="338"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="338"/>
+      <c r="A4" s="340"/>
       <c r="B4" s="310" t="s">
         <v>40</v>
       </c>
@@ -18349,1015 +18865,6 @@
       </c>
       <c r="S13">
         <v>0.97540000000000004</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:M3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17:S17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="306" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="338" t="s">
-        <v>263</v>
-      </c>
-      <c r="B3" s="336" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="336"/>
-      <c r="D3" s="336"/>
-      <c r="E3" s="336" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="336"/>
-      <c r="G3" s="336"/>
-      <c r="H3" s="336" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="336"/>
-      <c r="J3" s="336"/>
-      <c r="K3" s="336" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="336"/>
-      <c r="M3" s="336"/>
-      <c r="N3" s="336" t="s">
-        <v>96</v>
-      </c>
-      <c r="O3" s="336"/>
-      <c r="P3" s="336"/>
-      <c r="Q3" s="336" t="s">
-        <v>58</v>
-      </c>
-      <c r="R3" s="336"/>
-      <c r="S3" s="336"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="338"/>
-      <c r="B4" s="310" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="310" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="310" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="310" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="310" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="310" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="310" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="310" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="310" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="310" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="310" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" s="310" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" s="310" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" s="310" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" s="310" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" s="310" t="s">
-        <v>40</v>
-      </c>
-      <c r="R4" s="310" t="s">
-        <v>41</v>
-      </c>
-      <c r="S4" s="310" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>30</v>
-      </c>
-      <c r="B5">
-        <v>38.79</v>
-      </c>
-      <c r="C5">
-        <v>180</v>
-      </c>
-      <c r="D5">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="E5">
-        <v>0.31740000000000002</v>
-      </c>
-      <c r="F5">
-        <v>1.724</v>
-      </c>
-      <c r="G5">
-        <v>0.3705</v>
-      </c>
-      <c r="H5">
-        <v>0.1198</v>
-      </c>
-      <c r="I5">
-        <v>0.7137</v>
-      </c>
-      <c r="J5">
-        <v>0.37030000000000002</v>
-      </c>
-      <c r="K5">
-        <v>7.4080000000000004</v>
-      </c>
-      <c r="L5">
-        <v>42.49</v>
-      </c>
-      <c r="M5">
-        <v>0.40610000000000002</v>
-      </c>
-      <c r="N5">
-        <v>0.30599999999999999</v>
-      </c>
-      <c r="O5">
-        <v>1.62</v>
-      </c>
-      <c r="P5">
-        <v>0.37930000000000003</v>
-      </c>
-      <c r="Q5">
-        <v>2.1579999999999998E-2</v>
-      </c>
-      <c r="R5">
-        <v>3.9710000000000002E-2</v>
-      </c>
-      <c r="S5">
-        <v>0.28520000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>50</v>
-      </c>
-      <c r="B6">
-        <v>8.8010000000000002</v>
-      </c>
-      <c r="C6">
-        <v>27.28</v>
-      </c>
-      <c r="D6">
-        <v>0.29570000000000002</v>
-      </c>
-      <c r="E6">
-        <v>9.0300000000000005E-2</v>
-      </c>
-      <c r="F6">
-        <v>0.17119999999999999</v>
-      </c>
-      <c r="G6">
-        <v>0.2324</v>
-      </c>
-      <c r="H6">
-        <v>3.8800000000000001E-2</v>
-      </c>
-      <c r="I6">
-        <v>8.7300000000000003E-2</v>
-      </c>
-      <c r="J6">
-        <v>0.51049999999999995</v>
-      </c>
-      <c r="K6">
-        <v>1.8169999999999999</v>
-      </c>
-      <c r="L6">
-        <v>4.84</v>
-      </c>
-      <c r="M6">
-        <v>0.40210000000000001</v>
-      </c>
-      <c r="N6">
-        <v>9.7210000000000005E-2</v>
-      </c>
-      <c r="O6">
-        <v>0.1799</v>
-      </c>
-      <c r="P6">
-        <v>0.49120000000000003</v>
-      </c>
-      <c r="Q6">
-        <v>1.076E-2</v>
-      </c>
-      <c r="R6">
-        <v>1.8619999999999999E-3</v>
-      </c>
-      <c r="S6">
-        <v>1.17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>70</v>
-      </c>
-      <c r="B7">
-        <v>5.3689999999999998</v>
-      </c>
-      <c r="C7">
-        <v>23.49</v>
-      </c>
-      <c r="D7">
-        <v>0.58830000000000005</v>
-      </c>
-      <c r="E7">
-        <v>5.0900000000000001E-2</v>
-      </c>
-      <c r="F7">
-        <v>0.16969999999999999</v>
-      </c>
-      <c r="G7">
-        <v>0.38490000000000002</v>
-      </c>
-      <c r="H7">
-        <v>2.3E-2</v>
-      </c>
-      <c r="I7">
-        <v>7.1599999999999997E-2</v>
-      </c>
-      <c r="J7">
-        <v>0.73</v>
-      </c>
-      <c r="K7">
-        <v>0.71489999999999998</v>
-      </c>
-      <c r="L7">
-        <v>3.7890000000000001</v>
-      </c>
-      <c r="M7">
-        <v>0.53810000000000002</v>
-      </c>
-      <c r="N7">
-        <v>5.7910000000000003E-2</v>
-      </c>
-      <c r="O7">
-        <v>0.13569999999999999</v>
-      </c>
-      <c r="P7">
-        <v>0.5968</v>
-      </c>
-      <c r="Q7">
-        <v>8.5500000000000003E-3</v>
-      </c>
-      <c r="R7">
-        <v>5.3899999999999998E-4</v>
-      </c>
-      <c r="S7">
-        <v>1.194</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>100</v>
-      </c>
-      <c r="B8">
-        <v>2.5070000000000001</v>
-      </c>
-      <c r="C8">
-        <v>15.33</v>
-      </c>
-      <c r="D8">
-        <v>0.91239999999999999</v>
-      </c>
-      <c r="E8">
-        <v>3.95E-2</v>
-      </c>
-      <c r="F8">
-        <v>8.4400000000000003E-2</v>
-      </c>
-      <c r="G8">
-        <v>0.51910000000000001</v>
-      </c>
-      <c r="H8">
-        <v>1.47E-2</v>
-      </c>
-      <c r="I8">
-        <v>0.04</v>
-      </c>
-      <c r="J8">
-        <v>0.97519999999999996</v>
-      </c>
-      <c r="K8">
-        <v>0.34239999999999998</v>
-      </c>
-      <c r="L8">
-        <v>2.456</v>
-      </c>
-      <c r="M8">
-        <v>0.93879999999999997</v>
-      </c>
-      <c r="N8">
-        <v>4.2790000000000002E-2</v>
-      </c>
-      <c r="O8">
-        <v>8.9480000000000004E-2</v>
-      </c>
-      <c r="P8">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="Q8">
-        <v>7.2300000000000003E-3</v>
-      </c>
-      <c r="R8">
-        <v>8.9400000000000005E-4</v>
-      </c>
-      <c r="S8">
-        <v>1.3160000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>125</v>
-      </c>
-      <c r="B9">
-        <v>2.2330000000000001</v>
-      </c>
-      <c r="C9">
-        <v>7.8879999999999999</v>
-      </c>
-      <c r="D9">
-        <v>0.72950000000000004</v>
-      </c>
-      <c r="E9">
-        <v>3.5099999999999999E-2</v>
-      </c>
-      <c r="F9">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="G9">
-        <v>0.78320000000000001</v>
-      </c>
-      <c r="H9">
-        <v>1.2E-2</v>
-      </c>
-      <c r="I9">
-        <v>2.6700000000000002E-2</v>
-      </c>
-      <c r="J9">
-        <v>10.79</v>
-      </c>
-      <c r="K9">
-        <v>0.21379999999999999</v>
-      </c>
-      <c r="L9">
-        <v>1.69</v>
-      </c>
-      <c r="M9">
-        <v>1.0860000000000001</v>
-      </c>
-      <c r="N9">
-        <v>3.6540000000000003E-2</v>
-      </c>
-      <c r="O9">
-        <v>5.79E-2</v>
-      </c>
-      <c r="P9">
-        <v>1.093</v>
-      </c>
-      <c r="Q9">
-        <v>6.587E-3</v>
-      </c>
-      <c r="R9">
-        <v>-1.14E-3</v>
-      </c>
-      <c r="S9">
-        <v>1.1719999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>150</v>
-      </c>
-      <c r="B10">
-        <v>1.7909999999999999</v>
-      </c>
-      <c r="C10">
-        <v>5.4779999999999998</v>
-      </c>
-      <c r="D10">
-        <v>0.56779999999999997</v>
-      </c>
-      <c r="E10">
-        <v>3.2399999999999998E-2</v>
-      </c>
-      <c r="F10">
-        <v>7.7499999999999999E-2</v>
-      </c>
-      <c r="G10">
-        <v>1.5660000000000001</v>
-      </c>
-      <c r="H10">
-        <v>1.04E-2</v>
-      </c>
-      <c r="I10">
-        <v>2.0199999999999999E-2</v>
-      </c>
-      <c r="J10">
-        <v>1.135</v>
-      </c>
-      <c r="K10">
-        <v>0.15110000000000001</v>
-      </c>
-      <c r="L10">
-        <v>1.1240000000000001</v>
-      </c>
-      <c r="M10">
-        <v>1.151</v>
-      </c>
-      <c r="N10">
-        <v>3.2669999999999998E-2</v>
-      </c>
-      <c r="O10">
-        <v>4.0739999999999998E-2</v>
-      </c>
-      <c r="P10">
-        <v>1.1339999999999999</v>
-      </c>
-      <c r="Q10">
-        <v>6.0270000000000002E-3</v>
-      </c>
-      <c r="R10">
-        <v>-1.6299999999999999E-3</v>
-      </c>
-      <c r="S10">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>286</v>
-      </c>
-      <c r="B11">
-        <v>2.298</v>
-      </c>
-      <c r="C11">
-        <v>17.38</v>
-      </c>
-      <c r="D11">
-        <v>0.61929999999999996</v>
-      </c>
-      <c r="E11">
-        <v>3.61E-2</v>
-      </c>
-      <c r="F11">
-        <v>0.14330000000000001</v>
-      </c>
-      <c r="G11">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="H11">
-        <v>1.38E-2</v>
-      </c>
-      <c r="I11">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="J11">
-        <v>0.79369999999999996</v>
-      </c>
-      <c r="K11">
-        <v>0.21909999999999999</v>
-      </c>
-      <c r="L11">
-        <v>3.49</v>
-      </c>
-      <c r="M11">
-        <v>0.73580000000000001</v>
-      </c>
-      <c r="N11">
-        <v>3.8730000000000001E-2</v>
-      </c>
-      <c r="O11">
-        <v>0.10539999999999999</v>
-      </c>
-      <c r="P11">
-        <v>0.63970000000000005</v>
-      </c>
-      <c r="Q11">
-        <v>7.5519999999999997E-3</v>
-      </c>
-      <c r="R11">
-        <v>7.3700000000000002E-4</v>
-      </c>
-      <c r="S11">
-        <v>1.044</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>287</v>
-      </c>
-      <c r="B12">
-        <v>2.2559999999999998</v>
-      </c>
-      <c r="C12">
-        <v>13.8</v>
-      </c>
-      <c r="D12">
-        <v>0.88370000000000004</v>
-      </c>
-      <c r="E12">
-        <v>3.56E-2</v>
-      </c>
-      <c r="F12">
-        <v>0.1079</v>
-      </c>
-      <c r="G12">
-        <v>0.77049999999999996</v>
-      </c>
-      <c r="H12">
-        <v>1.2699999999999999E-2</v>
-      </c>
-      <c r="I12">
-        <v>4.4499999999999998E-2</v>
-      </c>
-      <c r="J12">
-        <v>1.0489999999999999</v>
-      </c>
-      <c r="K12">
-        <v>0.22109999999999999</v>
-      </c>
-      <c r="L12">
-        <v>2.8359999999999999</v>
-      </c>
-      <c r="M12">
-        <v>1.123</v>
-      </c>
-      <c r="N12">
-        <v>3.7490000000000002E-2</v>
-      </c>
-      <c r="O12">
-        <v>8.7099999999999997E-2</v>
-      </c>
-      <c r="P12">
-        <v>0.90859999999999996</v>
-      </c>
-      <c r="Q12">
-        <v>7.058E-3</v>
-      </c>
-      <c r="R12">
-        <v>2.2900000000000001E-4</v>
-      </c>
-      <c r="S12">
-        <v>1.875</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>288</v>
-      </c>
-      <c r="B13">
-        <v>2.5129999999999999</v>
-      </c>
-      <c r="C13">
-        <v>17.34</v>
-      </c>
-      <c r="D13">
-        <v>0.49940000000000001</v>
-      </c>
-      <c r="E13">
-        <v>3.9199999999999999E-2</v>
-      </c>
-      <c r="F13">
-        <v>0.1464</v>
-      </c>
-      <c r="G13">
-        <v>0.4486</v>
-      </c>
-      <c r="H13">
-        <v>1.6400000000000001E-2</v>
-      </c>
-      <c r="I13">
-        <v>6.08E-2</v>
-      </c>
-      <c r="J13">
-        <v>0.74719999999999998</v>
-      </c>
-      <c r="K13">
-        <v>0.24399999999999999</v>
-      </c>
-      <c r="L13">
-        <v>3.012</v>
-      </c>
-      <c r="M13">
-        <v>0.50190000000000001</v>
-      </c>
-      <c r="N13">
-        <v>4.299E-2</v>
-      </c>
-      <c r="O13">
-        <v>0.107</v>
-      </c>
-      <c r="P13">
-        <v>0.55379999999999996</v>
-      </c>
-      <c r="Q13">
-        <v>7.8869999999999999E-3</v>
-      </c>
-      <c r="R13">
-        <v>8.7699999999999996E-4</v>
-      </c>
-      <c r="S13">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>289</v>
-      </c>
-      <c r="B14">
-        <v>2.3220000000000001</v>
-      </c>
-      <c r="C14">
-        <v>12.91</v>
-      </c>
-      <c r="D14">
-        <v>0.75749999999999995</v>
-      </c>
-      <c r="E14">
-        <v>3.6299999999999999E-2</v>
-      </c>
-      <c r="F14">
-        <v>9.3600000000000003E-2</v>
-      </c>
-      <c r="G14">
-        <v>0.59550000000000003</v>
-      </c>
-      <c r="H14">
-        <v>1.3299999999999999E-2</v>
-      </c>
-      <c r="I14">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="J14">
-        <v>0.95660000000000001</v>
-      </c>
-      <c r="K14">
-        <v>0.2331</v>
-      </c>
-      <c r="L14">
-        <v>2.2130000000000001</v>
-      </c>
-      <c r="M14">
-        <v>0.80510000000000004</v>
-      </c>
-      <c r="N14">
-        <v>3.8859999999999999E-2</v>
-      </c>
-      <c r="O14">
-        <v>8.0909999999999996E-2</v>
-      </c>
-      <c r="P14">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="Q14">
-        <v>7.0569999999999999E-3</v>
-      </c>
-      <c r="R14">
-        <v>4.2200000000000001E-4</v>
-      </c>
-      <c r="S14">
-        <v>1.6639999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>235</v>
-      </c>
-      <c r="B15">
-        <v>2.2719999999999998</v>
-      </c>
-      <c r="C15">
-        <v>13.6</v>
-      </c>
-      <c r="D15">
-        <v>0.71840000000000004</v>
-      </c>
-      <c r="E15">
-        <v>3.56E-2</v>
-      </c>
-      <c r="F15">
-        <v>0.1114</v>
-      </c>
-      <c r="G15">
-        <v>0.66200000000000003</v>
-      </c>
-      <c r="H15">
-        <v>1.29E-2</v>
-      </c>
-      <c r="I15">
-        <v>4.5699999999999998E-2</v>
-      </c>
-      <c r="J15">
-        <v>0.9355</v>
-      </c>
-      <c r="K15">
-        <v>0.21490000000000001</v>
-      </c>
-      <c r="L15">
-        <v>2.6949999999999998</v>
-      </c>
-      <c r="M15">
-        <v>0.87680000000000002</v>
-      </c>
-      <c r="N15">
-        <v>3.7620000000000001E-2</v>
-      </c>
-      <c r="O15">
-        <v>8.8569999999999996E-2</v>
-      </c>
-      <c r="P15">
-        <v>0.80869999999999997</v>
-      </c>
-      <c r="Q15">
-        <v>7.1019999999999998E-3</v>
-      </c>
-      <c r="R15">
-        <v>3.4499999999999998E-4</v>
-      </c>
-      <c r="S15">
-        <v>1.698</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>290</v>
-      </c>
-      <c r="B16">
-        <v>2.2879999999999998</v>
-      </c>
-      <c r="C16">
-        <v>9.8480000000000008</v>
-      </c>
-      <c r="D16">
-        <v>1.054</v>
-      </c>
-      <c r="E16">
-        <v>3.6400000000000002E-2</v>
-      </c>
-      <c r="F16">
-        <v>6.59E-2</v>
-      </c>
-      <c r="G16">
-        <v>0.75429999999999997</v>
-      </c>
-      <c r="H16">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I16">
-        <v>2.9700000000000001E-2</v>
-      </c>
-      <c r="J16">
-        <v>1.1950000000000001</v>
-      </c>
-      <c r="K16">
-        <v>0.25180000000000002</v>
-      </c>
-      <c r="L16">
-        <v>1.829</v>
-      </c>
-      <c r="M16">
-        <v>1.2729999999999999</v>
-      </c>
-      <c r="N16">
-        <v>3.866E-2</v>
-      </c>
-      <c r="O16">
-        <v>6.2700000000000006E-2</v>
-      </c>
-      <c r="P16">
-        <v>1.1279999999999999</v>
-      </c>
-      <c r="Q16">
-        <v>7.4850000000000003E-3</v>
-      </c>
-      <c r="R16">
-        <v>-8.0999999999999996E-4</v>
-      </c>
-      <c r="S16">
-        <v>9.4589999999999994E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>291</v>
-      </c>
-      <c r="B17">
-        <v>29.91</v>
-      </c>
-      <c r="C17">
-        <v>184.4</v>
-      </c>
-      <c r="D17">
-        <v>0.35499999999999998</v>
-      </c>
-      <c r="E17">
-        <v>0.25390000000000001</v>
-      </c>
-      <c r="F17">
-        <v>1.8411</v>
-      </c>
-      <c r="G17">
-        <v>0.39240000000000003</v>
-      </c>
-      <c r="H17">
-        <v>8.8300000000000003E-2</v>
-      </c>
-      <c r="I17">
-        <v>0.75260000000000005</v>
-      </c>
-      <c r="J17">
-        <v>0.37859999999999999</v>
-      </c>
-      <c r="K17">
-        <v>5.7889999999999997</v>
-      </c>
-      <c r="L17">
-        <v>44.12</v>
-      </c>
-      <c r="M17">
-        <v>0.41239999999999999</v>
-      </c>
-      <c r="N17">
-        <v>0.2404</v>
-      </c>
-      <c r="O17">
-        <v>1.7090000000000001</v>
-      </c>
-      <c r="P17">
-        <v>0.39179999999999998</v>
-      </c>
-      <c r="Q17">
-        <v>1.8880000000000001E-2</v>
-      </c>
-      <c r="R17">
-        <v>4.172E-2</v>
-      </c>
-      <c r="S17">
-        <v>0.2903</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>292</v>
-      </c>
-      <c r="B18">
-        <v>2.3540000000000001</v>
-      </c>
-      <c r="C18">
-        <v>14.94</v>
-      </c>
-      <c r="D18">
-        <v>0.74809999999999999</v>
-      </c>
-      <c r="E18">
-        <v>3.7100000000000001E-2</v>
-      </c>
-      <c r="F18">
-        <v>0.1067</v>
-      </c>
-      <c r="G18">
-        <v>0.57330000000000003</v>
-      </c>
-      <c r="H18">
-        <v>1.3899999999999999E-2</v>
-      </c>
-      <c r="I18">
-        <v>4.6399999999999997E-2</v>
-      </c>
-      <c r="J18">
-        <v>0.91849999999999998</v>
-      </c>
-      <c r="K18">
-        <v>0.253</v>
-      </c>
-      <c r="L18">
-        <v>2.5920000000000001</v>
-      </c>
-      <c r="M18">
-        <v>0.79990000000000006</v>
-      </c>
-      <c r="N18">
-        <v>4.0009999999999997E-2</v>
-      </c>
-      <c r="O18">
-        <v>9.0300000000000005E-2</v>
-      </c>
-      <c r="P18">
-        <v>0.80189999999999995</v>
-      </c>
-      <c r="Q18">
-        <v>7.2659999999999999E-3</v>
-      </c>
-      <c r="R18">
-        <v>6.7400000000000001E-4</v>
-      </c>
-      <c r="S18">
-        <v>1.2335</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>293</v>
-      </c>
-      <c r="B19">
-        <v>2.661</v>
-      </c>
-      <c r="C19">
-        <v>19.54</v>
-      </c>
-      <c r="D19">
-        <v>0.50939999999999996</v>
-      </c>
-      <c r="E19">
-        <v>4.2189999999999998E-2</v>
-      </c>
-      <c r="F19">
-        <v>0.15590000000000001</v>
-      </c>
-      <c r="G19">
-        <v>0.44719999999999999</v>
-      </c>
-      <c r="H19">
-        <v>1.7469999999999999E-2</v>
-      </c>
-      <c r="I19">
-        <v>6.4219999999999999E-2</v>
-      </c>
-      <c r="J19">
-        <v>0.72989999999999999</v>
-      </c>
-      <c r="K19">
-        <v>0.3579</v>
-      </c>
-      <c r="L19">
-        <v>3.4660000000000002</v>
-      </c>
-      <c r="M19">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="N19">
-        <v>4.6120000000000001E-2</v>
-      </c>
-      <c r="O19">
-        <v>0.1198</v>
-      </c>
-      <c r="P19">
-        <v>0.5907</v>
-      </c>
-      <c r="Q19">
-        <v>8.0789999999999994E-3</v>
-      </c>
-      <c r="R19">
-        <v>8.4699999999999999E-4</v>
-      </c>
-      <c r="S19">
-        <v>0.97419999999999995</v>
       </c>
     </row>
   </sheetData>
@@ -19376,10 +18883,1019 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="306" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="340" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" s="338" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="338"/>
+      <c r="D3" s="338"/>
+      <c r="E3" s="338" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="338"/>
+      <c r="G3" s="338"/>
+      <c r="H3" s="338" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="338"/>
+      <c r="J3" s="338"/>
+      <c r="K3" s="338" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="338"/>
+      <c r="M3" s="338"/>
+      <c r="N3" s="338" t="s">
+        <v>96</v>
+      </c>
+      <c r="O3" s="338"/>
+      <c r="P3" s="338"/>
+      <c r="Q3" s="338" t="s">
+        <v>58</v>
+      </c>
+      <c r="R3" s="338"/>
+      <c r="S3" s="338"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="340"/>
+      <c r="B4" s="310" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="310" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="310" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="310" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="310" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="310" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="310" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="310" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="310" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="310" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="310" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="310" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="310" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="310" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="310" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="310" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="310" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" s="310" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>38.79</v>
+      </c>
+      <c r="C5">
+        <v>180</v>
+      </c>
+      <c r="D5">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="E5">
+        <v>0.31740000000000002</v>
+      </c>
+      <c r="F5">
+        <v>1.724</v>
+      </c>
+      <c r="G5">
+        <v>0.3705</v>
+      </c>
+      <c r="H5">
+        <v>0.1198</v>
+      </c>
+      <c r="I5">
+        <v>0.7137</v>
+      </c>
+      <c r="J5">
+        <v>0.37030000000000002</v>
+      </c>
+      <c r="K5">
+        <v>7.4080000000000004</v>
+      </c>
+      <c r="L5">
+        <v>42.49</v>
+      </c>
+      <c r="M5">
+        <v>0.40610000000000002</v>
+      </c>
+      <c r="N5">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="O5">
+        <v>1.62</v>
+      </c>
+      <c r="P5">
+        <v>0.37930000000000003</v>
+      </c>
+      <c r="Q5">
+        <v>2.1579999999999998E-2</v>
+      </c>
+      <c r="R5">
+        <v>3.9710000000000002E-2</v>
+      </c>
+      <c r="S5">
+        <v>0.28520000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>8.8010000000000002</v>
+      </c>
+      <c r="C6">
+        <v>27.28</v>
+      </c>
+      <c r="D6">
+        <v>0.29570000000000002</v>
+      </c>
+      <c r="E6">
+        <v>9.0300000000000005E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.17119999999999999</v>
+      </c>
+      <c r="G6">
+        <v>0.2324</v>
+      </c>
+      <c r="H6">
+        <v>3.8800000000000001E-2</v>
+      </c>
+      <c r="I6">
+        <v>8.7300000000000003E-2</v>
+      </c>
+      <c r="J6">
+        <v>0.51049999999999995</v>
+      </c>
+      <c r="K6">
+        <v>1.8169999999999999</v>
+      </c>
+      <c r="L6">
+        <v>4.84</v>
+      </c>
+      <c r="M6">
+        <v>0.40210000000000001</v>
+      </c>
+      <c r="N6">
+        <v>9.7210000000000005E-2</v>
+      </c>
+      <c r="O6">
+        <v>0.1799</v>
+      </c>
+      <c r="P6">
+        <v>0.49120000000000003</v>
+      </c>
+      <c r="Q6">
+        <v>1.076E-2</v>
+      </c>
+      <c r="R6">
+        <v>1.8619999999999999E-3</v>
+      </c>
+      <c r="S6">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>70</v>
+      </c>
+      <c r="B7">
+        <v>5.3689999999999998</v>
+      </c>
+      <c r="C7">
+        <v>23.49</v>
+      </c>
+      <c r="D7">
+        <v>0.58830000000000005</v>
+      </c>
+      <c r="E7">
+        <v>5.0900000000000001E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.16969999999999999</v>
+      </c>
+      <c r="G7">
+        <v>0.38490000000000002</v>
+      </c>
+      <c r="H7">
+        <v>2.3E-2</v>
+      </c>
+      <c r="I7">
+        <v>7.1599999999999997E-2</v>
+      </c>
+      <c r="J7">
+        <v>0.73</v>
+      </c>
+      <c r="K7">
+        <v>0.71489999999999998</v>
+      </c>
+      <c r="L7">
+        <v>3.7890000000000001</v>
+      </c>
+      <c r="M7">
+        <v>0.53810000000000002</v>
+      </c>
+      <c r="N7">
+        <v>5.7910000000000003E-2</v>
+      </c>
+      <c r="O7">
+        <v>0.13569999999999999</v>
+      </c>
+      <c r="P7">
+        <v>0.5968</v>
+      </c>
+      <c r="Q7">
+        <v>8.5500000000000003E-3</v>
+      </c>
+      <c r="R7">
+        <v>5.3899999999999998E-4</v>
+      </c>
+      <c r="S7">
+        <v>1.194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>100</v>
+      </c>
+      <c r="B8">
+        <v>2.5070000000000001</v>
+      </c>
+      <c r="C8">
+        <v>15.33</v>
+      </c>
+      <c r="D8">
+        <v>0.91239999999999999</v>
+      </c>
+      <c r="E8">
+        <v>3.95E-2</v>
+      </c>
+      <c r="F8">
+        <v>8.4400000000000003E-2</v>
+      </c>
+      <c r="G8">
+        <v>0.51910000000000001</v>
+      </c>
+      <c r="H8">
+        <v>1.47E-2</v>
+      </c>
+      <c r="I8">
+        <v>0.04</v>
+      </c>
+      <c r="J8">
+        <v>0.97519999999999996</v>
+      </c>
+      <c r="K8">
+        <v>0.34239999999999998</v>
+      </c>
+      <c r="L8">
+        <v>2.456</v>
+      </c>
+      <c r="M8">
+        <v>0.93879999999999997</v>
+      </c>
+      <c r="N8">
+        <v>4.2790000000000002E-2</v>
+      </c>
+      <c r="O8">
+        <v>8.9480000000000004E-2</v>
+      </c>
+      <c r="P8">
+        <v>1.0289999999999999</v>
+      </c>
+      <c r="Q8">
+        <v>7.2300000000000003E-3</v>
+      </c>
+      <c r="R8">
+        <v>8.9400000000000005E-4</v>
+      </c>
+      <c r="S8">
+        <v>1.3160000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>125</v>
+      </c>
+      <c r="B9">
+        <v>2.2330000000000001</v>
+      </c>
+      <c r="C9">
+        <v>7.8879999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.72950000000000004</v>
+      </c>
+      <c r="E9">
+        <v>3.5099999999999999E-2</v>
+      </c>
+      <c r="F9">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G9">
+        <v>0.78320000000000001</v>
+      </c>
+      <c r="H9">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I9">
+        <v>2.6700000000000002E-2</v>
+      </c>
+      <c r="J9">
+        <v>10.79</v>
+      </c>
+      <c r="K9">
+        <v>0.21379999999999999</v>
+      </c>
+      <c r="L9">
+        <v>1.69</v>
+      </c>
+      <c r="M9">
+        <v>1.0860000000000001</v>
+      </c>
+      <c r="N9">
+        <v>3.6540000000000003E-2</v>
+      </c>
+      <c r="O9">
+        <v>5.79E-2</v>
+      </c>
+      <c r="P9">
+        <v>1.093</v>
+      </c>
+      <c r="Q9">
+        <v>6.587E-3</v>
+      </c>
+      <c r="R9">
+        <v>-1.14E-3</v>
+      </c>
+      <c r="S9">
+        <v>1.1719999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>150</v>
+      </c>
+      <c r="B10">
+        <v>1.7909999999999999</v>
+      </c>
+      <c r="C10">
+        <v>5.4779999999999998</v>
+      </c>
+      <c r="D10">
+        <v>0.56779999999999997</v>
+      </c>
+      <c r="E10">
+        <v>3.2399999999999998E-2</v>
+      </c>
+      <c r="F10">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="G10">
+        <v>1.5660000000000001</v>
+      </c>
+      <c r="H10">
+        <v>1.04E-2</v>
+      </c>
+      <c r="I10">
+        <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="J10">
+        <v>1.135</v>
+      </c>
+      <c r="K10">
+        <v>0.15110000000000001</v>
+      </c>
+      <c r="L10">
+        <v>1.1240000000000001</v>
+      </c>
+      <c r="M10">
+        <v>1.151</v>
+      </c>
+      <c r="N10">
+        <v>3.2669999999999998E-2</v>
+      </c>
+      <c r="O10">
+        <v>4.0739999999999998E-2</v>
+      </c>
+      <c r="P10">
+        <v>1.1339999999999999</v>
+      </c>
+      <c r="Q10">
+        <v>6.0270000000000002E-3</v>
+      </c>
+      <c r="R10">
+        <v>-1.6299999999999999E-3</v>
+      </c>
+      <c r="S10">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>286</v>
+      </c>
+      <c r="B11">
+        <v>2.298</v>
+      </c>
+      <c r="C11">
+        <v>17.38</v>
+      </c>
+      <c r="D11">
+        <v>0.61929999999999996</v>
+      </c>
+      <c r="E11">
+        <v>3.61E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.14330000000000001</v>
+      </c>
+      <c r="G11">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H11">
+        <v>1.38E-2</v>
+      </c>
+      <c r="I11">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="J11">
+        <v>0.79369999999999996</v>
+      </c>
+      <c r="K11">
+        <v>0.21909999999999999</v>
+      </c>
+      <c r="L11">
+        <v>3.49</v>
+      </c>
+      <c r="M11">
+        <v>0.73580000000000001</v>
+      </c>
+      <c r="N11">
+        <v>3.8730000000000001E-2</v>
+      </c>
+      <c r="O11">
+        <v>0.10539999999999999</v>
+      </c>
+      <c r="P11">
+        <v>0.63970000000000005</v>
+      </c>
+      <c r="Q11">
+        <v>7.5519999999999997E-3</v>
+      </c>
+      <c r="R11">
+        <v>7.3700000000000002E-4</v>
+      </c>
+      <c r="S11">
+        <v>1.044</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>287</v>
+      </c>
+      <c r="B12">
+        <v>2.2559999999999998</v>
+      </c>
+      <c r="C12">
+        <v>13.8</v>
+      </c>
+      <c r="D12">
+        <v>0.88370000000000004</v>
+      </c>
+      <c r="E12">
+        <v>3.56E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.1079</v>
+      </c>
+      <c r="G12">
+        <v>0.77049999999999996</v>
+      </c>
+      <c r="H12">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="I12">
+        <v>4.4499999999999998E-2</v>
+      </c>
+      <c r="J12">
+        <v>1.0489999999999999</v>
+      </c>
+      <c r="K12">
+        <v>0.22109999999999999</v>
+      </c>
+      <c r="L12">
+        <v>2.8359999999999999</v>
+      </c>
+      <c r="M12">
+        <v>1.123</v>
+      </c>
+      <c r="N12">
+        <v>3.7490000000000002E-2</v>
+      </c>
+      <c r="O12">
+        <v>8.7099999999999997E-2</v>
+      </c>
+      <c r="P12">
+        <v>0.90859999999999996</v>
+      </c>
+      <c r="Q12">
+        <v>7.058E-3</v>
+      </c>
+      <c r="R12">
+        <v>2.2900000000000001E-4</v>
+      </c>
+      <c r="S12">
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>288</v>
+      </c>
+      <c r="B13">
+        <v>2.5129999999999999</v>
+      </c>
+      <c r="C13">
+        <v>17.34</v>
+      </c>
+      <c r="D13">
+        <v>0.49940000000000001</v>
+      </c>
+      <c r="E13">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="F13">
+        <v>0.1464</v>
+      </c>
+      <c r="G13">
+        <v>0.4486</v>
+      </c>
+      <c r="H13">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="I13">
+        <v>6.08E-2</v>
+      </c>
+      <c r="J13">
+        <v>0.74719999999999998</v>
+      </c>
+      <c r="K13">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="L13">
+        <v>3.012</v>
+      </c>
+      <c r="M13">
+        <v>0.50190000000000001</v>
+      </c>
+      <c r="N13">
+        <v>4.299E-2</v>
+      </c>
+      <c r="O13">
+        <v>0.107</v>
+      </c>
+      <c r="P13">
+        <v>0.55379999999999996</v>
+      </c>
+      <c r="Q13">
+        <v>7.8869999999999999E-3</v>
+      </c>
+      <c r="R13">
+        <v>8.7699999999999996E-4</v>
+      </c>
+      <c r="S13">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>289</v>
+      </c>
+      <c r="B14">
+        <v>2.3220000000000001</v>
+      </c>
+      <c r="C14">
+        <v>12.91</v>
+      </c>
+      <c r="D14">
+        <v>0.75749999999999995</v>
+      </c>
+      <c r="E14">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="F14">
+        <v>9.3600000000000003E-2</v>
+      </c>
+      <c r="G14">
+        <v>0.59550000000000003</v>
+      </c>
+      <c r="H14">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="I14">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="J14">
+        <v>0.95660000000000001</v>
+      </c>
+      <c r="K14">
+        <v>0.2331</v>
+      </c>
+      <c r="L14">
+        <v>2.2130000000000001</v>
+      </c>
+      <c r="M14">
+        <v>0.80510000000000004</v>
+      </c>
+      <c r="N14">
+        <v>3.8859999999999999E-2</v>
+      </c>
+      <c r="O14">
+        <v>8.0909999999999996E-2</v>
+      </c>
+      <c r="P14">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="Q14">
+        <v>7.0569999999999999E-3</v>
+      </c>
+      <c r="R14">
+        <v>4.2200000000000001E-4</v>
+      </c>
+      <c r="S14">
+        <v>1.6639999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B15">
+        <v>2.2719999999999998</v>
+      </c>
+      <c r="C15">
+        <v>13.6</v>
+      </c>
+      <c r="D15">
+        <v>0.71840000000000004</v>
+      </c>
+      <c r="E15">
+        <v>3.56E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.1114</v>
+      </c>
+      <c r="G15">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="H15">
+        <v>1.29E-2</v>
+      </c>
+      <c r="I15">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="J15">
+        <v>0.9355</v>
+      </c>
+      <c r="K15">
+        <v>0.21490000000000001</v>
+      </c>
+      <c r="L15">
+        <v>2.6949999999999998</v>
+      </c>
+      <c r="M15">
+        <v>0.87680000000000002</v>
+      </c>
+      <c r="N15">
+        <v>3.7620000000000001E-2</v>
+      </c>
+      <c r="O15">
+        <v>8.8569999999999996E-2</v>
+      </c>
+      <c r="P15">
+        <v>0.80869999999999997</v>
+      </c>
+      <c r="Q15">
+        <v>7.1019999999999998E-3</v>
+      </c>
+      <c r="R15">
+        <v>3.4499999999999998E-4</v>
+      </c>
+      <c r="S15">
+        <v>1.698</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>290</v>
+      </c>
+      <c r="B16">
+        <v>2.2879999999999998</v>
+      </c>
+      <c r="C16">
+        <v>9.8480000000000008</v>
+      </c>
+      <c r="D16">
+        <v>1.054</v>
+      </c>
+      <c r="E16">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="F16">
+        <v>6.59E-2</v>
+      </c>
+      <c r="G16">
+        <v>0.75429999999999997</v>
+      </c>
+      <c r="H16">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I16">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="J16">
+        <v>1.1950000000000001</v>
+      </c>
+      <c r="K16">
+        <v>0.25180000000000002</v>
+      </c>
+      <c r="L16">
+        <v>1.829</v>
+      </c>
+      <c r="M16">
+        <v>1.2729999999999999</v>
+      </c>
+      <c r="N16">
+        <v>3.866E-2</v>
+      </c>
+      <c r="O16">
+        <v>6.2700000000000006E-2</v>
+      </c>
+      <c r="P16">
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="Q16">
+        <v>7.4850000000000003E-3</v>
+      </c>
+      <c r="R16">
+        <v>-8.0999999999999996E-4</v>
+      </c>
+      <c r="S16">
+        <v>9.4589999999999994E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17">
+        <v>29.91</v>
+      </c>
+      <c r="C17">
+        <v>184.4</v>
+      </c>
+      <c r="D17">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="E17">
+        <v>0.25390000000000001</v>
+      </c>
+      <c r="F17">
+        <v>1.8411</v>
+      </c>
+      <c r="G17">
+        <v>0.39240000000000003</v>
+      </c>
+      <c r="H17">
+        <v>8.8300000000000003E-2</v>
+      </c>
+      <c r="I17">
+        <v>0.75260000000000005</v>
+      </c>
+      <c r="J17">
+        <v>0.37859999999999999</v>
+      </c>
+      <c r="K17">
+        <v>5.7889999999999997</v>
+      </c>
+      <c r="L17">
+        <v>44.12</v>
+      </c>
+      <c r="M17">
+        <v>0.41239999999999999</v>
+      </c>
+      <c r="N17">
+        <v>0.2404</v>
+      </c>
+      <c r="O17">
+        <v>1.7090000000000001</v>
+      </c>
+      <c r="P17">
+        <v>0.39179999999999998</v>
+      </c>
+      <c r="Q17">
+        <v>1.8880000000000001E-2</v>
+      </c>
+      <c r="R17">
+        <v>4.172E-2</v>
+      </c>
+      <c r="S17">
+        <v>0.2903</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>292</v>
+      </c>
+      <c r="B18">
+        <v>2.3540000000000001</v>
+      </c>
+      <c r="C18">
+        <v>14.94</v>
+      </c>
+      <c r="D18">
+        <v>0.74809999999999999</v>
+      </c>
+      <c r="E18">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="F18">
+        <v>0.1067</v>
+      </c>
+      <c r="G18">
+        <v>0.57330000000000003</v>
+      </c>
+      <c r="H18">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="I18">
+        <v>4.6399999999999997E-2</v>
+      </c>
+      <c r="J18">
+        <v>0.91849999999999998</v>
+      </c>
+      <c r="K18">
+        <v>0.253</v>
+      </c>
+      <c r="L18">
+        <v>2.5920000000000001</v>
+      </c>
+      <c r="M18">
+        <v>0.79990000000000006</v>
+      </c>
+      <c r="N18">
+        <v>4.0009999999999997E-2</v>
+      </c>
+      <c r="O18">
+        <v>9.0300000000000005E-2</v>
+      </c>
+      <c r="P18">
+        <v>0.80189999999999995</v>
+      </c>
+      <c r="Q18">
+        <v>7.2659999999999999E-3</v>
+      </c>
+      <c r="R18">
+        <v>6.7400000000000001E-4</v>
+      </c>
+      <c r="S18">
+        <v>1.2335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B19">
+        <v>2.661</v>
+      </c>
+      <c r="C19">
+        <v>19.54</v>
+      </c>
+      <c r="D19">
+        <v>0.50939999999999996</v>
+      </c>
+      <c r="E19">
+        <v>4.2189999999999998E-2</v>
+      </c>
+      <c r="F19">
+        <v>0.15590000000000001</v>
+      </c>
+      <c r="G19">
+        <v>0.44719999999999999</v>
+      </c>
+      <c r="H19">
+        <v>1.7469999999999999E-2</v>
+      </c>
+      <c r="I19">
+        <v>6.4219999999999999E-2</v>
+      </c>
+      <c r="J19">
+        <v>0.72989999999999999</v>
+      </c>
+      <c r="K19">
+        <v>0.3579</v>
+      </c>
+      <c r="L19">
+        <v>3.4660000000000002</v>
+      </c>
+      <c r="M19">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="N19">
+        <v>4.6120000000000001E-2</v>
+      </c>
+      <c r="O19">
+        <v>0.1198</v>
+      </c>
+      <c r="P19">
+        <v>0.5907</v>
+      </c>
+      <c r="Q19">
+        <v>8.0789999999999994E-3</v>
+      </c>
+      <c r="R19">
+        <v>8.4699999999999999E-4</v>
+      </c>
+      <c r="S19">
+        <v>0.97419999999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19393,36 +19909,36 @@
       <c r="A2" s="319" t="s">
         <v>303</v>
       </c>
-      <c r="B2" s="336" t="s">
+      <c r="B2" s="338" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="336"/>
-      <c r="D2" s="336"/>
-      <c r="E2" s="336" t="s">
+      <c r="C2" s="338"/>
+      <c r="D2" s="338"/>
+      <c r="E2" s="338" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="336"/>
-      <c r="G2" s="336"/>
-      <c r="H2" s="336" t="s">
+      <c r="F2" s="338"/>
+      <c r="G2" s="338"/>
+      <c r="H2" s="338" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="336"/>
-      <c r="J2" s="336"/>
-      <c r="K2" s="336" t="s">
+      <c r="I2" s="338"/>
+      <c r="J2" s="338"/>
+      <c r="K2" s="338" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="336"/>
-      <c r="M2" s="336"/>
-      <c r="N2" s="336" t="s">
+      <c r="L2" s="338"/>
+      <c r="M2" s="338"/>
+      <c r="N2" s="338" t="s">
         <v>96</v>
       </c>
-      <c r="O2" s="336"/>
-      <c r="P2" s="336"/>
-      <c r="Q2" s="336" t="s">
+      <c r="O2" s="338"/>
+      <c r="P2" s="338"/>
+      <c r="Q2" s="338" t="s">
         <v>58</v>
       </c>
-      <c r="R2" s="336"/>
-      <c r="S2" s="336"/>
+      <c r="R2" s="338"/>
+      <c r="S2" s="338"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -19736,36 +20252,36 @@
       <c r="A12" s="319" t="s">
         <v>302</v>
       </c>
-      <c r="B12" s="336" t="s">
+      <c r="B12" s="338" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="336"/>
-      <c r="D12" s="336"/>
-      <c r="E12" s="336" t="s">
+      <c r="C12" s="338"/>
+      <c r="D12" s="338"/>
+      <c r="E12" s="338" t="s">
         <v>95</v>
       </c>
-      <c r="F12" s="336"/>
-      <c r="G12" s="336"/>
-      <c r="H12" s="336" t="s">
+      <c r="F12" s="338"/>
+      <c r="G12" s="338"/>
+      <c r="H12" s="338" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="336"/>
-      <c r="J12" s="336"/>
-      <c r="K12" s="336" t="s">
+      <c r="I12" s="338"/>
+      <c r="J12" s="338"/>
+      <c r="K12" s="338" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="336"/>
-      <c r="M12" s="336"/>
-      <c r="N12" s="336" t="s">
+      <c r="L12" s="338"/>
+      <c r="M12" s="338"/>
+      <c r="N12" s="338" t="s">
         <v>96</v>
       </c>
-      <c r="O12" s="336"/>
-      <c r="P12" s="336"/>
-      <c r="Q12" s="336" t="s">
+      <c r="O12" s="338"/>
+      <c r="P12" s="338"/>
+      <c r="Q12" s="338" t="s">
         <v>58</v>
       </c>
-      <c r="R12" s="336"/>
-      <c r="S12" s="336"/>
+      <c r="R12" s="338"/>
+      <c r="S12" s="338"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -20197,36 +20713,36 @@
       <c r="A24" s="319" t="s">
         <v>301</v>
       </c>
-      <c r="B24" s="336" t="s">
+      <c r="B24" s="338" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="336"/>
-      <c r="D24" s="336"/>
-      <c r="E24" s="336" t="s">
+      <c r="C24" s="338"/>
+      <c r="D24" s="338"/>
+      <c r="E24" s="338" t="s">
         <v>95</v>
       </c>
-      <c r="F24" s="336"/>
-      <c r="G24" s="336"/>
-      <c r="H24" s="336" t="s">
+      <c r="F24" s="338"/>
+      <c r="G24" s="338"/>
+      <c r="H24" s="338" t="s">
         <v>52</v>
       </c>
-      <c r="I24" s="336"/>
-      <c r="J24" s="336"/>
-      <c r="K24" s="336" t="s">
+      <c r="I24" s="338"/>
+      <c r="J24" s="338"/>
+      <c r="K24" s="338" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="336"/>
-      <c r="M24" s="336"/>
-      <c r="N24" s="336" t="s">
+      <c r="L24" s="338"/>
+      <c r="M24" s="338"/>
+      <c r="N24" s="338" t="s">
         <v>96</v>
       </c>
-      <c r="O24" s="336"/>
-      <c r="P24" s="336"/>
-      <c r="Q24" s="336" t="s">
+      <c r="O24" s="338"/>
+      <c r="P24" s="338"/>
+      <c r="Q24" s="338" t="s">
         <v>58</v>
       </c>
-      <c r="R24" s="336"/>
-      <c r="S24" s="336"/>
+      <c r="R24" s="338"/>
+      <c r="S24" s="338"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -20537,36 +21053,36 @@
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C34" s="336" t="s">
+      <c r="C34" s="338" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="336"/>
-      <c r="E34" s="336"/>
-      <c r="F34" s="336" t="s">
+      <c r="D34" s="338"/>
+      <c r="E34" s="338"/>
+      <c r="F34" s="338" t="s">
         <v>95</v>
       </c>
-      <c r="G34" s="336"/>
-      <c r="H34" s="336"/>
-      <c r="I34" s="336" t="s">
+      <c r="G34" s="338"/>
+      <c r="H34" s="338"/>
+      <c r="I34" s="338" t="s">
         <v>52</v>
       </c>
-      <c r="J34" s="336"/>
-      <c r="K34" s="336"/>
-      <c r="L34" s="336" t="s">
+      <c r="J34" s="338"/>
+      <c r="K34" s="338"/>
+      <c r="L34" s="338" t="s">
         <v>54</v>
       </c>
-      <c r="M34" s="336"/>
-      <c r="N34" s="336"/>
-      <c r="O34" s="336" t="s">
+      <c r="M34" s="338"/>
+      <c r="N34" s="338"/>
+      <c r="O34" s="338" t="s">
         <v>96</v>
       </c>
-      <c r="P34" s="336"/>
-      <c r="Q34" s="336"/>
-      <c r="R34" s="336" t="s">
+      <c r="P34" s="338"/>
+      <c r="Q34" s="338"/>
+      <c r="R34" s="338" t="s">
         <v>58</v>
       </c>
-      <c r="S34" s="336"/>
-      <c r="T34" s="336"/>
+      <c r="S34" s="338"/>
+      <c r="T34" s="338"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C35" s="310" t="s">
@@ -20752,18 +21268,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
     <mergeCell ref="Q24:S24"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="E12:G12"/>
@@ -20776,7 +21280,410 @@
     <mergeCell ref="H24:J24"/>
     <mergeCell ref="K24:M24"/>
     <mergeCell ref="N24:P24"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="O34:Q34"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="343" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="305" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="305" t="s">
+        <v>324</v>
+      </c>
+      <c r="B2" s="305" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="305" t="s">
+        <v>325</v>
+      </c>
+      <c r="D2" s="305" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2" s="305" t="s">
+        <v>327</v>
+      </c>
+      <c r="F2" s="305" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="C3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D3">
+        <v>0.96</v>
+      </c>
+      <c r="E3">
+        <v>511</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B4">
+        <f>12.7*60</f>
+        <v>762</v>
+      </c>
+      <c r="C4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D4">
+        <v>0.65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>335</v>
+      </c>
+      <c r="F4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B5">
+        <v>109.8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>346</v>
+      </c>
+      <c r="D5">
+        <v>0.63</v>
+      </c>
+      <c r="E5">
+        <v>511</v>
+      </c>
+      <c r="F5">
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>336</v>
+      </c>
+      <c r="B6">
+        <v>68.3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>346</v>
+      </c>
+      <c r="D6">
+        <v>1.9</v>
+      </c>
+      <c r="E6">
+        <v>511</v>
+      </c>
+      <c r="F6">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>341</v>
+      </c>
+      <c r="B7">
+        <f>4.2*3600*24</f>
+        <v>362880</v>
+      </c>
+      <c r="C7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D7" t="s">
+        <v>342</v>
+      </c>
+      <c r="E7" t="s">
+        <v>343</v>
+      </c>
+      <c r="F7" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>331</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>345</v>
+      </c>
+      <c r="D8">
+        <v>1.19</v>
+      </c>
+      <c r="E8">
+        <v>511</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>332</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>345</v>
+      </c>
+      <c r="D9">
+        <v>1.72</v>
+      </c>
+      <c r="E9">
+        <v>511</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>337</v>
+      </c>
+      <c r="B10">
+        <f>76/60</f>
+        <v>1.2666666666666666</v>
+      </c>
+      <c r="C10" t="s">
+        <v>346</v>
+      </c>
+      <c r="D10">
+        <v>3.35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>338</v>
+      </c>
+      <c r="F10" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="343" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="344"/>
+      <c r="B13" s="305" t="s">
+        <v>349</v>
+      </c>
+      <c r="C13" s="305" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="305" t="s">
+        <v>324</v>
+      </c>
+      <c r="B14" s="305" t="s">
+        <v>351</v>
+      </c>
+      <c r="C14" s="305" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>329</v>
+      </c>
+      <c r="B15">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="C15">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>334</v>
+      </c>
+      <c r="B16">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C16">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>333</v>
+      </c>
+      <c r="B17">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="C17">
+        <v>0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>336</v>
+      </c>
+      <c r="B18">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C18">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>341</v>
+      </c>
+      <c r="B19">
+        <v>0.185</v>
+      </c>
+      <c r="C19">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>331</v>
+      </c>
+      <c r="B20">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="C20">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>332</v>
+      </c>
+      <c r="B21">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="C21">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>337</v>
+      </c>
+      <c r="B22">
+        <v>0.159</v>
+      </c>
+      <c r="C22">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="342" t="s">
+        <v>321</v>
+      </c>
+      <c r="B24" s="324"/>
+      <c r="C24" s="324"/>
+      <c r="D24" s="324"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>319</v>
+      </c>
+      <c r="B25" s="310" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="310" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="310" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26">
+        <v>1.5429999999999999</v>
+      </c>
+      <c r="C26">
+        <v>-0.44080000000000003</v>
+      </c>
+      <c r="D26">
+        <v>2.1360000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27">
+        <v>0.15390000000000001</v>
+      </c>
+      <c r="C27">
+        <v>-0.11609999999999999</v>
+      </c>
+      <c r="D27">
+        <v>2.0752000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>320</v>
+      </c>
+      <c r="B28">
+        <v>0.57040000000000002</v>
+      </c>
+      <c r="C28">
+        <v>-0.30630000000000002</v>
+      </c>
+      <c r="D28">
+        <v>0.63260000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="319" t="s">
+        <v>295</v>
+      </c>
+      <c r="B30" s="306" t="s">
+        <v>322</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A3:F10">
+    <sortCondition ref="A3:A10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -20797,22 +21704,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1" s="323" t="s">
+      <c r="B1" s="325" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="323"/>
-      <c r="D1" s="323" t="s">
+      <c r="C1" s="325"/>
+      <c r="D1" s="325" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="323"/>
-      <c r="F1" s="323"/>
-      <c r="H1" s="324" t="s">
+      <c r="E1" s="325"/>
+      <c r="F1" s="325"/>
+      <c r="H1" s="326" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="323"/>
-      <c r="J1" s="323"/>
-      <c r="K1" s="323"/>
-      <c r="L1" s="323"/>
+      <c r="I1" s="325"/>
+      <c r="J1" s="325"/>
+      <c r="K1" s="325"/>
+      <c r="L1" s="325"/>
       <c r="M1" s="293"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -20907,13 +21814,13 @@
       <c r="D5" s="315"/>
       <c r="E5" s="315"/>
       <c r="F5" s="315"/>
-      <c r="H5" s="325" t="s">
+      <c r="H5" s="327" t="s">
         <v>184</v>
       </c>
-      <c r="I5" s="326"/>
-      <c r="J5" s="326"/>
-      <c r="K5" s="326"/>
-      <c r="L5" s="326"/>
+      <c r="I5" s="328"/>
+      <c r="J5" s="328"/>
+      <c r="K5" s="328"/>
+      <c r="L5" s="328"/>
       <c r="M5" s="293"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -21933,8 +22840,8 @@
   </sheetPr>
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30:K44"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22222,14 +23129,14 @@
       <c r="M18" s="264"/>
       <c r="N18" s="263"/>
       <c r="P18" s="278"/>
-      <c r="Q18" s="327" t="s">
+      <c r="Q18" s="329" t="s">
         <v>173</v>
       </c>
-      <c r="R18" s="327"/>
-      <c r="S18" s="327"/>
-      <c r="T18" s="327"/>
-      <c r="U18" s="327"/>
-      <c r="V18" s="328"/>
+      <c r="R18" s="329"/>
+      <c r="S18" s="329"/>
+      <c r="T18" s="329"/>
+      <c r="U18" s="329"/>
+      <c r="V18" s="330"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="215"/>
@@ -22260,16 +23167,16 @@
       </c>
       <c r="N19" s="275"/>
       <c r="P19" s="215"/>
-      <c r="Q19" s="329" t="s">
+      <c r="Q19" s="331" t="s">
         <v>172</v>
       </c>
-      <c r="R19" s="329"/>
-      <c r="S19" s="329"/>
-      <c r="T19" s="330" t="s">
+      <c r="R19" s="331"/>
+      <c r="S19" s="331"/>
+      <c r="T19" s="332" t="s">
         <v>95</v>
       </c>
-      <c r="U19" s="330"/>
-      <c r="V19" s="331"/>
+      <c r="U19" s="332"/>
+      <c r="V19" s="333"/>
     </row>
     <row r="20" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="215"/>
@@ -22466,14 +23373,14 @@
       <c r="N24" s="216"/>
       <c r="O24" s="216"/>
       <c r="P24" s="253"/>
-      <c r="Q24" s="327" t="s">
+      <c r="Q24" s="329" t="s">
         <v>173</v>
       </c>
-      <c r="R24" s="327"/>
-      <c r="S24" s="327"/>
-      <c r="T24" s="327"/>
-      <c r="U24" s="327"/>
-      <c r="V24" s="328"/>
+      <c r="R24" s="329"/>
+      <c r="S24" s="329"/>
+      <c r="T24" s="329"/>
+      <c r="U24" s="329"/>
+      <c r="V24" s="330"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="223" t="s">
@@ -22559,7 +23466,7 @@
       <c r="H27" s="248" t="s">
         <v>48</v>
       </c>
-      <c r="J27" s="332" t="s">
+      <c r="J27" s="334" t="s">
         <v>162</v>
       </c>
       <c r="K27" s="210" t="s">
@@ -22622,7 +23529,7 @@
       <c r="H28" s="245" t="s">
         <v>122</v>
       </c>
-      <c r="J28" s="332"/>
+      <c r="J28" s="334"/>
       <c r="K28" s="210" t="s">
         <v>183</v>
       </c>
@@ -23551,6 +24458,237 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="12.83203125" style="323"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="345" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="346" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="355"/>
+      <c r="F2" s="347"/>
+      <c r="G2" s="347"/>
+      <c r="H2" s="348"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="349" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="356" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="350" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="357"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="341" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="354" t="s">
+        <v>355</v>
+      </c>
+      <c r="B7" s="358" t="s">
+        <v>333</v>
+      </c>
+      <c r="C7" s="358" t="s">
+        <v>337</v>
+      </c>
+      <c r="D7" s="358"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="352" t="s">
+        <v>365</v>
+      </c>
+      <c r="B8" s="358">
+        <f>16*5</f>
+        <v>80</v>
+      </c>
+      <c r="C8" s="358">
+        <v>5</v>
+      </c>
+      <c r="D8" s="358"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="343" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="351" t="s">
+        <v>355</v>
+      </c>
+      <c r="B11" s="351" t="s">
+        <v>357</v>
+      </c>
+      <c r="C11" s="351" t="s">
+        <v>358</v>
+      </c>
+      <c r="D11" s="351" t="s">
+        <v>362</v>
+      </c>
+      <c r="E11" s="352" t="s">
+        <v>363</v>
+      </c>
+      <c r="F11" s="351" t="s">
+        <v>361</v>
+      </c>
+      <c r="G11" s="351" t="s">
+        <v>359</v>
+      </c>
+      <c r="H11" s="351" t="s">
+        <v>360</v>
+      </c>
+      <c r="I11" s="351" t="s">
+        <v>366</v>
+      </c>
+      <c r="J11" s="351" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="359" t="str">
+        <f>IF(B7="","",B7)</f>
+        <v>F-18</v>
+      </c>
+      <c r="B12" s="359">
+        <v>370</v>
+      </c>
+      <c r="C12" s="359">
+        <v>55</v>
+      </c>
+      <c r="D12" s="359">
+        <v>15</v>
+      </c>
+      <c r="E12" s="353">
+        <f>IF(A12="","",VLOOKUP(A12,AAPMTG108!$A$3:$B$10,2,FALSE))</f>
+        <v>109.8</v>
+      </c>
+      <c r="F12" s="353">
+        <f>IF(B12="","",(B12*0.64)*1.443*E12*(1-EXP(-LN(2)*C12/E12))/C12)</f>
+        <v>200.10510580027605</v>
+      </c>
+      <c r="G12" s="353">
+        <f>IF(B12="","",(B12*0.64)*EXP(-LN(2)*C12/E12))</f>
+        <v>167.33721553195579</v>
+      </c>
+      <c r="H12" s="353">
+        <f>IF(G12="","",G12*0.85)</f>
+        <v>142.23663320216241</v>
+      </c>
+      <c r="I12" s="353">
+        <f>IF(H12="","",H12*1.443*E12*(1-EXP(-LN(2)*D12/E12))/D12)</f>
+        <v>135.73859264685737</v>
+      </c>
+      <c r="J12" s="353">
+        <f>IF(H12="","",H12*EXP(-LN(2)*D12/E12))</f>
+        <v>129.3859585066418</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="359" t="str">
+        <f>IF(C7="","",C7)</f>
+        <v>Rb-82</v>
+      </c>
+      <c r="B13" s="359">
+        <v>1110</v>
+      </c>
+      <c r="C13" s="359">
+        <v>10</v>
+      </c>
+      <c r="D13" s="359">
+        <v>5</v>
+      </c>
+      <c r="E13" s="353">
+        <f>IF(A13="","",VLOOKUP(A13,AAPMTG108!$A$3:$B$10,2,FALSE))</f>
+        <v>1.2666666666666666</v>
+      </c>
+      <c r="F13" s="353">
+        <f t="shared" ref="F13:F14" si="0">IF(B13="","",(B13*0.64)*1.443*E13*(1-EXP(-LN(2)*C13/E13))/C13)</f>
+        <v>129.30130613715559</v>
+      </c>
+      <c r="G13" s="353">
+        <f t="shared" ref="G13:G14" si="1">IF(B13="","",(B13*0.64)*EXP(-LN(2)*C13/E13))</f>
+        <v>2.9850413767610053</v>
+      </c>
+      <c r="H13" s="353">
+        <f t="shared" ref="H13:H14" si="2">IF(G13="","",G13*0.85)</f>
+        <v>2.5372851702468546</v>
+      </c>
+      <c r="I13" s="353">
+        <f t="shared" ref="I13:I14" si="3">IF(H13="","",H13*1.443*E13*(1-EXP(-LN(2)*D13/E13))/D13)</f>
+        <v>0.86740544283679122</v>
+      </c>
+      <c r="J13" s="353">
+        <f t="shared" ref="J13:J14" si="4">IF(H13="","",H13*EXP(-LN(2)*D13/E13))</f>
+        <v>0.16447238209500251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="359" t="str">
+        <f>IF(D7="","",D7)</f>
+        <v/>
+      </c>
+      <c r="B14" s="359"/>
+      <c r="C14" s="359"/>
+      <c r="D14" s="359"/>
+      <c r="E14" s="353" t="str">
+        <f>IF(A14="","",VLOOKUP(A14,AAPMTG108!$A$3:$B$10,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="F14" s="353" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G14" s="353" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H14" s="353" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I14" s="353" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J14" s="353" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="343" t="s">
+        <v>367</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V47"/>
   <sheetViews>
@@ -23946,7 +25084,7 @@
       <c r="E18" s="167" t="s">
         <v>120</v>
       </c>
-      <c r="F18" s="333" t="s">
+      <c r="F18" s="335" t="s">
         <v>121</v>
       </c>
       <c r="G18" s="167"/>
@@ -23996,7 +25134,7 @@
       <c r="E19" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="F19" s="333"/>
+      <c r="F19" s="335"/>
       <c r="G19" s="167" t="s">
         <v>48</v>
       </c>
@@ -24029,22 +25167,22 @@
       <c r="E20" s="168" t="s">
         <v>181</v>
       </c>
-      <c r="F20" s="334"/>
+      <c r="F20" s="336"/>
       <c r="G20" s="168" t="s">
         <v>122</v>
       </c>
       <c r="H20" s="168" t="s">
         <v>118</v>
       </c>
-      <c r="L20" s="335" t="s">
+      <c r="L20" s="337" t="s">
         <v>123</v>
       </c>
-      <c r="M20" s="335"/>
-      <c r="N20" s="335"/>
-      <c r="O20" s="335"/>
-      <c r="P20" s="335"/>
-      <c r="Q20" s="335"/>
-      <c r="R20" s="335"/>
+      <c r="M20" s="337"/>
+      <c r="N20" s="337"/>
+      <c r="O20" s="337"/>
+      <c r="P20" s="337"/>
+      <c r="Q20" s="337"/>
+      <c r="R20" s="337"/>
       <c r="T20" s="158">
         <v>1.1906250009999999</v>
       </c>
@@ -24851,7 +25989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF32"/>
   <sheetViews>
@@ -27948,7 +29086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -28026,7 +29164,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
@@ -28045,16 +29183,16 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="336" t="s">
+      <c r="B3" s="338" t="s">
         <v>229</v>
       </c>
-      <c r="C3" s="336"/>
-      <c r="D3" s="336"/>
-      <c r="E3" s="336" t="s">
+      <c r="C3" s="338"/>
+      <c r="D3" s="338"/>
+      <c r="E3" s="338" t="s">
         <v>230</v>
       </c>
-      <c r="F3" s="336"/>
-      <c r="G3" s="336"/>
+      <c r="F3" s="338"/>
+      <c r="G3" s="338"/>
     </row>
     <row r="4" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="311" t="s">
@@ -28901,11 +30039,11 @@
       <c r="A30" t="s">
         <v>241</v>
       </c>
-      <c r="B30" s="336">
+      <c r="B30" s="338">
         <v>110</v>
       </c>
-      <c r="C30" s="336"/>
-      <c r="D30" s="336"/>
+      <c r="C30" s="338"/>
+      <c r="D30" s="338"/>
       <c r="E30">
         <v>18</v>
       </c>
@@ -28935,7 +30073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -28960,14 +30098,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="337" t="s">
+      <c r="C3" s="339" t="s">
         <v>244</v>
       </c>
-      <c r="D3" s="337"/>
-      <c r="E3" s="337" t="s">
+      <c r="D3" s="339"/>
+      <c r="E3" s="339" t="s">
         <v>245</v>
       </c>
-      <c r="F3" s="337"/>
+      <c r="F3" s="339"/>
     </row>
     <row r="4" spans="1:6" s="305" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="311" t="s">
@@ -29180,68 +30318,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="306" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>209</v>
-      </c>
-      <c r="B4">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>254</v>
-      </c>
-      <c r="B5">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>255</v>
-      </c>
-      <c r="B6">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>256</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove extra rows from ODS conversion
</commit_message>
<xml_diff>
--- a/MUSCShield_form.xlsx
+++ b/MUSCShield_form.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8190" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8190" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -3794,6 +3794,12 @@
     <xf numFmtId="164" fontId="24" fillId="0" borderId="8" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="24" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3804,12 +3810,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5264,13 +5264,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>155067</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5809,9 +5809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:H5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -24989,6 +24987,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="AB34:AD34"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="H34:L34"/>
+    <mergeCell ref="M34:Q34"/>
+    <mergeCell ref="R34:V34"/>
+    <mergeCell ref="W34:AA34"/>
+    <mergeCell ref="AA2:AC2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="V2:X2"/>
     <mergeCell ref="AA24:AC24"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="G12:I12"/>
@@ -25001,18 +25011,6 @@
     <mergeCell ref="L24:N24"/>
     <mergeCell ref="Q24:S24"/>
     <mergeCell ref="V24:X24"/>
-    <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="AB34:AD34"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="H34:L34"/>
-    <mergeCell ref="M34:Q34"/>
-    <mergeCell ref="R34:V34"/>
-    <mergeCell ref="W34:AA34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25020,11 +25018,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R88"/>
+  <dimension ref="A1:R82"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54:F66"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -25032,8 +25028,8 @@
     <col min="2" max="16" width="8.6640625" style="306" customWidth="1"/>
     <col min="17" max="17" width="8.6640625" style="321" customWidth="1"/>
     <col min="18" max="18" width="8.6640625" style="314" customWidth="1"/>
-    <col min="19" max="1026" width="8.6640625" style="306" customWidth="1"/>
-    <col min="1027" max="16384" width="9.33203125" style="306"/>
+    <col min="19" max="20" width="8.6640625" style="306" customWidth="1"/>
+    <col min="21" max="16384" width="9.33203125" style="306"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -25052,8 +25048,8 @@
       <c r="A2" s="321" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="331"/>
-      <c r="C2" s="332"/>
+      <c r="B2" s="333"/>
+      <c r="C2" s="334"/>
       <c r="R2" s="314" t="s">
         <v>318</v>
       </c>
@@ -25078,22 +25074,22 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B5" s="333" t="s">
+      <c r="B5" s="335" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="333"/>
-      <c r="D5" s="333" t="s">
+      <c r="C5" s="335"/>
+      <c r="D5" s="335" t="s">
         <v>328</v>
       </c>
-      <c r="E5" s="333"/>
-      <c r="F5" s="333"/>
-      <c r="J5" s="334" t="s">
+      <c r="E5" s="335"/>
+      <c r="F5" s="335"/>
+      <c r="J5" s="336" t="s">
         <v>305</v>
       </c>
-      <c r="K5" s="333"/>
-      <c r="L5" s="333"/>
-      <c r="M5" s="333"/>
-      <c r="N5" s="333"/>
+      <c r="K5" s="335"/>
+      <c r="L5" s="335"/>
+      <c r="M5" s="335"/>
+      <c r="N5" s="335"/>
       <c r="R5" s="314" t="s">
         <v>321</v>
       </c>
@@ -25256,13 +25252,13 @@
         <f>NCRP147_4.7!H8</f>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="J9" s="335" t="s">
+      <c r="J9" s="331" t="s">
         <v>306</v>
       </c>
-      <c r="K9" s="336"/>
-      <c r="L9" s="336"/>
-      <c r="M9" s="336"/>
-      <c r="N9" s="336"/>
+      <c r="K9" s="332"/>
+      <c r="L9" s="332"/>
+      <c r="M9" s="332"/>
+      <c r="N9" s="332"/>
       <c r="Q9" s="321" t="s">
         <v>195</v>
       </c>
@@ -25396,13 +25392,13 @@
         <v>309</v>
       </c>
       <c r="B13" s="312"/>
-      <c r="J13" s="335" t="s">
+      <c r="J13" s="331" t="s">
         <v>303</v>
       </c>
-      <c r="K13" s="336"/>
-      <c r="L13" s="336"/>
-      <c r="M13" s="336"/>
-      <c r="N13" s="336"/>
+      <c r="K13" s="332"/>
+      <c r="L13" s="332"/>
+      <c r="M13" s="332"/>
+      <c r="N13" s="332"/>
       <c r="Q13" s="321" t="s">
         <v>322</v>
       </c>
@@ -25494,13 +25490,13 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B17"/>
-      <c r="J17" s="335" t="s">
+      <c r="J17" s="331" t="s">
         <v>304</v>
       </c>
-      <c r="K17" s="336"/>
-      <c r="L17" s="336"/>
-      <c r="M17" s="336"/>
-      <c r="N17" s="336"/>
+      <c r="K17" s="332"/>
+      <c r="L17" s="332"/>
+      <c r="M17" s="332"/>
+      <c r="N17" s="332"/>
       <c r="Q17" s="321" t="s">
         <v>324</v>
       </c>
@@ -27099,30 +27095,6 @@
       </c>
       <c r="Q82" s="2"/>
       <c r="R82" s="322"/>
-    </row>
-    <row r="83" spans="1:18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="Q83" s="2"/>
-      <c r="R83" s="322"/>
-    </row>
-    <row r="84" spans="1:18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="Q84" s="2"/>
-      <c r="R84" s="322"/>
-    </row>
-    <row r="85" spans="1:18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="Q85" s="2"/>
-      <c r="R85" s="322"/>
-    </row>
-    <row r="86" spans="1:18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="Q86" s="2"/>
-      <c r="R86" s="322"/>
-    </row>
-    <row r="87" spans="1:18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="Q87" s="2"/>
-      <c r="R87" s="322"/>
-    </row>
-    <row r="88" spans="1:18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="Q88" s="2"/>
-      <c r="R88" s="322"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -27145,9 +27117,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V71"/>
+  <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -28610,133 +28582,6 @@
       <c r="N50" s="232"/>
       <c r="O50" s="231"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J51" s="232"/>
-      <c r="K51" s="234"/>
-      <c r="L51" s="233"/>
-      <c r="M51" s="232"/>
-      <c r="N51" s="232"/>
-      <c r="O51" s="231"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J52" s="232"/>
-      <c r="K52" s="234"/>
-      <c r="L52" s="233"/>
-      <c r="M52" s="232"/>
-      <c r="N52" s="232"/>
-      <c r="O52" s="231"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J53" s="232"/>
-      <c r="K53" s="234"/>
-      <c r="L53" s="233"/>
-      <c r="M53" s="232"/>
-      <c r="N53" s="232"/>
-      <c r="O53" s="231"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J54" s="232"/>
-      <c r="K54" s="234"/>
-      <c r="L54" s="233"/>
-      <c r="M54" s="232"/>
-      <c r="N54" s="232"/>
-      <c r="O54" s="231"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J55" s="232"/>
-      <c r="K55" s="234"/>
-      <c r="L55" s="233"/>
-      <c r="M55" s="232"/>
-      <c r="N55" s="232"/>
-      <c r="O55" s="231"/>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J56" s="232"/>
-      <c r="K56" s="234"/>
-      <c r="L56" s="233"/>
-      <c r="M56" s="232"/>
-      <c r="N56" s="232"/>
-      <c r="O56" s="231"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J57" s="232"/>
-      <c r="K57" s="234"/>
-      <c r="L57" s="233"/>
-      <c r="M57" s="232"/>
-      <c r="N57" s="232"/>
-      <c r="O57" s="231"/>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J58" s="232"/>
-      <c r="K58" s="234"/>
-      <c r="L58" s="233"/>
-      <c r="M58" s="232"/>
-      <c r="N58" s="232"/>
-      <c r="O58" s="231"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J59" s="232"/>
-      <c r="K59" s="234"/>
-      <c r="L59" s="233"/>
-      <c r="M59" s="232"/>
-      <c r="N59" s="232"/>
-      <c r="O59" s="231"/>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J60" s="232"/>
-      <c r="K60" s="234"/>
-      <c r="L60" s="233"/>
-      <c r="M60" s="232"/>
-      <c r="N60" s="232"/>
-      <c r="O60" s="231"/>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J61" s="232"/>
-      <c r="K61" s="234"/>
-      <c r="L61" s="233"/>
-      <c r="M61" s="232"/>
-      <c r="N61" s="232"/>
-      <c r="O61" s="231"/>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J62" s="232"/>
-      <c r="K62" s="234"/>
-      <c r="L62" s="233"/>
-      <c r="M62" s="232"/>
-      <c r="N62" s="232"/>
-      <c r="O62" s="231"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J64"/>
-    </row>
-    <row r="65" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J65"/>
-      <c r="K65" s="215"/>
-    </row>
-    <row r="66" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J66"/>
-      <c r="K66" s="215"/>
-    </row>
-    <row r="67" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J67"/>
-      <c r="K67" s="215"/>
-    </row>
-    <row r="68" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J68"/>
-      <c r="K68" s="215"/>
-    </row>
-    <row r="69" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J69"/>
-      <c r="K69" s="215"/>
-    </row>
-    <row r="70" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J70"/>
-      <c r="K70" s="215"/>
-    </row>
-    <row r="71" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J71" s="215"/>
-      <c r="K71" s="215"/>
-    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="Q18:V18"/>
@@ -28757,7 +28602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Add WIP sheet for NM shielding
</commit_message>
<xml_diff>
--- a/MUSCShield_form.xlsx
+++ b/MUSCShield_form.xlsx
@@ -9,26 +9,30 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8190" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
     <sheet name="RadFluoro" sheetId="5" r:id="rId2"/>
-    <sheet name="CT" sheetId="4" r:id="rId3"/>
-    <sheet name="ShieldEvaluation" sheetId="2" r:id="rId4"/>
-    <sheet name="FitParameters" sheetId="3" r:id="rId5"/>
-    <sheet name="NCRP147_4.1" sheetId="16" r:id="rId6"/>
-    <sheet name="NCRP147_4.2" sheetId="17" r:id="rId7"/>
-    <sheet name="NCRP147_4.3" sheetId="18" r:id="rId8"/>
-    <sheet name="NCRP147_4.4" sheetId="19" r:id="rId9"/>
-    <sheet name="NCRP147_4.5" sheetId="26" r:id="rId10"/>
-    <sheet name="NCRP147_4.7" sheetId="20" r:id="rId11"/>
-    <sheet name="NCRP147_5.2" sheetId="21" r:id="rId12"/>
-    <sheet name="NCRP147_A1" sheetId="22" r:id="rId13"/>
-    <sheet name="NCRP147_B1" sheetId="23" r:id="rId14"/>
-    <sheet name="NCRP147_C1" sheetId="24" r:id="rId15"/>
-    <sheet name="W_Rh_Al_Ag" sheetId="25" r:id="rId16"/>
+    <sheet name="NM" sheetId="27" r:id="rId3"/>
+    <sheet name="CT" sheetId="4" r:id="rId4"/>
+    <sheet name="ShieldEvaluation" sheetId="2" r:id="rId5"/>
+    <sheet name="FitParameters" sheetId="3" r:id="rId6"/>
+    <sheet name="NCRP147_4.1" sheetId="16" r:id="rId7"/>
+    <sheet name="NCRP147_4.2" sheetId="17" r:id="rId8"/>
+    <sheet name="NCRP147_4.3" sheetId="18" r:id="rId9"/>
+    <sheet name="NCRP147_4.4" sheetId="19" r:id="rId10"/>
+    <sheet name="NCRP147_4.5" sheetId="26" r:id="rId11"/>
+    <sheet name="NCRP147_4.7" sheetId="20" r:id="rId12"/>
+    <sheet name="NCRP147_5.2" sheetId="21" r:id="rId13"/>
+    <sheet name="NCRP147_A1" sheetId="22" r:id="rId14"/>
+    <sheet name="NCRP147_B1" sheetId="23" r:id="rId15"/>
+    <sheet name="NCRP147_C1" sheetId="24" r:id="rId16"/>
+    <sheet name="W_Rh_Al_Ag" sheetId="25" r:id="rId17"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId18"/>
+  </externalReferences>
   <definedNames>
     <definedName name="FitParams">FitParameters!$A$5:$AF$30</definedName>
     <definedName name="inch_value">Table!$AF$6:$AF$41</definedName>
@@ -52,11 +56,18 @@
     <definedName name="KsRFRadSS">RadFluoro!$F$11</definedName>
     <definedName name="minimum_Pb">Table!$AG$6:$AG$41</definedName>
     <definedName name="mm_value">Table!$AE$6:$AE$41</definedName>
+    <definedName name="NDAY">NM!$B$2</definedName>
     <definedName name="Nfl">RadFluoro!$B$13</definedName>
     <definedName name="Nrad">RadFluoro!$B$14</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">CT!$A$1:$H$50</definedName>
+    <definedName name="NWEEK">NM!$B$3</definedName>
+    <definedName name="PBHVL">NM!$M$18</definedName>
+    <definedName name="PBMU">NM!$M$17</definedName>
+    <definedName name="PBMURHO">NM!$M$15</definedName>
+    <definedName name="PBRHO">NM!$M$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">CT!$A$1:$H$50</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">NM!$A$1:$Q$73</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">RadFluoro!$A$1:$N$66</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">ShieldEvaluation!$A$1:$H$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">ShieldEvaluation!$A$1:$H$34</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Table!$A$1:$N$112</definedName>
     <definedName name="RefDist">ShieldEvaluation!$F$16</definedName>
     <definedName name="RefExp">ShieldEvaluation!$G$16</definedName>
@@ -293,6 +304,162 @@
     <author>Eugene Mah</author>
   </authors>
   <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Gamma ray exposure constant from Table 22-4, Cherry, Sorenson, Phelps, Physics in Nuclear Medicine 3ed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Assumes activity in patient is attenuated by ~1 HVL of soft tissue (about 5 cm)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction of hour @ avg. activity</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Assumes 0.15 voided activity factor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Type of area
+C - Controlled
+U - Uncontrolled</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B47" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Sum of the exposures from the source areas to each target area</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eugene Mah</author>
+  </authors>
+  <commentList>
     <comment ref="Q18" authorId="0" shapeId="0">
       <text>
         <r>
@@ -493,7 +660,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Eugene Mah</author>
@@ -766,7 +933,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="392">
   <si>
     <t>Shielding Calculations</t>
   </si>
@@ -2152,6 +2319,183 @@
   </si>
   <si>
     <t>Ksec(tot)</t>
+  </si>
+  <si>
+    <t>Tc-99m</t>
+  </si>
+  <si>
+    <t>mSv-m^2/MBq-h</t>
+  </si>
+  <si>
+    <t>Activity Calculations</t>
+  </si>
+  <si>
+    <t>N/day</t>
+  </si>
+  <si>
+    <t>mCi</t>
+  </si>
+  <si>
+    <t>MBq</t>
+  </si>
+  <si>
+    <t>N/week</t>
+  </si>
+  <si>
+    <t>Patients per week</t>
+  </si>
+  <si>
+    <t>Administered activity</t>
+  </si>
+  <si>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>Avg activity (MBq)</t>
+  </si>
+  <si>
+    <t>Work factor</t>
+  </si>
+  <si>
+    <t>MBq-h/wk</t>
+  </si>
+  <si>
+    <t>mSv-m^2/wk</t>
+  </si>
+  <si>
+    <t>Equivalent unshielded activity in patient</t>
+  </si>
+  <si>
+    <t>Hot lab</t>
+  </si>
+  <si>
+    <t>Uptake duration (minutes)</t>
+  </si>
+  <si>
+    <t>NM Hold 1</t>
+  </si>
+  <si>
+    <t>Avg activity during uptake</t>
+  </si>
+  <si>
+    <t>NM Hold 2</t>
+  </si>
+  <si>
+    <t>Activity at end of uptake</t>
+  </si>
+  <si>
+    <t>NM Camera 1</t>
+  </si>
+  <si>
+    <t>Activity following void</t>
+  </si>
+  <si>
+    <t>NM Camera 2</t>
+  </si>
+  <si>
+    <t>Scan duration (minutes)</t>
+  </si>
+  <si>
+    <t>Stress Lab</t>
+  </si>
+  <si>
+    <t>Avg activity during scan</t>
+  </si>
+  <si>
+    <t>Hot Toilet</t>
+  </si>
+  <si>
+    <t>Activty at end of scan</t>
+  </si>
+  <si>
+    <t>Radiology Waiting</t>
+  </si>
+  <si>
+    <t>Lead mass attenuation coeff</t>
+  </si>
+  <si>
+    <t>Lead density</t>
+  </si>
+  <si>
+    <t>Areas</t>
+  </si>
+  <si>
+    <t>Dose limit (mSv/wk)</t>
+  </si>
+  <si>
+    <t>Target limit</t>
+  </si>
+  <si>
+    <t>Lead attenuation coeff (1/cm)</t>
+  </si>
+  <si>
+    <t>Tech area</t>
+  </si>
+  <si>
+    <t>Lead HVL (mm)</t>
+  </si>
+  <si>
+    <t>CT Tech area</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>US 1</t>
+  </si>
+  <si>
+    <t>US 2</t>
+  </si>
+  <si>
+    <t>Office 2221</t>
+  </si>
+  <si>
+    <t>Office 2302</t>
+  </si>
+  <si>
+    <t>Consult A</t>
+  </si>
+  <si>
+    <t>Consult B</t>
+  </si>
+  <si>
+    <t>Lactation</t>
+  </si>
+  <si>
+    <t>Reading Room</t>
+  </si>
+  <si>
+    <t>Distances (m)</t>
+  </si>
+  <si>
+    <t>Unshielded exposures (mSv/wk)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Required shielding</t>
+  </si>
+  <si>
+    <t>Unshielded Exp</t>
+  </si>
+  <si>
+    <t>Atten factor</t>
+  </si>
+  <si>
+    <t>HVLs</t>
+  </si>
+  <si>
+    <t>Lead thickness (mm)</t>
+  </si>
+  <si>
+    <t>Target area</t>
+  </si>
+  <si>
+    <t>Source area</t>
+  </si>
+  <si>
+    <t>Required shielding for each target area from each source area</t>
   </si>
 </sst>
 </file>
@@ -2396,7 +2740,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -2935,6 +3279,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2950,7 +3307,7 @@
     </xf>
     <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="349">
+  <cellXfs count="372">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -3848,6 +4205,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3857,7 +4283,15 @@
     <cellStyle name="Normal_shieldevaluation" xfId="1"/>
     <cellStyle name="Percent 2" xfId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3910,7 +4344,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4317,7 +4750,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4435,7 +4867,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4539,7 +4970,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4635,7 +5065,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5435,6 +5864,75 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Table"/>
+      <sheetName val="RadFluoro"/>
+      <sheetName val="CT"/>
+      <sheetName val="NM"/>
+      <sheetName val="ShieldEvaluation"/>
+      <sheetName val="FitParameters"/>
+      <sheetName val="NCRP147_4.1"/>
+      <sheetName val="NCRP147_4.2"/>
+      <sheetName val="NCRP147_4.3"/>
+      <sheetName val="NCRP147_4.4"/>
+      <sheetName val="NCRP147_4.5"/>
+      <sheetName val="NCRP147_4.7"/>
+      <sheetName val="NCRP147_5.2"/>
+      <sheetName val="NCRP147_A1"/>
+      <sheetName val="NCRP147_B1"/>
+      <sheetName val="NCRP147_C1"/>
+      <sheetName val="W_Rh_Al_Ag"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="AE6">
+            <v>-25.4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="7">
+          <cell r="C7">
+            <v>5.2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="19">
+          <cell r="B19" t="str">
+            <v>Patients per day</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
+        <row r="16">
+          <cell r="H16" t="str">
+            <v/>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -15175,6 +15673,68 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="292" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15250,7 +15810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
@@ -15623,7 +16183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -15727,7 +16287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ61"/>
   <sheetViews>
@@ -19735,7 +20295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE13"/>
   <sheetViews>
@@ -20866,7 +21426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE21"/>
   <sheetViews>
@@ -22659,7 +23219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF39"/>
   <sheetViews>
@@ -24987,18 +25547,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="AB34:AD34"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="H34:L34"/>
-    <mergeCell ref="M34:Q34"/>
-    <mergeCell ref="R34:V34"/>
-    <mergeCell ref="W34:AA34"/>
-    <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="V2:X2"/>
     <mergeCell ref="AA24:AC24"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="G12:I12"/>
@@ -25011,6 +25559,18 @@
     <mergeCell ref="L24:N24"/>
     <mergeCell ref="Q24:S24"/>
     <mergeCell ref="V24:X24"/>
+    <mergeCell ref="AA2:AC2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="AB34:AD34"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="H34:L34"/>
+    <mergeCell ref="M34:Q34"/>
+    <mergeCell ref="R34:V34"/>
+    <mergeCell ref="W34:AA34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27113,6 +27673,2725 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" style="349" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="349" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="349" customWidth="1"/>
+    <col min="4" max="4" width="11" style="349" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="349" customWidth="1"/>
+    <col min="6" max="11" width="10.6640625" style="349" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" style="349" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="349" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.33203125" style="349"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="349" t="s">
+        <v>333</v>
+      </c>
+      <c r="B1" s="350">
+        <v>3.3170000000000003E-5</v>
+      </c>
+      <c r="C1" s="349" t="s">
+        <v>334</v>
+      </c>
+      <c r="H1" s="351"/>
+      <c r="L1" s="351" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="349" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" s="349">
+        <v>20</v>
+      </c>
+      <c r="C2" s="349" t="str">
+        <f>[1]CT!B19</f>
+        <v>Patients per day</v>
+      </c>
+      <c r="L2" s="349" t="s">
+        <v>337</v>
+      </c>
+      <c r="M2" s="349" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="349" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" s="349">
+        <f>NDAY*5</f>
+        <v>100</v>
+      </c>
+      <c r="C3" s="349" t="s">
+        <v>340</v>
+      </c>
+      <c r="L3" s="352">
+        <v>30</v>
+      </c>
+      <c r="M3" s="352">
+        <f>L3*37</f>
+        <v>1110</v>
+      </c>
+      <c r="N3" s="349" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L4" s="355">
+        <f>L3/(2^1)</f>
+        <v>15</v>
+      </c>
+      <c r="M4" s="355">
+        <f>M3/(2^1)</f>
+        <v>555</v>
+      </c>
+      <c r="N4" s="349" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="353" t="s">
+        <v>342</v>
+      </c>
+      <c r="L5" s="352"/>
+      <c r="M5" s="352">
+        <v>60</v>
+      </c>
+      <c r="N5" s="349" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="354" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B6" s="363" t="s">
+        <v>343</v>
+      </c>
+      <c r="C6" s="363" t="s">
+        <v>344</v>
+      </c>
+      <c r="D6" s="363" t="s">
+        <v>345</v>
+      </c>
+      <c r="E6" s="363" t="s">
+        <v>346</v>
+      </c>
+      <c r="L6" s="352">
+        <f>L4*1.443*109.8*(1-EXP(-LN(2)*M5/109.8))/M5</f>
+        <v>12.488993056193506</v>
+      </c>
+      <c r="M6" s="352">
+        <f>M4*1.443*109.8*(1-EXP(-LN(2)*M5/109.8))/M5</f>
+        <v>462.09274307915973</v>
+      </c>
+      <c r="N6" s="349" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="359" t="s">
+        <v>348</v>
+      </c>
+      <c r="B7" s="361">
+        <f>M3</f>
+        <v>1110</v>
+      </c>
+      <c r="C7" s="360">
+        <v>0.05</v>
+      </c>
+      <c r="D7" s="361">
+        <f>B7*C7*40*NWEEK</f>
+        <v>222000</v>
+      </c>
+      <c r="E7" s="362">
+        <f>D7*$B$1</f>
+        <v>7.3637400000000008</v>
+      </c>
+      <c r="L7" s="352">
+        <f>L4*EXP(-LN(2)*M5/109.8)</f>
+        <v>10.270556916490195</v>
+      </c>
+      <c r="M7" s="352">
+        <f>M4*EXP(-LN(2)*M5/109.8)</f>
+        <v>380.01060591013726</v>
+      </c>
+      <c r="N7" s="349" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="359" t="s">
+        <v>350</v>
+      </c>
+      <c r="B8" s="361">
+        <f>M4</f>
+        <v>555</v>
+      </c>
+      <c r="C8" s="360">
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="361">
+        <f>B8*C8*40*NWEEK</f>
+        <v>444000</v>
+      </c>
+      <c r="E8" s="362">
+        <f t="shared" ref="E8:E14" si="0">D8*$B$1</f>
+        <v>14.727480000000002</v>
+      </c>
+      <c r="L8" s="352">
+        <f>L7*0.85</f>
+        <v>8.7299733790166663</v>
+      </c>
+      <c r="M8" s="352">
+        <f>M7*0.85</f>
+        <v>323.00901502361666</v>
+      </c>
+      <c r="N8" s="349" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="359" t="s">
+        <v>352</v>
+      </c>
+      <c r="B9" s="361">
+        <f>M4</f>
+        <v>555</v>
+      </c>
+      <c r="C9" s="360">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="361">
+        <f>B9*C9*40*NWEEK</f>
+        <v>444000</v>
+      </c>
+      <c r="E9" s="362">
+        <f t="shared" si="0"/>
+        <v>14.727480000000002</v>
+      </c>
+      <c r="L9" s="352"/>
+      <c r="M9" s="352">
+        <v>15</v>
+      </c>
+      <c r="N9" s="349" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="359" t="s">
+        <v>354</v>
+      </c>
+      <c r="B10" s="361">
+        <f>M8</f>
+        <v>323.00901502361666</v>
+      </c>
+      <c r="C10" s="360">
+        <v>0.4</v>
+      </c>
+      <c r="D10" s="361">
+        <f>B10*C10*40*NWEEK</f>
+        <v>516814.42403778672</v>
+      </c>
+      <c r="E10" s="362">
+        <f t="shared" si="0"/>
+        <v>17.142734445333389</v>
+      </c>
+      <c r="L10" s="352">
+        <f>L8*1.443*109.8*(1-EXP(-LN(2)*M9/109.8))/M9</f>
+        <v>8.3311470022494643</v>
+      </c>
+      <c r="M10" s="352">
+        <f>M8*1.443*109.8*(1-EXP(-LN(2)*M9/109.8))/M9</f>
+        <v>308.25243908323023</v>
+      </c>
+      <c r="N10" s="349" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="359" t="s">
+        <v>356</v>
+      </c>
+      <c r="B11" s="361">
+        <f>M8</f>
+        <v>323.00901502361666</v>
+      </c>
+      <c r="C11" s="360">
+        <v>0.4</v>
+      </c>
+      <c r="D11" s="361">
+        <f>B11*C11*40*NWEEK</f>
+        <v>516814.42403778672</v>
+      </c>
+      <c r="E11" s="362">
+        <f t="shared" si="0"/>
+        <v>17.142734445333389</v>
+      </c>
+      <c r="L11" s="352">
+        <f>L8*EXP(-LN(2)*M9/109.8)</f>
+        <v>7.9412451486820315</v>
+      </c>
+      <c r="M11" s="352">
+        <f>M8*EXP(-LN(2)*M9/109.8)</f>
+        <v>293.82607050123517</v>
+      </c>
+      <c r="N11" s="349" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="359" t="s">
+        <v>358</v>
+      </c>
+      <c r="B12" s="361">
+        <f>M4</f>
+        <v>555</v>
+      </c>
+      <c r="C12" s="360">
+        <v>0.4</v>
+      </c>
+      <c r="D12" s="361">
+        <f>B12*C12*40*NWEEK</f>
+        <v>888000</v>
+      </c>
+      <c r="E12" s="362">
+        <f t="shared" si="0"/>
+        <v>29.454960000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="359" t="s">
+        <v>360</v>
+      </c>
+      <c r="B13" s="361">
+        <f>M7</f>
+        <v>380.01060591013726</v>
+      </c>
+      <c r="C13" s="360">
+        <v>0.3</v>
+      </c>
+      <c r="D13" s="361">
+        <f>B13*C13*40*NWEEK</f>
+        <v>456012.72709216474</v>
+      </c>
+      <c r="E13" s="362">
+        <f t="shared" si="0"/>
+        <v>15.125942157647106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="359" t="s">
+        <v>362</v>
+      </c>
+      <c r="B14" s="361">
+        <f>M6</f>
+        <v>462.09274307915973</v>
+      </c>
+      <c r="C14" s="360">
+        <v>0.75</v>
+      </c>
+      <c r="D14" s="361">
+        <f>B14*C14*40*NWEEK</f>
+        <v>1386278.2292374792</v>
+      </c>
+      <c r="E14" s="362">
+        <f t="shared" si="0"/>
+        <v>45.982848863807185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M15" s="349">
+        <v>2.2650000000000001</v>
+      </c>
+      <c r="N15" s="349" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="351" t="s">
+        <v>365</v>
+      </c>
+      <c r="M16" s="349">
+        <v>11.34</v>
+      </c>
+      <c r="N16" s="349" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B17" s="360" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="360" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="360" t="s">
+        <v>162</v>
+      </c>
+      <c r="E17" s="360" t="s">
+        <v>366</v>
+      </c>
+      <c r="F17" s="360" t="s">
+        <v>367</v>
+      </c>
+      <c r="M17" s="349">
+        <f>M15*M16</f>
+        <v>25.685100000000002</v>
+      </c>
+      <c r="N17" s="349" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="360">
+        <v>1</v>
+      </c>
+      <c r="B18" s="360" t="s">
+        <v>369</v>
+      </c>
+      <c r="C18" s="360" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="360">
+        <v>1</v>
+      </c>
+      <c r="E18" s="360">
+        <f>IF(C18="U",0.02,IF(C18="C",0.1,""))</f>
+        <v>0.02</v>
+      </c>
+      <c r="F18" s="359">
+        <f>E18/D18</f>
+        <v>0.02</v>
+      </c>
+      <c r="M18" s="356">
+        <f>LN(2)/M17*10</f>
+        <v>0.26986353199323548</v>
+      </c>
+      <c r="N18" s="349" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="360">
+        <v>2</v>
+      </c>
+      <c r="B19" s="360" t="s">
+        <v>371</v>
+      </c>
+      <c r="C19" s="360" t="s">
+        <v>372</v>
+      </c>
+      <c r="D19" s="360">
+        <v>1</v>
+      </c>
+      <c r="E19" s="360">
+        <f t="shared" ref="E19:E29" si="1">IF(C19="U",0.02,IF(C19="C",0.1,""))</f>
+        <v>0.1</v>
+      </c>
+      <c r="F19" s="359">
+        <f t="shared" ref="F19:F29" si="2">E19/D19</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="360">
+        <v>3</v>
+      </c>
+      <c r="B20" s="360" t="s">
+        <v>373</v>
+      </c>
+      <c r="C20" s="360" t="s">
+        <v>191</v>
+      </c>
+      <c r="D20" s="360">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="360">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="F20" s="359">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="360">
+        <v>4</v>
+      </c>
+      <c r="B21" s="360" t="s">
+        <v>374</v>
+      </c>
+      <c r="C21" s="360" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="360">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="360">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="F21" s="359">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="360">
+        <v>5</v>
+      </c>
+      <c r="B22" s="360" t="s">
+        <v>375</v>
+      </c>
+      <c r="C22" s="360" t="s">
+        <v>191</v>
+      </c>
+      <c r="D22" s="360">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="360">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="F22" s="359">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="360">
+        <v>6</v>
+      </c>
+      <c r="B23" s="360" t="s">
+        <v>376</v>
+      </c>
+      <c r="C23" s="360" t="s">
+        <v>191</v>
+      </c>
+      <c r="D23" s="360">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="360">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="F23" s="359">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="360">
+        <v>7</v>
+      </c>
+      <c r="B24" s="360" t="s">
+        <v>377</v>
+      </c>
+      <c r="C24" s="360" t="s">
+        <v>191</v>
+      </c>
+      <c r="D24" s="360">
+        <v>0.1</v>
+      </c>
+      <c r="E24" s="360">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="F24" s="359">
+        <f t="shared" si="2"/>
+        <v>0.19999999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="360">
+        <v>8</v>
+      </c>
+      <c r="B25" s="360" t="s">
+        <v>378</v>
+      </c>
+      <c r="C25" s="360" t="s">
+        <v>191</v>
+      </c>
+      <c r="D25" s="360">
+        <v>0.1</v>
+      </c>
+      <c r="E25" s="360">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="F25" s="359">
+        <f t="shared" si="2"/>
+        <v>0.19999999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="360">
+        <v>9</v>
+      </c>
+      <c r="B26" s="360" t="s">
+        <v>379</v>
+      </c>
+      <c r="C26" s="360" t="s">
+        <v>191</v>
+      </c>
+      <c r="D26" s="360">
+        <v>0.1</v>
+      </c>
+      <c r="E26" s="360">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="F26" s="359">
+        <f t="shared" si="2"/>
+        <v>0.19999999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="360">
+        <v>10</v>
+      </c>
+      <c r="B27" s="360" t="s">
+        <v>380</v>
+      </c>
+      <c r="C27" s="360" t="s">
+        <v>372</v>
+      </c>
+      <c r="D27" s="360">
+        <v>1</v>
+      </c>
+      <c r="E27" s="360">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="F27" s="359">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="360">
+        <v>11</v>
+      </c>
+      <c r="B28" s="360" t="s">
+        <v>196</v>
+      </c>
+      <c r="C28" s="360" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" s="360">
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="360">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="F28" s="359">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="360">
+        <v>12</v>
+      </c>
+      <c r="B29" s="360" t="s">
+        <v>197</v>
+      </c>
+      <c r="C29" s="360" t="s">
+        <v>191</v>
+      </c>
+      <c r="D29" s="360">
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="360">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="F29" s="359">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="358" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C32" s="364" t="s">
+        <v>389</v>
+      </c>
+      <c r="D32" s="364"/>
+      <c r="E32" s="364"/>
+      <c r="F32" s="364"/>
+      <c r="G32" s="364"/>
+      <c r="H32" s="364"/>
+      <c r="I32" s="364"/>
+      <c r="J32" s="364"/>
+      <c r="K32" s="364"/>
+      <c r="L32" s="364"/>
+      <c r="M32" s="364"/>
+      <c r="N32" s="364"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C33" s="360" t="s">
+        <v>369</v>
+      </c>
+      <c r="D33" s="360" t="s">
+        <v>371</v>
+      </c>
+      <c r="E33" s="360" t="s">
+        <v>373</v>
+      </c>
+      <c r="F33" s="360" t="s">
+        <v>374</v>
+      </c>
+      <c r="G33" s="360" t="s">
+        <v>375</v>
+      </c>
+      <c r="H33" s="360" t="s">
+        <v>376</v>
+      </c>
+      <c r="I33" s="360" t="s">
+        <v>377</v>
+      </c>
+      <c r="J33" s="360" t="s">
+        <v>378</v>
+      </c>
+      <c r="K33" s="360" t="s">
+        <v>379</v>
+      </c>
+      <c r="L33" s="360" t="s">
+        <v>380</v>
+      </c>
+      <c r="M33" s="359" t="s">
+        <v>196</v>
+      </c>
+      <c r="N33" s="359" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="364" t="s">
+        <v>390</v>
+      </c>
+      <c r="B34" s="359" t="str">
+        <f>A7</f>
+        <v>Hot lab</v>
+      </c>
+      <c r="C34" s="361">
+        <f>48*12*0.0254</f>
+        <v>14.6304</v>
+      </c>
+      <c r="D34" s="361">
+        <f>39*12*0.0254</f>
+        <v>11.8872</v>
+      </c>
+      <c r="E34" s="361">
+        <f>29*12*0.0254</f>
+        <v>8.8391999999999999</v>
+      </c>
+      <c r="F34" s="361">
+        <f>44*12*0.0254</f>
+        <v>13.411199999999999</v>
+      </c>
+      <c r="G34" s="361">
+        <f>24*12*0.0254</f>
+        <v>7.3151999999999999</v>
+      </c>
+      <c r="H34" s="361">
+        <f>34*12*0.0254</f>
+        <v>10.363199999999999</v>
+      </c>
+      <c r="I34" s="361">
+        <f>23*12*0.0254</f>
+        <v>7.0103999999999997</v>
+      </c>
+      <c r="J34" s="361">
+        <f>20*12*0.0254</f>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="K34" s="361">
+        <f>22*12*0.0254</f>
+        <v>6.7055999999999996</v>
+      </c>
+      <c r="L34" s="361">
+        <f>9*12*0.0254</f>
+        <v>2.7431999999999999</v>
+      </c>
+      <c r="M34" s="361">
+        <f>20*12*0.0254</f>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="N34" s="361">
+        <f t="shared" ref="N34:N41" si="3">SQRT(2*(18^2))*12*0.0254</f>
+        <v>7.7589412886037472</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="364"/>
+      <c r="B35" s="359" t="str">
+        <f>A8</f>
+        <v>NM Hold 1</v>
+      </c>
+      <c r="C35" s="361">
+        <f>39*12*0.0254</f>
+        <v>11.8872</v>
+      </c>
+      <c r="D35" s="361">
+        <f>52*12*0.0254</f>
+        <v>15.849599999999999</v>
+      </c>
+      <c r="E35" s="361">
+        <f>57.5*12*0.0254</f>
+        <v>17.526</v>
+      </c>
+      <c r="F35" s="361">
+        <f>74*12*0.0254</f>
+        <v>22.555199999999999</v>
+      </c>
+      <c r="G35" s="361">
+        <f>56*12*0.0254</f>
+        <v>17.0688</v>
+      </c>
+      <c r="H35" s="361">
+        <f>65*12*0.0254</f>
+        <v>19.811999999999998</v>
+      </c>
+      <c r="I35" s="361">
+        <f>46*12*0.0254</f>
+        <v>14.020799999999999</v>
+      </c>
+      <c r="J35" s="361">
+        <f>38*12*0.0254</f>
+        <v>11.5824</v>
+      </c>
+      <c r="K35" s="361">
+        <f>28*12*0.0254</f>
+        <v>8.5343999999999998</v>
+      </c>
+      <c r="L35" s="361">
+        <f>40*12*0.0254</f>
+        <v>12.192</v>
+      </c>
+      <c r="M35" s="361">
+        <f t="shared" ref="M35:M41" si="4">20*12*0.0254</f>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="N35" s="361">
+        <f t="shared" si="3"/>
+        <v>7.7589412886037472</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="364"/>
+      <c r="B36" s="359" t="str">
+        <f>A9</f>
+        <v>NM Hold 2</v>
+      </c>
+      <c r="C36" s="361">
+        <f>43*12*0.0254</f>
+        <v>13.106399999999999</v>
+      </c>
+      <c r="D36" s="361">
+        <f>40*12*0.0254</f>
+        <v>12.192</v>
+      </c>
+      <c r="E36" s="361">
+        <f>36*12*0.0254</f>
+        <v>10.972799999999999</v>
+      </c>
+      <c r="F36" s="361">
+        <f>52*12*0.0254</f>
+        <v>15.849599999999999</v>
+      </c>
+      <c r="G36" s="361">
+        <f>32*12*0.0254</f>
+        <v>9.7535999999999987</v>
+      </c>
+      <c r="H36" s="361">
+        <f>43*12*0.0254</f>
+        <v>13.106399999999999</v>
+      </c>
+      <c r="I36" s="361">
+        <f>28*12*0.0254</f>
+        <v>8.5343999999999998</v>
+      </c>
+      <c r="J36" s="361">
+        <f>22*12*0.0254</f>
+        <v>6.7055999999999996</v>
+      </c>
+      <c r="K36" s="361">
+        <f>20*12*0.0254</f>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="L36" s="361">
+        <f>17*12*0.0254</f>
+        <v>5.1815999999999995</v>
+      </c>
+      <c r="M36" s="361">
+        <f t="shared" si="4"/>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="N36" s="361">
+        <f t="shared" si="3"/>
+        <v>7.7589412886037472</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="364"/>
+      <c r="B37" s="359" t="str">
+        <f>A10</f>
+        <v>NM Camera 1</v>
+      </c>
+      <c r="C37" s="361">
+        <f>25*12*0.0254</f>
+        <v>7.62</v>
+      </c>
+      <c r="D37" s="361">
+        <f>49*12*0.0254</f>
+        <v>14.9352</v>
+      </c>
+      <c r="E37" s="361">
+        <f>63*12*0.0254</f>
+        <v>19.202400000000001</v>
+      </c>
+      <c r="F37" s="361">
+        <f>80*12*0.0254</f>
+        <v>24.384</v>
+      </c>
+      <c r="G37" s="361">
+        <f>65*12*0.0254</f>
+        <v>19.811999999999998</v>
+      </c>
+      <c r="H37" s="361">
+        <f>76*12*0.0254</f>
+        <v>23.1648</v>
+      </c>
+      <c r="I37" s="361">
+        <f>62*12*0.0254</f>
+        <v>18.897600000000001</v>
+      </c>
+      <c r="J37" s="361">
+        <f>55*12*0.0254</f>
+        <v>16.763999999999999</v>
+      </c>
+      <c r="K37" s="361">
+        <f>46*12*0.0254</f>
+        <v>14.020799999999999</v>
+      </c>
+      <c r="L37" s="361">
+        <f>50*12*0.0254</f>
+        <v>15.24</v>
+      </c>
+      <c r="M37" s="361">
+        <f t="shared" si="4"/>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="N37" s="361">
+        <f t="shared" si="3"/>
+        <v>7.7589412886037472</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="364"/>
+      <c r="B38" s="359" t="str">
+        <f>A11</f>
+        <v>NM Camera 2</v>
+      </c>
+      <c r="C38" s="361">
+        <f>32.5*12*0.0254</f>
+        <v>9.9059999999999988</v>
+      </c>
+      <c r="D38" s="361">
+        <f>23*12*0.0254</f>
+        <v>7.0103999999999997</v>
+      </c>
+      <c r="E38" s="361">
+        <f>28*12*0.0254</f>
+        <v>8.5343999999999998</v>
+      </c>
+      <c r="F38" s="361">
+        <f>45*12*0.0254</f>
+        <v>13.715999999999999</v>
+      </c>
+      <c r="G38" s="361">
+        <f>31*12*0.0254</f>
+        <v>9.4488000000000003</v>
+      </c>
+      <c r="H38" s="361">
+        <f>42*12*0.0254</f>
+        <v>12.801599999999999</v>
+      </c>
+      <c r="I38" s="361">
+        <f>39*12*0.0254</f>
+        <v>11.8872</v>
+      </c>
+      <c r="J38" s="361">
+        <f>37*12*0.0254</f>
+        <v>11.2776</v>
+      </c>
+      <c r="K38" s="361">
+        <f>37*12*0.0254</f>
+        <v>11.2776</v>
+      </c>
+      <c r="L38" s="361">
+        <f>17*12*0.0254</f>
+        <v>5.1815999999999995</v>
+      </c>
+      <c r="M38" s="361">
+        <f t="shared" si="4"/>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="N38" s="361">
+        <f t="shared" si="3"/>
+        <v>7.7589412886037472</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="364"/>
+      <c r="B39" s="359" t="str">
+        <f>A12</f>
+        <v>Stress Lab</v>
+      </c>
+      <c r="C39" s="361">
+        <f>51*12*0.0254</f>
+        <v>15.544799999999999</v>
+      </c>
+      <c r="D39" s="361">
+        <f>28*12*0.0254</f>
+        <v>8.5343999999999998</v>
+      </c>
+      <c r="E39" s="361">
+        <f>5*12*0.0254</f>
+        <v>1.524</v>
+      </c>
+      <c r="F39" s="361">
+        <f>20*12*0.0254</f>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="G39" s="361">
+        <f>10*12*0.0254</f>
+        <v>3.048</v>
+      </c>
+      <c r="H39" s="361">
+        <f>17*12*0.0254</f>
+        <v>5.1815999999999995</v>
+      </c>
+      <c r="I39" s="361">
+        <f>35*12*0.0254</f>
+        <v>10.667999999999999</v>
+      </c>
+      <c r="J39" s="361">
+        <f>38*12*0.0254</f>
+        <v>11.5824</v>
+      </c>
+      <c r="K39" s="361">
+        <f>43*12*0.0254</f>
+        <v>13.106399999999999</v>
+      </c>
+      <c r="L39" s="361">
+        <f>8*12*0.0254</f>
+        <v>2.4383999999999997</v>
+      </c>
+      <c r="M39" s="361">
+        <f t="shared" si="4"/>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="N39" s="361">
+        <f t="shared" si="3"/>
+        <v>7.7589412886037472</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="364"/>
+      <c r="B40" s="359" t="str">
+        <f>A13</f>
+        <v>Hot Toilet</v>
+      </c>
+      <c r="C40" s="361">
+        <f>41*12*0.0254</f>
+        <v>12.4968</v>
+      </c>
+      <c r="D40" s="361">
+        <f>62*12*0.0254</f>
+        <v>18.897600000000001</v>
+      </c>
+      <c r="E40" s="361">
+        <f>72*12*0.0254</f>
+        <v>21.945599999999999</v>
+      </c>
+      <c r="F40" s="361">
+        <f>88*12*0.0254</f>
+        <v>26.822399999999998</v>
+      </c>
+      <c r="G40" s="361">
+        <f>69*12*0.0254</f>
+        <v>21.031199999999998</v>
+      </c>
+      <c r="H40" s="361">
+        <f>79*12*0.0254</f>
+        <v>24.0792</v>
+      </c>
+      <c r="I40" s="361">
+        <f>62*12*0.0254</f>
+        <v>18.897600000000001</v>
+      </c>
+      <c r="J40" s="361">
+        <f>50*12*0.0254</f>
+        <v>15.24</v>
+      </c>
+      <c r="K40" s="361">
+        <f>41*12*0.0254</f>
+        <v>12.4968</v>
+      </c>
+      <c r="L40" s="361">
+        <f>55.5*12*0.0254</f>
+        <v>16.916399999999999</v>
+      </c>
+      <c r="M40" s="361">
+        <f t="shared" si="4"/>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="N40" s="361">
+        <f t="shared" si="3"/>
+        <v>7.7589412886037472</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="364"/>
+      <c r="B41" s="359" t="str">
+        <f>A14</f>
+        <v>Radiology Waiting</v>
+      </c>
+      <c r="C41" s="361">
+        <f>80*12*0.0254</f>
+        <v>24.384</v>
+      </c>
+      <c r="D41" s="361">
+        <f>63*12*0.0254</f>
+        <v>19.202400000000001</v>
+      </c>
+      <c r="E41" s="361">
+        <f>37*12*0.0254</f>
+        <v>11.2776</v>
+      </c>
+      <c r="F41" s="361">
+        <f>40*12*0.0254</f>
+        <v>12.192</v>
+      </c>
+      <c r="G41" s="361">
+        <f>24*12*0.0254</f>
+        <v>7.3151999999999999</v>
+      </c>
+      <c r="H41" s="361">
+        <f>26*12*0.0254</f>
+        <v>7.9247999999999994</v>
+      </c>
+      <c r="I41" s="361">
+        <f>12*12*0.0254</f>
+        <v>3.6576</v>
+      </c>
+      <c r="J41" s="361">
+        <f>22*12*0.0254</f>
+        <v>6.7055999999999996</v>
+      </c>
+      <c r="K41" s="361">
+        <f>33*12*0.0254</f>
+        <v>10.058399999999999</v>
+      </c>
+      <c r="L41" s="361">
+        <f>20*12*0.0254</f>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="M41" s="361">
+        <f t="shared" si="4"/>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="N41" s="361">
+        <f t="shared" si="3"/>
+        <v>7.7589412886037472</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="351" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C45" s="364" t="s">
+        <v>389</v>
+      </c>
+      <c r="D45" s="364"/>
+      <c r="E45" s="364"/>
+      <c r="F45" s="364"/>
+      <c r="G45" s="364"/>
+      <c r="H45" s="364"/>
+      <c r="I45" s="364"/>
+      <c r="J45" s="364"/>
+      <c r="K45" s="364"/>
+      <c r="L45" s="364"/>
+      <c r="M45" s="364"/>
+      <c r="N45" s="364"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C46" s="360" t="str">
+        <f>C33</f>
+        <v>Tech area</v>
+      </c>
+      <c r="D46" s="360" t="str">
+        <f>D33</f>
+        <v>CT Tech area</v>
+      </c>
+      <c r="E46" s="360" t="str">
+        <f>E33</f>
+        <v>US 1</v>
+      </c>
+      <c r="F46" s="360" t="str">
+        <f>F33</f>
+        <v>US 2</v>
+      </c>
+      <c r="G46" s="360" t="str">
+        <f>G33</f>
+        <v>Office 2221</v>
+      </c>
+      <c r="H46" s="360" t="str">
+        <f>H33</f>
+        <v>Office 2302</v>
+      </c>
+      <c r="I46" s="360" t="str">
+        <f>I33</f>
+        <v>Consult A</v>
+      </c>
+      <c r="J46" s="360" t="str">
+        <f>J33</f>
+        <v>Consult B</v>
+      </c>
+      <c r="K46" s="360" t="str">
+        <f>K33</f>
+        <v>Lactation</v>
+      </c>
+      <c r="L46" s="360" t="str">
+        <f>L33</f>
+        <v>Reading Room</v>
+      </c>
+      <c r="M46" s="360" t="str">
+        <f>M33</f>
+        <v>Floor</v>
+      </c>
+      <c r="N46" s="360" t="str">
+        <f>N33</f>
+        <v>Ceiling</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B47" s="367" t="s">
+        <v>383</v>
+      </c>
+      <c r="C47" s="368">
+        <f>SUM(C48:C55)</f>
+        <v>0.9903830236204284</v>
+      </c>
+      <c r="D47" s="368">
+        <f t="shared" ref="D47:N47" si="5">SUM(D48:D55)</f>
+        <v>1.2069456032276571</v>
+      </c>
+      <c r="E47" s="368">
+        <f t="shared" si="5"/>
+        <v>13.621340154463082</v>
+      </c>
+      <c r="F47" s="368">
+        <f t="shared" si="5"/>
+        <v>1.371468842771582</v>
+      </c>
+      <c r="G47" s="368">
+        <f t="shared" si="5"/>
+        <v>4.6426544264576028</v>
+      </c>
+      <c r="H47" s="368">
+        <f t="shared" si="5"/>
+        <v>2.1837049529420849</v>
+      </c>
+      <c r="I47" s="368">
+        <f t="shared" si="5"/>
+        <v>4.33463407109216</v>
+      </c>
+      <c r="J47" s="368">
+        <f t="shared" si="5"/>
+        <v>2.1385807499842233</v>
+      </c>
+      <c r="K47" s="368">
+        <f t="shared" si="5"/>
+        <v>1.7071011492309554</v>
+      </c>
+      <c r="L47" s="368">
+        <f t="shared" si="5"/>
+        <v>8.5826167963290843</v>
+      </c>
+      <c r="M47" s="368">
+        <f t="shared" si="5"/>
+        <v>4.3504475179746827</v>
+      </c>
+      <c r="N47" s="368">
+        <f t="shared" si="5"/>
+        <v>2.6854614308485707</v>
+      </c>
+      <c r="O47" s="365"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" s="364" t="s">
+        <v>390</v>
+      </c>
+      <c r="B48" s="359" t="str">
+        <f>A7</f>
+        <v>Hot lab</v>
+      </c>
+      <c r="C48" s="366">
+        <f>$E7/(C34^2)</f>
+        <v>3.4402186498238743E-2</v>
+      </c>
+      <c r="D48" s="366">
+        <f>$E7/(D34^2)</f>
+        <v>5.2112187831651585E-2</v>
+      </c>
+      <c r="E48" s="366">
+        <f>$E7/(E34^2)</f>
+        <v>9.4248082867945379E-2</v>
+      </c>
+      <c r="F48" s="366">
+        <f>$E7/(F34^2)</f>
+        <v>4.0941445088813054E-2</v>
+      </c>
+      <c r="G48" s="366">
+        <f>$E7/(G34^2)</f>
+        <v>0.13760874599295497</v>
+      </c>
+      <c r="H48" s="366">
+        <f>$E7/(H34^2)</f>
+        <v>6.8566295581264772E-2</v>
+      </c>
+      <c r="I48" s="366">
+        <f>$E7/(I34^2)</f>
+        <v>0.14983485386000389</v>
+      </c>
+      <c r="J48" s="366">
+        <f>$E7/(J34^2)</f>
+        <v>0.19815659422985513</v>
+      </c>
+      <c r="K48" s="366">
+        <f>$E7/(K34^2)</f>
+        <v>0.16376578035525222</v>
+      </c>
+      <c r="L48" s="366">
+        <f>$E7/(L34^2)</f>
+        <v>0.97855108261656876</v>
+      </c>
+      <c r="M48" s="366">
+        <f>$E7/(M34^2)</f>
+        <v>0.19815659422985513</v>
+      </c>
+      <c r="N48" s="366">
+        <f>$E7/(N34^2)</f>
+        <v>0.12231888532707112</v>
+      </c>
+      <c r="O48" s="357"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" s="364"/>
+      <c r="B49" s="359" t="str">
+        <f>A8</f>
+        <v>NM Hold 1</v>
+      </c>
+      <c r="C49" s="366">
+        <f>$E8/(C35^2)</f>
+        <v>0.10422437566330317</v>
+      </c>
+      <c r="D49" s="366">
+        <f>$E8/(D35^2)</f>
+        <v>5.8626211310608044E-2</v>
+      </c>
+      <c r="E49" s="366">
+        <f>$E8/(E35^2)</f>
+        <v>4.7947153235201254E-2</v>
+      </c>
+      <c r="F49" s="366">
+        <f>$E8/(F35^2)</f>
+        <v>2.8949100690994177E-2</v>
+      </c>
+      <c r="G49" s="366">
+        <f>$E8/(G35^2)</f>
+        <v>5.0550151589248762E-2</v>
+      </c>
+      <c r="H49" s="366">
+        <f>$E8/(H35^2)</f>
+        <v>3.7520775238789147E-2</v>
+      </c>
+      <c r="I49" s="366">
+        <f>$E8/(I35^2)</f>
+        <v>7.4917426930001946E-2</v>
+      </c>
+      <c r="J49" s="366">
+        <f>$E8/(J35^2)</f>
+        <v>0.1097820466647397</v>
+      </c>
+      <c r="K49" s="366">
+        <f>$E8/(K35^2)</f>
+        <v>0.20220060635699505</v>
+      </c>
+      <c r="L49" s="366">
+        <f>$E8/(L35^2)</f>
+        <v>9.9078297114927563E-2</v>
+      </c>
+      <c r="M49" s="366">
+        <f>$E8/(M35^2)</f>
+        <v>0.39631318845971025</v>
+      </c>
+      <c r="N49" s="366">
+        <f>$E8/(N35^2)</f>
+        <v>0.24463777065414224</v>
+      </c>
+      <c r="O49" s="357"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" s="364"/>
+      <c r="B50" s="359" t="str">
+        <f>A9</f>
+        <v>NM Hold 2</v>
+      </c>
+      <c r="C50" s="366">
+        <f>$E9/(C36^2)</f>
+        <v>8.5735681657049284E-2</v>
+      </c>
+      <c r="D50" s="366">
+        <f>$E9/(D36^2)</f>
+        <v>9.9078297114927563E-2</v>
+      </c>
+      <c r="E50" s="366">
+        <f>$E9/(E36^2)</f>
+        <v>0.12231888532707109</v>
+      </c>
+      <c r="F50" s="366">
+        <f>$E9/(F36^2)</f>
+        <v>5.8626211310608044E-2</v>
+      </c>
+      <c r="G50" s="366">
+        <f>$E9/(G36^2)</f>
+        <v>0.15480983924207437</v>
+      </c>
+      <c r="H50" s="366">
+        <f>$E9/(H36^2)</f>
+        <v>8.5735681657049284E-2</v>
+      </c>
+      <c r="I50" s="366">
+        <f>$E9/(I36^2)</f>
+        <v>0.20220060635699505</v>
+      </c>
+      <c r="J50" s="366">
+        <f>$E9/(J36^2)</f>
+        <v>0.32753156071050443</v>
+      </c>
+      <c r="K50" s="366">
+        <f>$E9/(K36^2)</f>
+        <v>0.39631318845971025</v>
+      </c>
+      <c r="L50" s="366">
+        <f>$E9/(L36^2)</f>
+        <v>0.54853036465011817</v>
+      </c>
+      <c r="M50" s="366">
+        <f>$E9/(M36^2)</f>
+        <v>0.39631318845971025</v>
+      </c>
+      <c r="N50" s="366">
+        <f>$E9/(N36^2)</f>
+        <v>0.24463777065414224</v>
+      </c>
+      <c r="O50" s="357"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" s="364"/>
+      <c r="B51" s="359" t="str">
+        <f>A10</f>
+        <v>NM Camera 1</v>
+      </c>
+      <c r="C51" s="366">
+        <f>$E10/(C37^2)</f>
+        <v>0.29523657258722019</v>
+      </c>
+      <c r="D51" s="366">
+        <f>$E10/(D37^2)</f>
+        <v>7.6852502235323875E-2</v>
+      </c>
+      <c r="E51" s="366">
+        <f>$E10/(E37^2)</f>
+        <v>4.6491019870751472E-2</v>
+      </c>
+      <c r="F51" s="366">
+        <f>$E10/(F37^2)</f>
+        <v>2.8831696541720721E-2</v>
+      </c>
+      <c r="G51" s="366">
+        <f>$E10/(G37^2)</f>
+        <v>4.3674049199292936E-2</v>
+      </c>
+      <c r="H51" s="366">
+        <f>$E10/(H37^2)</f>
+        <v>3.1946478162571443E-2</v>
+      </c>
+      <c r="I51" s="366">
+        <f>$E10/(I37^2)</f>
+        <v>4.8002824627214523E-2</v>
+      </c>
+      <c r="J51" s="366">
+        <f>$E10/(J37^2)</f>
+        <v>6.0999291856863688E-2</v>
+      </c>
+      <c r="K51" s="366">
+        <f>$E10/(K37^2)</f>
+        <v>8.7203619029779134E-2</v>
+      </c>
+      <c r="L51" s="366">
+        <f>$E10/(L37^2)</f>
+        <v>7.3809143146805048E-2</v>
+      </c>
+      <c r="M51" s="366">
+        <f>$E10/(M37^2)</f>
+        <v>0.46130714466753153</v>
+      </c>
+      <c r="N51" s="366">
+        <f>$E10/(N37^2)</f>
+        <v>0.28475749670835293</v>
+      </c>
+      <c r="O51" s="357"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" s="364"/>
+      <c r="B52" s="359" t="str">
+        <f>A11</f>
+        <v>NM Camera 2</v>
+      </c>
+      <c r="C52" s="366">
+        <f>$E11/(C38^2)</f>
+        <v>0.17469619679717174</v>
+      </c>
+      <c r="D52" s="366">
+        <f>$E11/(D38^2)</f>
+        <v>0.34881447611911653</v>
+      </c>
+      <c r="E52" s="366">
+        <f>$E11/(E38^2)</f>
+        <v>0.23536078809567937</v>
+      </c>
+      <c r="F52" s="366">
+        <f>$E11/(F38^2)</f>
+        <v>9.1122398946672914E-2</v>
+      </c>
+      <c r="G52" s="366">
+        <f>$E11/(G38^2)</f>
+        <v>0.19201129850885809</v>
+      </c>
+      <c r="H52" s="366">
+        <f>$E11/(H38^2)</f>
+        <v>0.10460479470919085</v>
+      </c>
+      <c r="I52" s="366">
+        <f>$E11/(I38^2)</f>
+        <v>0.12131680333136924</v>
+      </c>
+      <c r="J52" s="366">
+        <f>$E11/(J38^2)</f>
+        <v>0.13478660180205451</v>
+      </c>
+      <c r="K52" s="366">
+        <f>$E11/(K38^2)</f>
+        <v>0.13478660180205451</v>
+      </c>
+      <c r="L52" s="366">
+        <f>$E11/(L38^2)</f>
+        <v>0.63848739746371164</v>
+      </c>
+      <c r="M52" s="366">
+        <f>$E11/(M38^2)</f>
+        <v>0.46130714466753153</v>
+      </c>
+      <c r="N52" s="366">
+        <f>$E11/(N38^2)</f>
+        <v>0.28475749670835293</v>
+      </c>
+      <c r="O52" s="357"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" s="364"/>
+      <c r="B53" s="359" t="str">
+        <f>A12</f>
+        <v>Stress Lab</v>
+      </c>
+      <c r="C53" s="366">
+        <f>$E12/(C39^2)</f>
+        <v>0.12189563658891514</v>
+      </c>
+      <c r="D53" s="366">
+        <f>$E12/(D39^2)</f>
+        <v>0.4044012127139901</v>
+      </c>
+      <c r="E53" s="366">
+        <f>$E12/(E39^2)</f>
+        <v>12.682022030710728</v>
+      </c>
+      <c r="F53" s="366">
+        <f>$E12/(F39^2)</f>
+        <v>0.79262637691942051</v>
+      </c>
+      <c r="G53" s="366">
+        <f>$E12/(G39^2)</f>
+        <v>3.170505507677682</v>
+      </c>
+      <c r="H53" s="366">
+        <f>$E12/(H39^2)</f>
+        <v>1.0970607293002363</v>
+      </c>
+      <c r="I53" s="366">
+        <f>$E12/(I39^2)</f>
+        <v>0.2588167761369537</v>
+      </c>
+      <c r="J53" s="366">
+        <f>$E12/(J39^2)</f>
+        <v>0.2195640933294794</v>
+      </c>
+      <c r="K53" s="366">
+        <f>$E12/(K39^2)</f>
+        <v>0.17147136331409857</v>
+      </c>
+      <c r="L53" s="366">
+        <f>$E12/(L39^2)</f>
+        <v>4.9539148557463797</v>
+      </c>
+      <c r="M53" s="366">
+        <f>$E12/(M39^2)</f>
+        <v>0.79262637691942051</v>
+      </c>
+      <c r="N53" s="366">
+        <f>$E12/(N39^2)</f>
+        <v>0.48927554130828449</v>
+      </c>
+      <c r="O53" s="357"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" s="364"/>
+      <c r="B54" s="359" t="str">
+        <f>A13</f>
+        <v>Hot Toilet</v>
+      </c>
+      <c r="C54" s="366">
+        <f>$E13/(C40^2)</f>
+        <v>9.6855613535542187E-2</v>
+      </c>
+      <c r="D54" s="366">
+        <f>$E13/(D40^2)</f>
+        <v>4.2355433494601046E-2</v>
+      </c>
+      <c r="E54" s="366">
+        <f>$E13/(E40^2)</f>
+        <v>3.1407076842833032E-2</v>
+      </c>
+      <c r="F54" s="366">
+        <f>$E13/(F40^2)</f>
+        <v>2.1024572101400626E-2</v>
+      </c>
+      <c r="G54" s="366">
+        <f>$E13/(G40^2)</f>
+        <v>3.4197497658736913E-2</v>
+      </c>
+      <c r="H54" s="366">
+        <f>$E13/(H40^2)</f>
+        <v>2.6087852323865793E-2</v>
+      </c>
+      <c r="I54" s="366">
+        <f>$E13/(I40^2)</f>
+        <v>4.2355433494601046E-2</v>
+      </c>
+      <c r="J54" s="366">
+        <f>$E13/(J40^2)</f>
+        <v>6.5125714541298563E-2</v>
+      </c>
+      <c r="K54" s="366">
+        <f>$E13/(K40^2)</f>
+        <v>9.6855613535542187E-2</v>
+      </c>
+      <c r="L54" s="366">
+        <f>$E13/(L40^2)</f>
+        <v>5.2857490902766473E-2</v>
+      </c>
+      <c r="M54" s="366">
+        <f>$E13/(M40^2)</f>
+        <v>0.40703571588311599</v>
+      </c>
+      <c r="N54" s="366">
+        <f>$E13/(N40^2)</f>
+        <v>0.25125661474266431</v>
+      </c>
+      <c r="O54" s="357"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" s="364"/>
+      <c r="B55" s="359" t="str">
+        <f>A14</f>
+        <v>Radiology Waiting</v>
+      </c>
+      <c r="C55" s="366">
+        <f>$E14/(C41^2)</f>
+        <v>7.7336760292987958E-2</v>
+      </c>
+      <c r="D55" s="366">
+        <f>$E14/(D41^2)</f>
+        <v>0.12470528240743838</v>
+      </c>
+      <c r="E55" s="366">
+        <f>$E14/(E41^2)</f>
+        <v>0.36154511751287288</v>
+      </c>
+      <c r="F55" s="366">
+        <f>$E14/(F41^2)</f>
+        <v>0.30934704117195183</v>
+      </c>
+      <c r="G55" s="366">
+        <f>$E14/(G41^2)</f>
+        <v>0.85929733658875518</v>
+      </c>
+      <c r="H55" s="366">
+        <f>$E14/(H41^2)</f>
+        <v>0.73218234596911691</v>
+      </c>
+      <c r="I55" s="366">
+        <f>$E14/(I41^2)</f>
+        <v>3.4371893463550207</v>
+      </c>
+      <c r="J55" s="366">
+        <f>$E14/(J41^2)</f>
+        <v>1.0226348468494277</v>
+      </c>
+      <c r="K55" s="366">
+        <f>$E14/(K41^2)</f>
+        <v>0.45450437637752344</v>
+      </c>
+      <c r="L55" s="366">
+        <f>$E14/(L41^2)</f>
+        <v>1.2373881646878073</v>
+      </c>
+      <c r="M55" s="366">
+        <f>$E14/(M41^2)</f>
+        <v>1.2373881646878073</v>
+      </c>
+      <c r="N55" s="366">
+        <f>$E14/(N41^2)</f>
+        <v>0.76381985474556047</v>
+      </c>
+      <c r="O55" s="357"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57" s="351" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B58" s="364" t="s">
+        <v>389</v>
+      </c>
+      <c r="C58" s="364"/>
+      <c r="D58" s="364"/>
+      <c r="E58" s="364"/>
+      <c r="F58" s="364"/>
+      <c r="G58" s="364"/>
+      <c r="H58" s="364"/>
+      <c r="I58" s="364"/>
+      <c r="J58" s="364"/>
+      <c r="K58" s="364"/>
+      <c r="L58" s="364"/>
+      <c r="M58" s="364"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59" s="359" t="s">
+        <v>365</v>
+      </c>
+      <c r="B59" s="360" t="str">
+        <f>C33</f>
+        <v>Tech area</v>
+      </c>
+      <c r="C59" s="360" t="str">
+        <f>D33</f>
+        <v>CT Tech area</v>
+      </c>
+      <c r="D59" s="360" t="str">
+        <f>E33</f>
+        <v>US 1</v>
+      </c>
+      <c r="E59" s="360" t="str">
+        <f>F33</f>
+        <v>US 2</v>
+      </c>
+      <c r="F59" s="360" t="str">
+        <f>G33</f>
+        <v>Office 2221</v>
+      </c>
+      <c r="G59" s="360" t="str">
+        <f>H33</f>
+        <v>Office 2302</v>
+      </c>
+      <c r="H59" s="360" t="str">
+        <f>I33</f>
+        <v>Consult A</v>
+      </c>
+      <c r="I59" s="360" t="str">
+        <f>J33</f>
+        <v>Consult B</v>
+      </c>
+      <c r="J59" s="360" t="str">
+        <f>K33</f>
+        <v>Lactation</v>
+      </c>
+      <c r="K59" s="360" t="str">
+        <f>L33</f>
+        <v>Reading Room</v>
+      </c>
+      <c r="L59" s="360" t="str">
+        <f>M33</f>
+        <v>Floor</v>
+      </c>
+      <c r="M59" s="360" t="str">
+        <f>N33</f>
+        <v>Ceiling</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A60" s="359" t="s">
+        <v>385</v>
+      </c>
+      <c r="B60" s="366">
+        <f>C47</f>
+        <v>0.9903830236204284</v>
+      </c>
+      <c r="C60" s="366">
+        <f>D47</f>
+        <v>1.2069456032276571</v>
+      </c>
+      <c r="D60" s="366">
+        <f>E47</f>
+        <v>13.621340154463082</v>
+      </c>
+      <c r="E60" s="366">
+        <f>F47</f>
+        <v>1.371468842771582</v>
+      </c>
+      <c r="F60" s="366">
+        <f>G47</f>
+        <v>4.6426544264576028</v>
+      </c>
+      <c r="G60" s="366">
+        <f>H47</f>
+        <v>2.1837049529420849</v>
+      </c>
+      <c r="H60" s="366">
+        <f>I47</f>
+        <v>4.33463407109216</v>
+      </c>
+      <c r="I60" s="366">
+        <f>J47</f>
+        <v>2.1385807499842233</v>
+      </c>
+      <c r="J60" s="366">
+        <f>K47</f>
+        <v>1.7071011492309554</v>
+      </c>
+      <c r="K60" s="366">
+        <f>L47</f>
+        <v>8.5826167963290843</v>
+      </c>
+      <c r="L60" s="366">
+        <f>M47</f>
+        <v>4.3504475179746827</v>
+      </c>
+      <c r="M60" s="366">
+        <f>N47</f>
+        <v>2.6854614308485707</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61" s="359" t="s">
+        <v>367</v>
+      </c>
+      <c r="B61" s="360">
+        <f>F18</f>
+        <v>0.02</v>
+      </c>
+      <c r="C61" s="360">
+        <f>F19</f>
+        <v>0.1</v>
+      </c>
+      <c r="D61" s="360">
+        <f>F20</f>
+        <v>0.04</v>
+      </c>
+      <c r="E61" s="360">
+        <f>F21</f>
+        <v>0.04</v>
+      </c>
+      <c r="F61" s="360">
+        <f>F22</f>
+        <v>0.04</v>
+      </c>
+      <c r="G61" s="360">
+        <f>F23</f>
+        <v>0.04</v>
+      </c>
+      <c r="H61" s="360">
+        <f>F24</f>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="I61" s="360">
+        <f>F25</f>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="J61" s="360">
+        <f>F26</f>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="K61" s="360">
+        <f>F27</f>
+        <v>0.1</v>
+      </c>
+      <c r="L61" s="360">
+        <f>F28</f>
+        <v>0.04</v>
+      </c>
+      <c r="M61" s="360">
+        <f>F29</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" s="359" t="s">
+        <v>386</v>
+      </c>
+      <c r="B62" s="366">
+        <f>B61/B60</f>
+        <v>2.0194207213779087E-2</v>
+      </c>
+      <c r="C62" s="366">
+        <f t="shared" ref="C62:M62" si="6">C61/C60</f>
+        <v>8.2853775458128706E-2</v>
+      </c>
+      <c r="D62" s="366">
+        <f t="shared" si="6"/>
+        <v>2.9365686155993875E-3</v>
+      </c>
+      <c r="E62" s="366">
+        <f t="shared" si="6"/>
+        <v>2.9165810226621385E-2</v>
+      </c>
+      <c r="F62" s="366">
+        <f t="shared" si="6"/>
+        <v>8.6157607966786467E-3</v>
+      </c>
+      <c r="G62" s="366">
+        <f t="shared" si="6"/>
+        <v>1.8317492913183339E-2</v>
+      </c>
+      <c r="H62" s="366">
+        <f t="shared" si="6"/>
+        <v>4.613999629952794E-2</v>
+      </c>
+      <c r="I62" s="366">
+        <f t="shared" si="6"/>
+        <v>9.3519966455077944E-2</v>
+      </c>
+      <c r="J62" s="366">
+        <f t="shared" si="6"/>
+        <v>0.11715767404298184</v>
+      </c>
+      <c r="K62" s="366">
+        <f t="shared" si="6"/>
+        <v>1.1651458101073734E-2</v>
+      </c>
+      <c r="L62" s="366">
+        <f t="shared" si="6"/>
+        <v>9.194456394366916E-3</v>
+      </c>
+      <c r="M62" s="366">
+        <f t="shared" si="6"/>
+        <v>1.4895019358874398E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" s="359" t="s">
+        <v>387</v>
+      </c>
+      <c r="B63" s="366">
+        <f>-LN(B62)/LN(2)</f>
+        <v>5.6299146800892492</v>
+      </c>
+      <c r="C63" s="366">
+        <f t="shared" ref="C63:M63" si="7">-LN(C62)/LN(2)</f>
+        <v>3.5932887504979729</v>
+      </c>
+      <c r="D63" s="366">
+        <f t="shared" si="7"/>
+        <v>8.4116529365497357</v>
+      </c>
+      <c r="E63" s="366">
+        <f t="shared" si="7"/>
+        <v>5.0995780369776718</v>
+      </c>
+      <c r="F63" s="366">
+        <f t="shared" si="7"/>
+        <v>6.8588060884285262</v>
+      </c>
+      <c r="G63" s="366">
+        <f t="shared" si="7"/>
+        <v>5.7706341322585439</v>
+      </c>
+      <c r="H63" s="366">
+        <f t="shared" si="7"/>
+        <v>4.4378383014593537</v>
+      </c>
+      <c r="I63" s="366">
+        <f t="shared" si="7"/>
+        <v>3.4185817773891309</v>
+      </c>
+      <c r="J63" s="366">
+        <f t="shared" si="7"/>
+        <v>3.093476638414439</v>
+      </c>
+      <c r="K63" s="366">
+        <f t="shared" si="7"/>
+        <v>6.4233456800833784</v>
+      </c>
+      <c r="L63" s="366">
+        <f t="shared" si="7"/>
+        <v>6.7650200042428716</v>
+      </c>
+      <c r="M63" s="366">
+        <f t="shared" si="7"/>
+        <v>6.0690261911329726</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" s="359" t="s">
+        <v>388</v>
+      </c>
+      <c r="B64" s="362">
+        <f>B63*PBHVL</f>
+        <v>1.5193086603894512</v>
+      </c>
+      <c r="C64" s="362">
+        <f>C63*PBHVL</f>
+        <v>0.96969759368094288</v>
+      </c>
+      <c r="D64" s="362">
+        <f>D63*PBHVL</f>
+        <v>2.2699983713585827</v>
+      </c>
+      <c r="E64" s="362">
+        <f>E63*PBHVL</f>
+        <v>1.376190140733925</v>
+      </c>
+      <c r="F64" s="362">
+        <f>F63*PBHVL</f>
+        <v>1.8509416362800299</v>
+      </c>
+      <c r="G64" s="362">
+        <f>G63*PBHVL</f>
+        <v>1.5572837087720102</v>
+      </c>
+      <c r="H64" s="362">
+        <f>H63*PBHVL</f>
+        <v>1.1976107184466822</v>
+      </c>
+      <c r="I64" s="362">
+        <f>I63*PBHVL</f>
+        <v>0.92255055285394361</v>
+      </c>
+      <c r="J64" s="362">
+        <f>J63*PBHVL</f>
+        <v>0.83481653178108151</v>
+      </c>
+      <c r="K64" s="362">
+        <f>K63*PBHVL</f>
+        <v>1.7334267524407918</v>
+      </c>
+      <c r="L64" s="362">
+        <f>L63*PBHVL</f>
+        <v>1.8256321923498742</v>
+      </c>
+      <c r="M64" s="362">
+        <f>M63*PBHVL</f>
+        <v>1.6378088436985971</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A66" s="349" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C67" s="364" t="s">
+        <v>389</v>
+      </c>
+      <c r="D67" s="364"/>
+      <c r="E67" s="364"/>
+      <c r="F67" s="364"/>
+      <c r="G67" s="364"/>
+      <c r="H67" s="364"/>
+      <c r="I67" s="364"/>
+      <c r="J67" s="364"/>
+      <c r="K67" s="364"/>
+      <c r="L67" s="364"/>
+      <c r="M67" s="364"/>
+      <c r="N67" s="364"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C68" s="360" t="str">
+        <f>C33</f>
+        <v>Tech area</v>
+      </c>
+      <c r="D68" s="360" t="str">
+        <f>D33</f>
+        <v>CT Tech area</v>
+      </c>
+      <c r="E68" s="360" t="str">
+        <f>E33</f>
+        <v>US 1</v>
+      </c>
+      <c r="F68" s="360" t="str">
+        <f>F33</f>
+        <v>US 2</v>
+      </c>
+      <c r="G68" s="360" t="str">
+        <f>G33</f>
+        <v>Office 2221</v>
+      </c>
+      <c r="H68" s="360" t="str">
+        <f>H33</f>
+        <v>Office 2302</v>
+      </c>
+      <c r="I68" s="360" t="str">
+        <f>I33</f>
+        <v>Consult A</v>
+      </c>
+      <c r="J68" s="360" t="str">
+        <f>J33</f>
+        <v>Consult B</v>
+      </c>
+      <c r="K68" s="360" t="str">
+        <f>K33</f>
+        <v>Lactation</v>
+      </c>
+      <c r="L68" s="360" t="str">
+        <f>L33</f>
+        <v>Reading Room</v>
+      </c>
+      <c r="M68" s="360" t="str">
+        <f>M33</f>
+        <v>Floor</v>
+      </c>
+      <c r="N68" s="360" t="str">
+        <f>N33</f>
+        <v>Ceiling</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A69" s="369" t="s">
+        <v>390</v>
+      </c>
+      <c r="B69" s="359" t="str">
+        <f>A7</f>
+        <v>Hot lab</v>
+      </c>
+      <c r="C69" s="362">
+        <f>-LN((B$61/C48))/LN(2)*PBHVL</f>
+        <v>0.2111682842584843</v>
+      </c>
+      <c r="D69" s="362">
+        <f>-LN((C$61/D48))/LN(2)*PBHVL</f>
+        <v>-0.25375464104747575</v>
+      </c>
+      <c r="E69" s="362">
+        <f>-LN((D$61/E48))/LN(2)*PBHVL</f>
+        <v>0.33367634585173811</v>
+      </c>
+      <c r="F69" s="362">
+        <f>-LN((E$61/F48))/LN(2)*PBHVL</f>
+        <v>9.0571666920018813E-3</v>
+      </c>
+      <c r="G69" s="362">
+        <f>-LN((F$61/G48))/LN(2)*PBHVL</f>
+        <v>0.4810318162517197</v>
+      </c>
+      <c r="H69" s="362">
+        <f>-LN((G$61/H48))/LN(2)*PBHVL</f>
+        <v>0.20981878280570193</v>
+      </c>
+      <c r="I69" s="362">
+        <f>-LN((H$61/I48))/LN(2)*PBHVL</f>
+        <v>-0.11243236477016001</v>
+      </c>
+      <c r="J69" s="362">
+        <f>-LN((I$61/J48))/LN(2)*PBHVL</f>
+        <v>-3.6051128808088388E-3</v>
+      </c>
+      <c r="K69" s="362">
+        <f>-LN((J$61/K48))/LN(2)*PBHVL</f>
+        <v>-7.781948604215512E-2</v>
+      </c>
+      <c r="L69" s="362">
+        <f>-LN((K$61/L48))/LN(2)*PBHVL</f>
+        <v>0.88802566644085579</v>
+      </c>
+      <c r="M69" s="362">
+        <f>-LN((L$61/M48))/LN(2)*PBHVL</f>
+        <v>0.62299860383981909</v>
+      </c>
+      <c r="N69" s="362">
+        <f>-LN((M$61/N48))/LN(2)*PBHVL</f>
+        <v>0.43517525518854178</v>
+      </c>
+      <c r="O69" s="356"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A70" s="370"/>
+      <c r="B70" s="359" t="str">
+        <f>A8</f>
+        <v>NM Hold 1</v>
+      </c>
+      <c r="C70" s="362">
+        <f>-LN((B$61/C49))/LN(2)*PBHVL</f>
+        <v>0.64271260766638783</v>
+      </c>
+      <c r="D70" s="362">
+        <f>-LN((C$61/D49))/LN(2)*PBHVL</f>
+        <v>-0.20789807998429763</v>
+      </c>
+      <c r="E70" s="362">
+        <f>-LN((D$61/E49))/LN(2)*PBHVL</f>
+        <v>7.055451448891846E-2</v>
+      </c>
+      <c r="F70" s="362">
+        <f>-LN((E$61/F49))/LN(2)*PBHVL</f>
+        <v>-0.12588633674457109</v>
+      </c>
+      <c r="G70" s="362">
+        <f>-LN((F$61/G49))/LN(2)*PBHVL</f>
+        <v>9.1137075637720985E-2</v>
+      </c>
+      <c r="H70" s="362">
+        <f>-LN((G$61/H49))/LN(2)*PBHVL</f>
+        <v>-2.4911200725219192E-2</v>
+      </c>
+      <c r="I70" s="362">
+        <f>-LN((H$61/I49))/LN(2)*PBHVL</f>
+        <v>-0.38229589676339548</v>
+      </c>
+      <c r="J70" s="362">
+        <f>-LN((I$61/J49))/LN(2)*PBHVL</f>
+        <v>-0.23352852831810289</v>
+      </c>
+      <c r="K70" s="362">
+        <f>-LN((J$61/K49))/LN(2)*PBHVL</f>
+        <v>4.2604229035640177E-3</v>
+      </c>
+      <c r="L70" s="362">
+        <f>-LN((K$61/L49))/LN(2)*PBHVL</f>
+        <v>-3.6051128808089242E-3</v>
+      </c>
+      <c r="M70" s="362">
+        <f>-LN((L$61/M49))/LN(2)*PBHVL</f>
+        <v>0.89286213583305474</v>
+      </c>
+      <c r="N70" s="362">
+        <f>-LN((M$61/N49))/LN(2)*PBHVL</f>
+        <v>0.70503878718177726</v>
+      </c>
+      <c r="O70" s="356"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A71" s="370"/>
+      <c r="B71" s="359" t="str">
+        <f>A9</f>
+        <v>NM Hold 2</v>
+      </c>
+      <c r="C71" s="362">
+        <f>-LN((B$61/C50))/LN(2)*PBHVL</f>
+        <v>0.56668528477185676</v>
+      </c>
+      <c r="D71" s="362">
+        <f>-LN((C$61/D50))/LN(2)*PBHVL</f>
+        <v>-3.6051128808089242E-3</v>
+      </c>
+      <c r="E71" s="362">
+        <f>-LN((D$61/E50))/LN(2)*PBHVL</f>
+        <v>0.43517525518854172</v>
+      </c>
+      <c r="F71" s="362">
+        <f>-LN((E$61/F50))/LN(2)*PBHVL</f>
+        <v>0.14884210474309492</v>
+      </c>
+      <c r="G71" s="362">
+        <f>-LN((F$61/G50))/LN(2)*PBHVL</f>
+        <v>0.52688837731489779</v>
+      </c>
+      <c r="H71" s="362">
+        <f>-LN((G$61/H50))/LN(2)*PBHVL</f>
+        <v>0.29682175277862122</v>
+      </c>
+      <c r="I71" s="362">
+        <f>-LN((H$61/I50))/LN(2)*PBHVL</f>
+        <v>4.2604229035640177E-3</v>
+      </c>
+      <c r="J71" s="362">
+        <f>-LN((I$61/J50))/LN(2)*PBHVL</f>
+        <v>0.19204404595108038</v>
+      </c>
+      <c r="K71" s="362">
+        <f>-LN((J$61/K50))/LN(2)*PBHVL</f>
+        <v>0.26625841911242665</v>
+      </c>
+      <c r="L71" s="362">
+        <f>-LN((K$61/L50))/LN(2)*PBHVL</f>
+        <v>0.66266919405801594</v>
+      </c>
+      <c r="M71" s="362">
+        <f>-LN((L$61/M50))/LN(2)*PBHVL</f>
+        <v>0.89286213583305474</v>
+      </c>
+      <c r="N71" s="362">
+        <f>-LN((M$61/N50))/LN(2)*PBHVL</f>
+        <v>0.70503878718177726</v>
+      </c>
+      <c r="O71" s="356"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A72" s="370"/>
+      <c r="B72" s="359" t="str">
+        <f>A10</f>
+        <v>NM Camera 1</v>
+      </c>
+      <c r="C72" s="362">
+        <f>-LN((B$61/C51))/LN(2)*PBHVL</f>
+        <v>1.0480958619497696</v>
+      </c>
+      <c r="D72" s="362">
+        <f>-LN((C$61/D51))/LN(2)*PBHVL</f>
+        <v>-0.10250384718858385</v>
+      </c>
+      <c r="E72" s="362">
+        <f>-LN((D$61/E51))/LN(2)*PBHVL</f>
+        <v>5.8547453103158328E-2</v>
+      </c>
+      <c r="F72" s="362">
+        <f>-LN((E$61/F51))/LN(2)*PBHVL</f>
+        <v>-0.12746849254809384</v>
+      </c>
+      <c r="G72" s="362">
+        <f>-LN((F$61/G51))/LN(2)*PBHVL</f>
+        <v>3.4212298866574294E-2</v>
+      </c>
+      <c r="H72" s="362">
+        <f>-LN((G$61/H51))/LN(2)*PBHVL</f>
+        <v>-8.7528375992152352E-2</v>
+      </c>
+      <c r="I72" s="362">
+        <f>-LN((H$61/I51))/LN(2)*PBHVL</f>
+        <v>-0.55559741288576814</v>
+      </c>
+      <c r="J72" s="362">
+        <f>-LN((I$61/J51))/LN(2)*PBHVL</f>
+        <v>-0.4623128239119112</v>
+      </c>
+      <c r="K72" s="362">
+        <f>-LN((J$61/K51))/LN(2)*PBHVL</f>
+        <v>-0.32317239717160196</v>
+      </c>
+      <c r="L72" s="362">
+        <f>-LN((K$61/L51))/LN(2)*PBHVL</f>
+        <v>-0.11823491875732949</v>
+      </c>
+      <c r="M72" s="362">
+        <f>-LN((L$61/M51))/LN(2)*PBHVL</f>
+        <v>0.95198563542484815</v>
+      </c>
+      <c r="N72" s="362">
+        <f>-LN((M$61/N51))/LN(2)*PBHVL</f>
+        <v>0.76416228677357079</v>
+      </c>
+      <c r="O72" s="356"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A73" s="370"/>
+      <c r="B73" s="359" t="str">
+        <f>A11</f>
+        <v>NM Camera 2</v>
+      </c>
+      <c r="C73" s="362">
+        <f>-LN((B$61/C52))/LN(2)*PBHVL</f>
+        <v>0.84380289484628079</v>
+      </c>
+      <c r="D73" s="362">
+        <f>-LN((C$61/D52))/LN(2)*PBHVL</f>
+        <v>0.4864181988081045</v>
+      </c>
+      <c r="E73" s="362">
+        <f>-LN((D$61/E52))/LN(2)*PBHVL</f>
+        <v>0.68998763921598549</v>
+      </c>
+      <c r="F73" s="362">
+        <f>-LN((E$61/F52))/LN(2)*PBHVL</f>
+        <v>0.32054544931202117</v>
+      </c>
+      <c r="G73" s="362">
+        <f>-LN((F$61/G52))/LN(2)*PBHVL</f>
+        <v>0.61073336782133081</v>
+      </c>
+      <c r="H73" s="362">
+        <f>-LN((G$61/H52))/LN(2)*PBHVL</f>
+        <v>0.37426754615957197</v>
+      </c>
+      <c r="I73" s="362">
+        <f>-LN((H$61/I52))/LN(2)*PBHVL</f>
+        <v>-0.19463114145568225</v>
+      </c>
+      <c r="J73" s="362">
+        <f>-LN((I$61/J52))/LN(2)*PBHVL</f>
+        <v>-0.15363948988693457</v>
+      </c>
+      <c r="K73" s="362">
+        <f>-LN((J$61/K52))/LN(2)*PBHVL</f>
+        <v>-0.15363948988693457</v>
+      </c>
+      <c r="L73" s="362">
+        <f>-LN((K$61/L52))/LN(2)*PBHVL</f>
+        <v>0.72179269364980936</v>
+      </c>
+      <c r="M73" s="362">
+        <f>-LN((L$61/M52))/LN(2)*PBHVL</f>
+        <v>0.95198563542484815</v>
+      </c>
+      <c r="N73" s="362">
+        <f>-LN((M$61/N52))/LN(2)*PBHVL</f>
+        <v>0.76416228677357079</v>
+      </c>
+      <c r="O73" s="356"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A74" s="370"/>
+      <c r="B74" s="359" t="str">
+        <f>A12</f>
+        <v>Stress Lab</v>
+      </c>
+      <c r="C74" s="362">
+        <f>-LN((B$61/C53))/LN(2)*PBHVL</f>
+        <v>0.70368928572899481</v>
+      </c>
+      <c r="D74" s="362">
+        <f>-LN((C$61/D53))/LN(2)*PBHVL</f>
+        <v>0.54398748689003495</v>
+      </c>
+      <c r="E74" s="362">
+        <f>-LN((D$61/E53))/LN(2)*PBHVL</f>
+        <v>2.2421797957992324</v>
+      </c>
+      <c r="F74" s="362">
+        <f>-LN((E$61/F53))/LN(2)*PBHVL</f>
+        <v>1.1627256678262901</v>
+      </c>
+      <c r="G74" s="362">
+        <f>-LN((F$61/G53))/LN(2)*PBHVL</f>
+        <v>1.7024527318127611</v>
+      </c>
+      <c r="H74" s="362">
+        <f>-LN((G$61/H53))/LN(2)*PBHVL</f>
+        <v>1.2892729107786438</v>
+      </c>
+      <c r="I74" s="362">
+        <f>-LN((H$61/I53))/LN(2)*PBHVL</f>
+        <v>0.10037064942848542</v>
+      </c>
+      <c r="J74" s="362">
+        <f>-LN((I$61/J53))/LN(2)*PBHVL</f>
+        <v>3.63350036751326E-2</v>
+      </c>
+      <c r="K74" s="362">
+        <f>-LN((J$61/K53))/LN(2)*PBHVL</f>
+        <v>-5.9918431948771236E-2</v>
+      </c>
+      <c r="L74" s="362">
+        <f>-LN((K$61/L53))/LN(2)*PBHVL</f>
+        <v>1.5194658525536828</v>
+      </c>
+      <c r="M74" s="362">
+        <f>-LN((L$61/M53))/LN(2)*PBHVL</f>
+        <v>1.1627256678262901</v>
+      </c>
+      <c r="N74" s="362">
+        <f>-LN((M$61/N53))/LN(2)*PBHVL</f>
+        <v>0.9749023191750128</v>
+      </c>
+      <c r="O74" s="356"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A75" s="370"/>
+      <c r="B75" s="359" t="str">
+        <f>A13</f>
+        <v>Hot Toilet</v>
+      </c>
+      <c r="C75" s="362">
+        <f>-LN((B$61/C54))/LN(2)*PBHVL</f>
+        <v>0.61416505123607945</v>
+      </c>
+      <c r="D75" s="362">
+        <f>-LN((C$61/D54))/LN(2)*PBHVL</f>
+        <v>-0.33446374488138481</v>
+      </c>
+      <c r="E75" s="362">
+        <f>-LN((D$61/E54))/LN(2)*PBHVL</f>
+        <v>-9.415817319498769E-2</v>
+      </c>
+      <c r="F75" s="362">
+        <f>-LN((E$61/F54))/LN(2)*PBHVL</f>
+        <v>-0.25041272969829204</v>
+      </c>
+      <c r="G75" s="362">
+        <f>-LN((F$61/G54))/LN(2)*PBHVL</f>
+        <v>-6.1018637496239404E-2</v>
+      </c>
+      <c r="H75" s="362">
+        <f>-LN((G$61/H54))/LN(2)*PBHVL</f>
+        <v>-0.16640374237787289</v>
+      </c>
+      <c r="I75" s="362">
+        <f>-LN((H$61/I54))/LN(2)*PBHVL</f>
+        <v>-0.60432727687462018</v>
+      </c>
+      <c r="J75" s="362">
+        <f>-LN((I$61/J54))/LN(2)*PBHVL</f>
+        <v>-0.43682831473941691</v>
+      </c>
+      <c r="K75" s="362">
+        <f>-LN((J$61/K54))/LN(2)*PBHVL</f>
+        <v>-0.28230219747778407</v>
+      </c>
+      <c r="L75" s="362">
+        <f>-LN((K$61/L54))/LN(2)*PBHVL</f>
+        <v>-0.24822591493896465</v>
+      </c>
+      <c r="M75" s="362">
+        <f>-LN((L$61/M54))/LN(2)*PBHVL</f>
+        <v>0.90325577143599622</v>
+      </c>
+      <c r="N75" s="362">
+        <f>-LN((M$61/N54))/LN(2)*PBHVL</f>
+        <v>0.71543242278471875</v>
+      </c>
+      <c r="O75" s="356"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A76" s="371"/>
+      <c r="B76" s="359" t="str">
+        <f>A14</f>
+        <v>Radiology Waiting</v>
+      </c>
+      <c r="C76" s="362">
+        <f>-LN((B$61/C55))/LN(2)*PBHVL</f>
+        <v>0.52654539892616026</v>
+      </c>
+      <c r="D76" s="362">
+        <f>-LN((C$61/D55))/LN(2)*PBHVL</f>
+        <v>8.5957627856784416E-2</v>
+      </c>
+      <c r="E76" s="362">
+        <f>-LN((D$61/E55))/LN(2)*PBHVL</f>
+        <v>0.85711458631471205</v>
+      </c>
+      <c r="F76" s="362">
+        <f>-LN((E$61/F55))/LN(2)*PBHVL</f>
+        <v>0.7964089309193958</v>
+      </c>
+      <c r="G76" s="362">
+        <f>-LN((F$61/G55))/LN(2)*PBHVL</f>
+        <v>1.1941692073177674</v>
+      </c>
+      <c r="H76" s="362">
+        <f>-LN((G$61/H55))/LN(2)*PBHVL</f>
+        <v>1.1318430278023779</v>
+      </c>
+      <c r="I76" s="362">
+        <f>-LN((H$61/I55))/LN(2)*PBHVL</f>
+        <v>1.1072925545836103</v>
+      </c>
+      <c r="J76" s="362">
+        <f>-LN((I$61/J55))/LN(2)*PBHVL</f>
+        <v>0.63531790502389252</v>
+      </c>
+      <c r="K76" s="362">
+        <f>-LN((J$61/K55))/LN(2)*PBHVL</f>
+        <v>0.31959781196747894</v>
+      </c>
+      <c r="L76" s="362">
+        <f>-LN((K$61/L55))/LN(2)*PBHVL</f>
+        <v>0.97939581017847421</v>
+      </c>
+      <c r="M76" s="362">
+        <f>-LN((L$61/M55))/LN(2)*PBHVL</f>
+        <v>1.3361359949058669</v>
+      </c>
+      <c r="N76" s="362">
+        <f>-LN((M$61/N55))/LN(2)*PBHVL</f>
+        <v>1.1483126462545894</v>
+      </c>
+      <c r="O76" s="356"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="C67:N67"/>
+    <mergeCell ref="B58:M58"/>
+    <mergeCell ref="A69:A76"/>
+    <mergeCell ref="C32:N32"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A48:A55"/>
+    <mergeCell ref="C45:N45"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C48:C55">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48:D55">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48:E55">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F48:F55">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G48:G55">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H48:H55">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I48:I55">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J48:J55">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48:K55">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L48:L55">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C69:N76">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M48:N55">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="53" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -28598,11 +31877,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29897,7 +33176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF32"/>
   <sheetViews>
@@ -32992,7 +36271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -33070,7 +36349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
@@ -33977,7 +37256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -34220,66 +37499,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="292" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>196</v>
-      </c>
-      <c r="B4">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B5">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>241</v>
-      </c>
-      <c r="B6">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>242</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add tables from Kusano and Caldwell
</commit_message>
<xml_diff>
--- a/MUSCShield_form.xlsx
+++ b/MUSCShield_form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\workspace\EquipTestingSpreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maheug\Documents\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E528B03B-67FF-4B01-B5BB-8C1AE25C54F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BDB4AD-A29B-486F-85EC-8F75D95D887A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" firstSheet="13" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="NCRP147_C1" sheetId="15" r:id="rId16"/>
     <sheet name="W_Rh_Al_Ag" sheetId="16" r:id="rId17"/>
     <sheet name="TG108_PETCT" sheetId="18" r:id="rId18"/>
+    <sheet name="Kusano_Caldwell" sheetId="19" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="FitParams">FitParameters!$A$5:$AF$30</definedName>
@@ -46,7 +47,7 @@
     <definedName name="RefkV">ShieldEvaluation!$C$16</definedName>
     <definedName name="RefOutput">ShieldEvaluation!$H$16</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateCount="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -685,7 +686,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="375">
   <si>
     <t>Shielding Calculations</t>
   </si>
@@ -2204,6 +2205,54 @@
   <si>
     <t>Material</t>
   </si>
+  <si>
+    <t>Health Phys, 2014 Jul; 107(1):60-72</t>
+  </si>
+  <si>
+    <t>DOI: 10.1097/HP.0000000000000051</t>
+  </si>
+  <si>
+    <t>Table 3: Dose equivalent rate constants for soft tissue and TVL in lead and concrete</t>
+  </si>
+  <si>
+    <t>Dose equiv rate constant (uSv-m^2/GBq-h)</t>
+  </si>
+  <si>
+    <t>TVL Lead (mm)</t>
+  </si>
+  <si>
+    <t>TVL concrete (cm)</t>
+  </si>
+  <si>
+    <t>Ga-67</t>
+  </si>
+  <si>
+    <t>I-123</t>
+  </si>
+  <si>
+    <t>I-131</t>
+  </si>
+  <si>
+    <t>In-111</t>
+  </si>
+  <si>
+    <t>Tc-99m</t>
+  </si>
+  <si>
+    <t>Tl-201</t>
+  </si>
+  <si>
+    <t>Xe-133</t>
+  </si>
+  <si>
+    <t>Table 7: Archer fitting parameters for lead</t>
+  </si>
+  <si>
+    <t>Table 8: Archer fitting parameters for concrete</t>
+  </si>
+  <si>
+    <t>Dose equivalent rate constants and barrier transmission data for nuclear medicine facility dose calculations and shielding design</t>
+  </si>
 </sst>
 </file>
 
@@ -2224,7 +2273,7 @@
     <numFmt numFmtId="175" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="176" formatCode="#\ ???/???"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
@@ -2364,12 +2413,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2976,7 +3019,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="260">
+  <cellXfs count="264">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -3528,6 +3571,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3591,24 +3661,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3624,8 +3676,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -7719,12 +7774,12 @@
       <c r="I12" s="8"/>
       <c r="V12" s="33"/>
       <c r="W12" s="34"/>
-      <c r="X12" s="227" t="s">
+      <c r="X12" s="236" t="s">
         <v>34</v>
       </c>
-      <c r="Y12" s="227"/>
-      <c r="Z12" s="227"/>
-      <c r="AA12" s="227"/>
+      <c r="Y12" s="236"/>
+      <c r="Z12" s="236"/>
+      <c r="AA12" s="236"/>
       <c r="AB12" s="35"/>
       <c r="AD12" s="23"/>
       <c r="AE12" s="23">
@@ -7754,12 +7809,12 @@
       <c r="I13" s="8"/>
       <c r="V13" s="3"/>
       <c r="W13"/>
-      <c r="X13" s="228" t="s">
+      <c r="X13" s="237" t="s">
         <v>37</v>
       </c>
-      <c r="Y13" s="228"/>
-      <c r="Z13" s="228"/>
-      <c r="AA13" s="228"/>
+      <c r="Y13" s="237"/>
+      <c r="Z13" s="237"/>
+      <c r="AA13" s="237"/>
       <c r="AB13" s="37"/>
       <c r="AD13" s="23"/>
       <c r="AE13" s="23">
@@ -8390,12 +8445,12 @@
       <c r="AJ23" s="23"/>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="B24" s="229" t="s">
+      <c r="B24" s="238" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="229"/>
-      <c r="D24" s="229"/>
-      <c r="E24" s="229"/>
+      <c r="C24" s="238"/>
+      <c r="D24" s="238"/>
+      <c r="E24" s="238"/>
       <c r="I24" s="2" t="s">
         <v>62</v>
       </c>
@@ -9722,60 +9777,60 @@
       <c r="N42" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="O42" s="230" t="s">
+      <c r="O42" s="239" t="s">
         <v>90</v>
       </c>
-      <c r="P42" s="230"/>
-      <c r="Q42" s="230"/>
-      <c r="R42" s="230"/>
-      <c r="S42" s="230"/>
-      <c r="T42" s="230"/>
-      <c r="U42" s="230"/>
-      <c r="V42" s="230"/>
-      <c r="W42" s="230"/>
-      <c r="X42" s="230"/>
-      <c r="Y42" s="230"/>
-      <c r="Z42" s="230"/>
-      <c r="AA42" s="230"/>
-      <c r="AB42" s="230"/>
-      <c r="AC42" s="230"/>
-      <c r="AD42" s="230"/>
-      <c r="AE42" s="231" t="s">
+      <c r="P42" s="239"/>
+      <c r="Q42" s="239"/>
+      <c r="R42" s="239"/>
+      <c r="S42" s="239"/>
+      <c r="T42" s="239"/>
+      <c r="U42" s="239"/>
+      <c r="V42" s="239"/>
+      <c r="W42" s="239"/>
+      <c r="X42" s="239"/>
+      <c r="Y42" s="239"/>
+      <c r="Z42" s="239"/>
+      <c r="AA42" s="239"/>
+      <c r="AB42" s="239"/>
+      <c r="AC42" s="239"/>
+      <c r="AD42" s="239"/>
+      <c r="AE42" s="240" t="s">
         <v>90</v>
       </c>
-      <c r="AF42" s="231"/>
-      <c r="AG42" s="231"/>
-      <c r="AH42" s="231"/>
-      <c r="AI42" s="231"/>
-      <c r="AJ42" s="231"/>
-      <c r="AK42" s="231"/>
-      <c r="AL42" s="231"/>
-      <c r="AM42" s="231"/>
-      <c r="AN42" s="231"/>
-      <c r="AO42" s="231"/>
-      <c r="AP42" s="231"/>
-      <c r="AQ42" s="231"/>
-      <c r="AR42" s="231"/>
-      <c r="AS42" s="231"/>
-      <c r="AT42" s="231"/>
+      <c r="AF42" s="240"/>
+      <c r="AG42" s="240"/>
+      <c r="AH42" s="240"/>
+      <c r="AI42" s="240"/>
+      <c r="AJ42" s="240"/>
+      <c r="AK42" s="240"/>
+      <c r="AL42" s="240"/>
+      <c r="AM42" s="240"/>
+      <c r="AN42" s="240"/>
+      <c r="AO42" s="240"/>
+      <c r="AP42" s="240"/>
+      <c r="AQ42" s="240"/>
+      <c r="AR42" s="240"/>
+      <c r="AS42" s="240"/>
+      <c r="AT42" s="240"/>
     </row>
     <row r="43" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A43" s="13"/>
-      <c r="B43" s="232" t="s">
+      <c r="B43" s="241" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="232"/>
-      <c r="D43" s="232"/>
-      <c r="E43" s="233" t="s">
+      <c r="C43" s="241"/>
+      <c r="D43" s="241"/>
+      <c r="E43" s="242" t="s">
         <v>62</v>
       </c>
-      <c r="F43" s="233"/>
-      <c r="G43" s="233"/>
-      <c r="H43" s="232" t="s">
+      <c r="F43" s="242"/>
+      <c r="G43" s="242"/>
+      <c r="H43" s="241" t="s">
         <v>91</v>
       </c>
-      <c r="I43" s="232"/>
-      <c r="J43" s="232"/>
+      <c r="I43" s="241"/>
+      <c r="J43" s="241"/>
       <c r="K43" s="77" t="s">
         <v>92</v>
       </c>
@@ -9856,41 +9911,41 @@
         <v>94</v>
       </c>
       <c r="O44" s="3"/>
-      <c r="P44" s="234" t="s">
+      <c r="P44" s="243" t="s">
         <v>95</v>
       </c>
-      <c r="Q44" s="234"/>
-      <c r="R44" s="234"/>
+      <c r="Q44" s="243"/>
+      <c r="R44" s="243"/>
       <c r="S44"/>
       <c r="T44"/>
-      <c r="U44" s="234" t="s">
+      <c r="U44" s="243" t="s">
         <v>96</v>
       </c>
-      <c r="V44" s="234"/>
-      <c r="W44" s="234"/>
+      <c r="V44" s="243"/>
+      <c r="W44" s="243"/>
       <c r="X44"/>
       <c r="Y44"/>
-      <c r="Z44" s="234" t="s">
+      <c r="Z44" s="243" t="s">
         <v>53</v>
       </c>
-      <c r="AA44" s="234"/>
-      <c r="AB44" s="234"/>
+      <c r="AA44" s="243"/>
+      <c r="AB44" s="243"/>
       <c r="AC44"/>
-      <c r="AE44" s="232" t="s">
+      <c r="AE44" s="241" t="s">
         <v>55</v>
       </c>
-      <c r="AF44" s="232"/>
-      <c r="AG44" s="232"/>
-      <c r="AJ44" s="234" t="s">
+      <c r="AF44" s="241"/>
+      <c r="AG44" s="241"/>
+      <c r="AJ44" s="243" t="s">
         <v>97</v>
       </c>
-      <c r="AK44" s="234"/>
-      <c r="AL44" s="234"/>
-      <c r="AO44" s="234" t="s">
+      <c r="AK44" s="243"/>
+      <c r="AL44" s="243"/>
+      <c r="AO44" s="243" t="s">
         <v>59</v>
       </c>
-      <c r="AP44" s="234"/>
-      <c r="AQ44" s="234"/>
+      <c r="AP44" s="243"/>
+      <c r="AQ44" s="243"/>
       <c r="AT44" s="42"/>
     </row>
     <row r="45" spans="1:46" x14ac:dyDescent="0.2">
@@ -12406,21 +12461,21 @@
     </row>
     <row r="61" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A61" s="13"/>
-      <c r="B61" s="235" t="s">
+      <c r="B61" s="244" t="s">
         <v>60</v>
       </c>
-      <c r="C61" s="235"/>
-      <c r="D61" s="235"/>
-      <c r="E61" s="235" t="s">
+      <c r="C61" s="244"/>
+      <c r="D61" s="244"/>
+      <c r="E61" s="244" t="s">
         <v>62</v>
       </c>
-      <c r="F61" s="235"/>
-      <c r="G61" s="235"/>
-      <c r="H61" s="235" t="s">
+      <c r="F61" s="244"/>
+      <c r="G61" s="244"/>
+      <c r="H61" s="244" t="s">
         <v>91</v>
       </c>
-      <c r="I61" s="235"/>
-      <c r="J61" s="235"/>
+      <c r="I61" s="244"/>
+      <c r="J61" s="244"/>
       <c r="K61" s="93" t="s">
         <v>92</v>
       </c>
@@ -14519,21 +14574,21 @@
     </row>
     <row r="79" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A79" s="13"/>
-      <c r="B79" s="235" t="s">
+      <c r="B79" s="244" t="s">
         <v>60</v>
       </c>
-      <c r="C79" s="235"/>
-      <c r="D79" s="235"/>
-      <c r="E79" s="235" t="s">
+      <c r="C79" s="244"/>
+      <c r="D79" s="244"/>
+      <c r="E79" s="244" t="s">
         <v>62</v>
       </c>
-      <c r="F79" s="235"/>
-      <c r="G79" s="235"/>
-      <c r="H79" s="235" t="s">
+      <c r="F79" s="244"/>
+      <c r="G79" s="244"/>
+      <c r="H79" s="244" t="s">
         <v>91</v>
       </c>
-      <c r="I79" s="235"/>
-      <c r="J79" s="235"/>
+      <c r="I79" s="244"/>
+      <c r="J79" s="244"/>
       <c r="K79" s="93" t="s">
         <v>92</v>
       </c>
@@ -15443,21 +15498,21 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" s="13"/>
-      <c r="B97" s="235" t="s">
+      <c r="B97" s="244" t="s">
         <v>60</v>
       </c>
-      <c r="C97" s="235"/>
-      <c r="D97" s="235"/>
-      <c r="E97" s="235" t="s">
+      <c r="C97" s="244"/>
+      <c r="D97" s="244"/>
+      <c r="E97" s="244" t="s">
         <v>62</v>
       </c>
-      <c r="F97" s="235"/>
-      <c r="G97" s="235"/>
-      <c r="H97" s="235" t="s">
+      <c r="F97" s="244"/>
+      <c r="G97" s="244"/>
+      <c r="H97" s="244" t="s">
         <v>91</v>
       </c>
-      <c r="I97" s="235"/>
-      <c r="J97" s="235"/>
+      <c r="I97" s="244"/>
+      <c r="J97" s="244"/>
       <c r="K97" s="93" t="s">
         <v>92</v>
       </c>
@@ -16432,13 +16487,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E6" s="228" t="s">
+      <c r="E6" s="237" t="s">
         <v>278</v>
       </c>
-      <c r="F6" s="228"/>
-      <c r="G6" s="228"/>
-      <c r="H6" s="228"/>
-      <c r="I6" s="228"/>
+      <c r="F6" s="237"/>
+      <c r="G6" s="237"/>
+      <c r="H6" s="237"/>
+      <c r="I6" s="237"/>
     </row>
     <row r="7" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="222" t="s">
@@ -16889,48 +16944,48 @@
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="B4" s="228" t="s">
+      <c r="B4" s="237" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="228"/>
-      <c r="D4" s="228"/>
-      <c r="E4" s="228"/>
-      <c r="F4" s="228"/>
-      <c r="G4" s="228" t="s">
+      <c r="C4" s="237"/>
+      <c r="D4" s="237"/>
+      <c r="E4" s="237"/>
+      <c r="F4" s="237"/>
+      <c r="G4" s="237" t="s">
         <v>96</v>
       </c>
-      <c r="H4" s="228"/>
-      <c r="I4" s="228"/>
-      <c r="J4" s="228"/>
-      <c r="K4" s="228"/>
-      <c r="L4" s="228" t="s">
+      <c r="H4" s="237"/>
+      <c r="I4" s="237"/>
+      <c r="J4" s="237"/>
+      <c r="K4" s="237"/>
+      <c r="L4" s="237" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="228"/>
-      <c r="N4" s="228"/>
-      <c r="O4" s="228"/>
-      <c r="P4" s="228"/>
-      <c r="Q4" s="228" t="s">
+      <c r="M4" s="237"/>
+      <c r="N4" s="237"/>
+      <c r="O4" s="237"/>
+      <c r="P4" s="237"/>
+      <c r="Q4" s="237" t="s">
         <v>55</v>
       </c>
-      <c r="R4" s="228"/>
-      <c r="S4" s="228"/>
-      <c r="T4" s="228"/>
-      <c r="U4" s="228"/>
-      <c r="V4" s="228" t="s">
+      <c r="R4" s="237"/>
+      <c r="S4" s="237"/>
+      <c r="T4" s="237"/>
+      <c r="U4" s="237"/>
+      <c r="V4" s="237" t="s">
         <v>97</v>
       </c>
-      <c r="W4" s="228"/>
-      <c r="X4" s="228"/>
-      <c r="Y4" s="228"/>
-      <c r="Z4" s="228"/>
-      <c r="AA4" s="228" t="s">
+      <c r="W4" s="237"/>
+      <c r="X4" s="237"/>
+      <c r="Y4" s="237"/>
+      <c r="Z4" s="237"/>
+      <c r="AA4" s="237" t="s">
         <v>59</v>
       </c>
-      <c r="AB4" s="228"/>
-      <c r="AC4" s="228"/>
-      <c r="AD4" s="228"/>
-      <c r="AE4" s="228"/>
+      <c r="AB4" s="237"/>
+      <c r="AC4" s="237"/>
+      <c r="AD4" s="237"/>
+      <c r="AE4" s="237"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -19624,16 +19679,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="228" t="s">
+      <c r="B3" s="237" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="228"/>
-      <c r="D3" s="228"/>
-      <c r="E3" s="228" t="s">
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="228"/>
-      <c r="G3" s="228"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -19732,42 +19787,42 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="247" t="s">
+      <c r="A3" s="256" t="s">
         <v>270</v>
       </c>
-      <c r="B3" s="228" t="s">
+      <c r="B3" s="237" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="228"/>
-      <c r="D3" s="228"/>
-      <c r="E3" s="228" t="s">
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="228"/>
-      <c r="G3" s="228"/>
-      <c r="H3" s="228" t="s">
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
+      <c r="H3" s="237" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="228"/>
-      <c r="J3" s="228"/>
-      <c r="K3" s="228" t="s">
+      <c r="I3" s="237"/>
+      <c r="J3" s="237"/>
+      <c r="K3" s="237" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="228"/>
-      <c r="M3" s="228"/>
-      <c r="N3" s="228" t="s">
+      <c r="L3" s="237"/>
+      <c r="M3" s="237"/>
+      <c r="N3" s="237" t="s">
         <v>97</v>
       </c>
-      <c r="O3" s="228"/>
-      <c r="P3" s="228"/>
-      <c r="Q3" s="228" t="s">
+      <c r="O3" s="237"/>
+      <c r="P3" s="237"/>
+      <c r="Q3" s="237" t="s">
         <v>59</v>
       </c>
-      <c r="R3" s="228"/>
-      <c r="S3" s="228"/>
+      <c r="R3" s="237"/>
+      <c r="S3" s="237"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="247"/>
+      <c r="A4" s="256"/>
       <c r="B4" s="225" t="s">
         <v>41</v>
       </c>
@@ -20391,42 +20446,42 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="247" t="s">
+      <c r="A3" s="256" t="s">
         <v>270</v>
       </c>
-      <c r="B3" s="228" t="s">
+      <c r="B3" s="237" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="228"/>
-      <c r="D3" s="228"/>
-      <c r="E3" s="228" t="s">
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="228"/>
-      <c r="G3" s="228"/>
-      <c r="H3" s="228" t="s">
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
+      <c r="H3" s="237" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="228"/>
-      <c r="J3" s="228"/>
-      <c r="K3" s="228" t="s">
+      <c r="I3" s="237"/>
+      <c r="J3" s="237"/>
+      <c r="K3" s="237" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="228"/>
-      <c r="M3" s="228"/>
-      <c r="N3" s="228" t="s">
+      <c r="L3" s="237"/>
+      <c r="M3" s="237"/>
+      <c r="N3" s="237" t="s">
         <v>97</v>
       </c>
-      <c r="O3" s="228"/>
-      <c r="P3" s="228"/>
-      <c r="Q3" s="228" t="s">
+      <c r="O3" s="237"/>
+      <c r="P3" s="237"/>
+      <c r="Q3" s="237" t="s">
         <v>59</v>
       </c>
-      <c r="R3" s="228"/>
-      <c r="S3" s="228"/>
+      <c r="R3" s="237"/>
+      <c r="S3" s="237"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="247"/>
+      <c r="A4" s="256"/>
       <c r="B4" s="225" t="s">
         <v>41</v>
       </c>
@@ -21401,36 +21456,36 @@
       <c r="A2" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="B2" s="228" t="s">
+      <c r="B2" s="237" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228" t="s">
+      <c r="C2" s="237"/>
+      <c r="D2" s="237"/>
+      <c r="E2" s="237" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228" t="s">
+      <c r="F2" s="237"/>
+      <c r="G2" s="237"/>
+      <c r="H2" s="237" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228" t="s">
+      <c r="I2" s="237"/>
+      <c r="J2" s="237"/>
+      <c r="K2" s="237" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="228"/>
-      <c r="M2" s="228"/>
-      <c r="N2" s="228" t="s">
+      <c r="L2" s="237"/>
+      <c r="M2" s="237"/>
+      <c r="N2" s="237" t="s">
         <v>97</v>
       </c>
-      <c r="O2" s="228"/>
-      <c r="P2" s="228"/>
-      <c r="Q2" s="228" t="s">
+      <c r="O2" s="237"/>
+      <c r="P2" s="237"/>
+      <c r="Q2" s="237" t="s">
         <v>59</v>
       </c>
-      <c r="R2" s="228"/>
-      <c r="S2" s="228"/>
+      <c r="R2" s="237"/>
+      <c r="S2" s="237"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -21744,36 +21799,36 @@
       <c r="A12" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="B12" s="228" t="s">
+      <c r="B12" s="237" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="228"/>
-      <c r="D12" s="228"/>
-      <c r="E12" s="228" t="s">
+      <c r="C12" s="237"/>
+      <c r="D12" s="237"/>
+      <c r="E12" s="237" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="228"/>
-      <c r="G12" s="228"/>
-      <c r="H12" s="228" t="s">
+      <c r="F12" s="237"/>
+      <c r="G12" s="237"/>
+      <c r="H12" s="237" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="228"/>
-      <c r="J12" s="228"/>
-      <c r="K12" s="228" t="s">
+      <c r="I12" s="237"/>
+      <c r="J12" s="237"/>
+      <c r="K12" s="237" t="s">
         <v>55</v>
       </c>
-      <c r="L12" s="228"/>
-      <c r="M12" s="228"/>
-      <c r="N12" s="228" t="s">
+      <c r="L12" s="237"/>
+      <c r="M12" s="237"/>
+      <c r="N12" s="237" t="s">
         <v>97</v>
       </c>
-      <c r="O12" s="228"/>
-      <c r="P12" s="228"/>
-      <c r="Q12" s="228" t="s">
+      <c r="O12" s="237"/>
+      <c r="P12" s="237"/>
+      <c r="Q12" s="237" t="s">
         <v>59</v>
       </c>
-      <c r="R12" s="228"/>
-      <c r="S12" s="228"/>
+      <c r="R12" s="237"/>
+      <c r="S12" s="237"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -22205,36 +22260,36 @@
       <c r="A24" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="B24" s="228" t="s">
+      <c r="B24" s="237" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="228"/>
-      <c r="D24" s="228"/>
-      <c r="E24" s="228" t="s">
+      <c r="C24" s="237"/>
+      <c r="D24" s="237"/>
+      <c r="E24" s="237" t="s">
         <v>96</v>
       </c>
-      <c r="F24" s="228"/>
-      <c r="G24" s="228"/>
-      <c r="H24" s="228" t="s">
+      <c r="F24" s="237"/>
+      <c r="G24" s="237"/>
+      <c r="H24" s="237" t="s">
         <v>53</v>
       </c>
-      <c r="I24" s="228"/>
-      <c r="J24" s="228"/>
-      <c r="K24" s="228" t="s">
+      <c r="I24" s="237"/>
+      <c r="J24" s="237"/>
+      <c r="K24" s="237" t="s">
         <v>55</v>
       </c>
-      <c r="L24" s="228"/>
-      <c r="M24" s="228"/>
-      <c r="N24" s="228" t="s">
+      <c r="L24" s="237"/>
+      <c r="M24" s="237"/>
+      <c r="N24" s="237" t="s">
         <v>97</v>
       </c>
-      <c r="O24" s="228"/>
-      <c r="P24" s="228"/>
-      <c r="Q24" s="228" t="s">
+      <c r="O24" s="237"/>
+      <c r="P24" s="237"/>
+      <c r="Q24" s="237" t="s">
         <v>59</v>
       </c>
-      <c r="R24" s="228"/>
-      <c r="S24" s="228"/>
+      <c r="R24" s="237"/>
+      <c r="S24" s="237"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -22545,36 +22600,36 @@
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C34" s="228" t="s">
+      <c r="C34" s="237" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="228"/>
-      <c r="E34" s="228"/>
-      <c r="F34" s="228" t="s">
+      <c r="D34" s="237"/>
+      <c r="E34" s="237"/>
+      <c r="F34" s="237" t="s">
         <v>96</v>
       </c>
-      <c r="G34" s="228"/>
-      <c r="H34" s="228"/>
-      <c r="I34" s="228" t="s">
+      <c r="G34" s="237"/>
+      <c r="H34" s="237"/>
+      <c r="I34" s="237" t="s">
         <v>53</v>
       </c>
-      <c r="J34" s="228"/>
-      <c r="K34" s="228"/>
-      <c r="L34" s="228" t="s">
+      <c r="J34" s="237"/>
+      <c r="K34" s="237"/>
+      <c r="L34" s="237" t="s">
         <v>55</v>
       </c>
-      <c r="M34" s="228"/>
-      <c r="N34" s="228"/>
-      <c r="O34" s="228" t="s">
+      <c r="M34" s="237"/>
+      <c r="N34" s="237"/>
+      <c r="O34" s="237" t="s">
         <v>97</v>
       </c>
-      <c r="P34" s="228"/>
-      <c r="Q34" s="228"/>
-      <c r="R34" s="228" t="s">
+      <c r="P34" s="237"/>
+      <c r="Q34" s="237"/>
+      <c r="R34" s="237" t="s">
         <v>59</v>
       </c>
-      <c r="S34" s="228"/>
-      <c r="T34" s="228"/>
+      <c r="S34" s="237"/>
+      <c r="T34" s="237"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C35" s="225" t="s">
@@ -22794,775 +22849,775 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B19FC0C-B374-4655-B499-1D327735B887}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="248" customWidth="1"/>
-    <col min="2" max="2" width="14" style="248" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="248" customWidth="1"/>
-    <col min="4" max="16384" width="9.33203125" style="248"/>
+    <col min="1" max="1" width="16.5" style="228" customWidth="1"/>
+    <col min="2" max="2" width="14" style="228" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="228" customWidth="1"/>
+    <col min="4" max="16384" width="9.33203125" style="228"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="248" t="s">
+      <c r="A1" s="228" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="249" t="s">
+      <c r="A2" s="229" t="s">
         <v>323</v>
       </c>
-      <c r="B2" s="250" t="s">
+      <c r="B2" s="230" t="s">
         <v>328</v>
       </c>
-      <c r="C2" s="250" t="s">
+      <c r="C2" s="230" t="s">
         <v>324</v>
       </c>
-      <c r="D2" s="250" t="s">
+      <c r="D2" s="230" t="s">
         <v>325</v>
       </c>
-      <c r="E2" s="250" t="s">
+      <c r="E2" s="230" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="249" t="s">
+      <c r="A3" s="229" t="s">
         <v>327</v>
       </c>
-      <c r="B3" s="249">
+      <c r="B3" s="229">
         <v>20.399999999999999</v>
       </c>
-      <c r="C3" s="249">
+      <c r="C3" s="229">
         <v>0.96</v>
       </c>
-      <c r="D3" s="249">
+      <c r="D3" s="229">
         <v>511</v>
       </c>
-      <c r="E3" s="249">
+      <c r="E3" s="229">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="249" t="s">
+      <c r="A4" s="229" t="s">
         <v>329</v>
       </c>
-      <c r="B4" s="249">
+      <c r="B4" s="229">
         <v>10</v>
       </c>
-      <c r="C4" s="249">
+      <c r="C4" s="229">
         <v>1.19</v>
       </c>
-      <c r="D4" s="249">
+      <c r="D4" s="229">
         <v>511</v>
       </c>
-      <c r="E4" s="249">
+      <c r="E4" s="229">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="249" t="s">
+      <c r="A5" s="229" t="s">
         <v>330</v>
       </c>
-      <c r="B5" s="249">
+      <c r="B5" s="229">
         <v>2</v>
       </c>
-      <c r="C5" s="249">
+      <c r="C5" s="229">
         <v>1.72</v>
       </c>
-      <c r="D5" s="249">
+      <c r="D5" s="229">
         <v>511</v>
       </c>
-      <c r="E5" s="249">
+      <c r="E5" s="229">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="249" t="s">
+      <c r="A6" s="229" t="s">
         <v>331</v>
       </c>
-      <c r="B6" s="249">
+      <c r="B6" s="229">
         <v>109.8</v>
       </c>
-      <c r="C6" s="249">
+      <c r="C6" s="229">
         <v>0.63</v>
       </c>
-      <c r="D6" s="249">
+      <c r="D6" s="229">
         <v>511</v>
       </c>
-      <c r="E6" s="249">
+      <c r="E6" s="229">
         <v>1.93</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="254" t="s">
+      <c r="A7" s="257" t="s">
         <v>332</v>
       </c>
-      <c r="B7" s="251">
+      <c r="B7" s="262">
         <f>12.7*60</f>
         <v>762</v>
       </c>
-      <c r="C7" s="254">
+      <c r="C7" s="257">
         <v>0.65</v>
       </c>
-      <c r="D7" s="249">
+      <c r="D7" s="229">
         <v>511</v>
       </c>
-      <c r="E7" s="249">
+      <c r="E7" s="229">
         <v>0.38</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="255"/>
-      <c r="B8" s="251"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="249">
+      <c r="A8" s="258"/>
+      <c r="B8" s="262"/>
+      <c r="C8" s="258"/>
+      <c r="D8" s="229">
         <v>1346</v>
       </c>
-      <c r="E8" s="249">
+      <c r="E8" s="229">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="249" t="s">
+      <c r="A9" s="229" t="s">
         <v>333</v>
       </c>
-      <c r="B9" s="249">
+      <c r="B9" s="229">
         <v>68.3</v>
       </c>
-      <c r="C9" s="249">
+      <c r="C9" s="229">
         <v>1.9</v>
       </c>
-      <c r="D9" s="249">
+      <c r="D9" s="229">
         <v>511</v>
       </c>
-      <c r="E9" s="249">
+      <c r="E9" s="229">
         <v>1.84</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="254" t="s">
+      <c r="A10" s="257" t="s">
         <v>334</v>
       </c>
-      <c r="B10" s="252">
+      <c r="B10" s="263">
         <f>76/60</f>
         <v>1.2666666666666666</v>
       </c>
-      <c r="C10" s="254">
+      <c r="C10" s="257">
         <v>3.35</v>
       </c>
-      <c r="D10" s="249">
+      <c r="D10" s="229">
         <v>511</v>
       </c>
-      <c r="E10" s="249">
+      <c r="E10" s="229">
         <v>1.9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="255"/>
-      <c r="B11" s="252"/>
-      <c r="C11" s="255"/>
-      <c r="D11" s="249">
+      <c r="A11" s="258"/>
+      <c r="B11" s="263"/>
+      <c r="C11" s="258"/>
+      <c r="D11" s="229">
         <v>776</v>
       </c>
-      <c r="E11" s="249">
+      <c r="E11" s="229">
         <v>0.13</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="254" t="s">
+      <c r="A12" s="257" t="s">
         <v>335</v>
       </c>
-      <c r="B12" s="251">
+      <c r="B12" s="262">
         <f>4.2*60*24</f>
         <v>6048</v>
       </c>
-      <c r="C12" s="249">
+      <c r="C12" s="229">
         <v>1.54</v>
       </c>
-      <c r="D12" s="249">
+      <c r="D12" s="229">
         <v>511</v>
       </c>
-      <c r="E12" s="249">
+      <c r="E12" s="229">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="256"/>
-      <c r="B13" s="251"/>
-      <c r="C13" s="249">
+      <c r="A13" s="259"/>
+      <c r="B13" s="262"/>
+      <c r="C13" s="229">
         <v>2.17</v>
       </c>
-      <c r="D13" s="249">
+      <c r="D13" s="229">
         <v>603</v>
       </c>
-      <c r="E13" s="249">
+      <c r="E13" s="229">
         <v>0.62</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="255"/>
-      <c r="B14" s="251"/>
-      <c r="C14" s="249"/>
-      <c r="D14" s="249">
+      <c r="A14" s="258"/>
+      <c r="B14" s="262"/>
+      <c r="C14" s="229"/>
+      <c r="D14" s="229">
         <v>1693</v>
       </c>
-      <c r="E14" s="249">
+      <c r="E14" s="229">
         <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="248" t="s">
+      <c r="A16" s="228" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="249" t="s">
+      <c r="A17" s="229" t="s">
         <v>323</v>
       </c>
-      <c r="B17" s="250" t="s">
+      <c r="B17" s="230" t="s">
         <v>337</v>
       </c>
-      <c r="C17" s="250" t="s">
+      <c r="C17" s="230" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="249" t="s">
+      <c r="A18" s="229" t="s">
         <v>327</v>
       </c>
-      <c r="B18" s="249">
+      <c r="B18" s="229">
         <v>0.14799999999999999</v>
       </c>
-      <c r="C18" s="249">
+      <c r="C18" s="229">
         <v>6.3E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="249" t="s">
+      <c r="A19" s="229" t="s">
         <v>329</v>
       </c>
-      <c r="B19" s="249">
+      <c r="B19" s="229">
         <v>0.14799999999999999</v>
       </c>
-      <c r="C19" s="249">
+      <c r="C19" s="229">
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="249" t="s">
+      <c r="A20" s="229" t="s">
         <v>330</v>
       </c>
-      <c r="B20" s="249">
+      <c r="B20" s="229">
         <v>0.14799999999999999</v>
       </c>
-      <c r="C20" s="249">
+      <c r="C20" s="229">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="249" t="s">
+      <c r="A21" s="229" t="s">
         <v>331</v>
       </c>
-      <c r="B21" s="249">
+      <c r="B21" s="229">
         <v>0.14299999999999999</v>
       </c>
-      <c r="C21" s="249">
+      <c r="C21" s="229">
         <v>0.11899999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="249" t="s">
+      <c r="A22" s="229" t="s">
         <v>332</v>
       </c>
-      <c r="B22" s="249">
+      <c r="B22" s="229">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="C22" s="249">
+      <c r="C22" s="229">
         <v>0.24</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="249" t="s">
+      <c r="A23" s="229" t="s">
         <v>333</v>
       </c>
-      <c r="B23" s="249">
+      <c r="B23" s="229">
         <v>0.13400000000000001</v>
       </c>
-      <c r="C23" s="249">
+      <c r="C23" s="229">
         <v>0.10100000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="249" t="s">
+      <c r="A24" s="229" t="s">
         <v>334</v>
       </c>
-      <c r="B24" s="249">
+      <c r="B24" s="229">
         <v>0.159</v>
       </c>
-      <c r="C24" s="249">
+      <c r="C24" s="229">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="249" t="s">
+      <c r="A25" s="229" t="s">
         <v>335</v>
       </c>
-      <c r="B25" s="249">
+      <c r="B25" s="229">
         <v>0.185</v>
       </c>
-      <c r="C25" s="249">
+      <c r="C25" s="229">
         <v>0.184</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="248" t="s">
+      <c r="A27" s="228" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="251" t="s">
+      <c r="A28" s="262" t="s">
         <v>340</v>
       </c>
-      <c r="B28" s="251"/>
-      <c r="C28" s="249" t="s">
+      <c r="B28" s="262"/>
+      <c r="C28" s="229" t="s">
         <v>341</v>
       </c>
-      <c r="D28" s="257" t="s">
+      <c r="D28" s="260" t="s">
         <v>342</v>
       </c>
-      <c r="E28" s="258"/>
-      <c r="F28" s="253" t="s">
+      <c r="E28" s="261"/>
+      <c r="F28" s="231" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="251" t="s">
+      <c r="A29" s="262" t="s">
         <v>343</v>
       </c>
-      <c r="B29" s="251"/>
-      <c r="C29" s="249">
+      <c r="B29" s="262"/>
+      <c r="C29" s="229">
         <v>15.4</v>
       </c>
-      <c r="D29" s="257" t="s">
+      <c r="D29" s="260" t="s">
         <v>344</v>
       </c>
-      <c r="E29" s="258"/>
-      <c r="F29" s="253"/>
+      <c r="E29" s="261"/>
+      <c r="F29" s="231"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="251" t="s">
+      <c r="A30" s="262" t="s">
         <v>345</v>
       </c>
-      <c r="B30" s="251"/>
-      <c r="C30" s="249">
+      <c r="B30" s="262"/>
+      <c r="C30" s="229">
         <v>0.13400000000000001</v>
       </c>
-      <c r="D30" s="251" t="s">
+      <c r="D30" s="262" t="s">
         <v>346</v>
       </c>
-      <c r="E30" s="251"/>
-      <c r="F30" s="253"/>
+      <c r="E30" s="262"/>
+      <c r="F30" s="231"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="251" t="s">
+      <c r="A31" s="262" t="s">
         <v>347</v>
       </c>
-      <c r="B31" s="251"/>
-      <c r="C31" s="249">
+      <c r="B31" s="262"/>
+      <c r="C31" s="229">
         <v>0.14299999999999999</v>
       </c>
-      <c r="D31" s="251"/>
-      <c r="E31" s="251"/>
-      <c r="F31" s="253"/>
+      <c r="D31" s="262"/>
+      <c r="E31" s="262"/>
+      <c r="F31" s="231"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="251" t="s">
+      <c r="A32" s="262" t="s">
         <v>348</v>
       </c>
-      <c r="B32" s="251"/>
-      <c r="C32" s="249">
+      <c r="B32" s="262"/>
+      <c r="C32" s="229">
         <v>0.14799999999999999</v>
       </c>
-      <c r="D32" s="251"/>
-      <c r="E32" s="251"/>
-      <c r="F32" s="253" t="s">
+      <c r="D32" s="262"/>
+      <c r="E32" s="262"/>
+      <c r="F32" s="231" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="251" t="s">
+      <c r="A33" s="262" t="s">
         <v>349</v>
       </c>
-      <c r="B33" s="251"/>
-      <c r="C33" s="249">
+      <c r="B33" s="262"/>
+      <c r="C33" s="229">
         <v>0.183</v>
       </c>
-      <c r="D33" s="251"/>
-      <c r="E33" s="251"/>
-      <c r="F33" s="253"/>
+      <c r="D33" s="262"/>
+      <c r="E33" s="262"/>
+      <c r="F33" s="231"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="251" t="s">
+      <c r="A34" s="262" t="s">
         <v>350</v>
       </c>
-      <c r="B34" s="251"/>
-      <c r="C34" s="249">
+      <c r="B34" s="262"/>
+      <c r="C34" s="229">
         <v>0.188</v>
       </c>
-      <c r="D34" s="251"/>
-      <c r="E34" s="251"/>
-      <c r="F34" s="253"/>
+      <c r="D34" s="262"/>
+      <c r="E34" s="262"/>
+      <c r="F34" s="231"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="248" t="s">
+      <c r="A36" s="228" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="250" t="s">
+      <c r="A37" s="230" t="s">
         <v>354</v>
       </c>
-      <c r="B37" s="250" t="s">
+      <c r="B37" s="230" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="250" t="s">
+      <c r="C37" s="230" t="s">
         <v>356</v>
       </c>
-      <c r="D37" s="250" t="s">
+      <c r="D37" s="230" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="249">
+      <c r="A38" s="229">
         <v>0</v>
       </c>
-      <c r="B38" s="249">
+      <c r="B38" s="229">
         <v>1</v>
       </c>
-      <c r="C38" s="249">
+      <c r="C38" s="229">
         <v>1</v>
       </c>
-      <c r="D38" s="249">
+      <c r="D38" s="229">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="249">
+      <c r="A39" s="229">
         <v>1</v>
       </c>
-      <c r="B39" s="249">
+      <c r="B39" s="229">
         <v>0.89119999999999999</v>
       </c>
-      <c r="C39" s="249">
+      <c r="C39" s="229">
         <v>0.95830000000000004</v>
       </c>
-      <c r="D39" s="249">
+      <c r="D39" s="229">
         <v>0.74839999999999995</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="249">
+      <c r="A40" s="229">
         <v>2</v>
       </c>
-      <c r="B40" s="249">
+      <c r="B40" s="229">
         <v>0.7873</v>
       </c>
-      <c r="C40" s="249">
+      <c r="C40" s="229">
         <v>0.90880000000000005</v>
       </c>
-      <c r="D40" s="249">
+      <c r="D40" s="229">
         <v>0.53249999999999997</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="249">
+      <c r="A41" s="229">
         <v>3</v>
       </c>
-      <c r="B41" s="249">
+      <c r="B41" s="229">
         <v>0.6905</v>
       </c>
-      <c r="C41" s="249">
+      <c r="C41" s="229">
         <v>0.85189999999999999</v>
       </c>
-      <c r="D41" s="249">
+      <c r="D41" s="229">
         <v>0.3614</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="249">
+      <c r="A42" s="229">
         <v>4</v>
       </c>
-      <c r="B42" s="249">
+      <c r="B42" s="229">
         <v>0.60209999999999997</v>
       </c>
-      <c r="C42" s="249">
+      <c r="C42" s="229">
         <v>0.78890000000000005</v>
       </c>
-      <c r="D42" s="249">
+      <c r="D42" s="229">
         <v>0.23530000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="249">
+      <c r="A43" s="229">
         <v>5</v>
       </c>
-      <c r="B43" s="249">
+      <c r="B43" s="229">
         <v>0.52270000000000005</v>
       </c>
-      <c r="C43" s="249">
+      <c r="C43" s="229">
         <v>0.7218</v>
       </c>
-      <c r="D43" s="249">
+      <c r="D43" s="229">
         <v>0.1479</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="249">
+      <c r="A44" s="229">
         <v>6</v>
       </c>
-      <c r="B44" s="249">
+      <c r="B44" s="229">
         <v>0.45219999999999999</v>
       </c>
-      <c r="C44" s="249">
+      <c r="C44" s="229">
         <v>0.65280000000000005</v>
       </c>
-      <c r="D44" s="249">
+      <c r="D44" s="229">
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="249">
+      <c r="A45" s="229">
         <v>7</v>
       </c>
-      <c r="B45" s="249">
+      <c r="B45" s="229">
         <v>0.39029999999999998</v>
       </c>
-      <c r="C45" s="249">
+      <c r="C45" s="229">
         <v>0.58420000000000005</v>
       </c>
-      <c r="D45" s="249">
+      <c r="D45" s="229">
         <v>5.4199999999999998E-2</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="249">
+      <c r="A46" s="229">
         <v>8</v>
       </c>
-      <c r="B46" s="249">
+      <c r="B46" s="229">
         <v>0.3362</v>
       </c>
-      <c r="C46" s="249">
+      <c r="C46" s="229">
         <v>0.51800000000000002</v>
       </c>
-      <c r="D46" s="249">
+      <c r="D46" s="229">
         <v>3.1899999999999998E-2</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="249">
+      <c r="A47" s="229">
         <v>9</v>
       </c>
-      <c r="B47" s="249">
+      <c r="B47" s="229">
         <v>0.28920000000000001</v>
       </c>
-      <c r="C47" s="249">
+      <c r="C47" s="229">
         <v>0.45579999999999998</v>
       </c>
-      <c r="D47" s="249">
+      <c r="D47" s="229">
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="249">
+      <c r="A48" s="229">
         <v>10</v>
       </c>
-      <c r="B48" s="249">
+      <c r="B48" s="229">
         <v>0.2485</v>
       </c>
-      <c r="C48" s="249">
+      <c r="C48" s="229">
         <v>0.3987</v>
       </c>
-      <c r="D48" s="249">
+      <c r="D48" s="229">
         <v>1.0699999999999999E-2</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="249">
+      <c r="A49" s="229">
         <v>12</v>
       </c>
-      <c r="B49" s="249">
+      <c r="B49" s="229">
         <v>0.18310000000000001</v>
       </c>
-      <c r="C49" s="249">
+      <c r="C49" s="229">
         <v>0.30080000000000001</v>
       </c>
-      <c r="D49" s="249">
+      <c r="D49" s="229">
         <v>3.5000000000000001E-3</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="249">
+      <c r="A50" s="229">
         <v>14</v>
       </c>
-      <c r="B50" s="249">
+      <c r="B50" s="229">
         <v>0.13469999999999999</v>
       </c>
-      <c r="C50" s="249">
+      <c r="C50" s="229">
         <v>0.2243</v>
       </c>
-      <c r="D50" s="249">
+      <c r="D50" s="229">
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="249">
+      <c r="A51" s="229">
         <v>16</v>
       </c>
-      <c r="B51" s="249">
+      <c r="B51" s="229">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="C51" s="249">
+      <c r="C51" s="229">
         <v>0.16619999999999999</v>
       </c>
-      <c r="D51" s="249">
+      <c r="D51" s="229">
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="249">
+      <c r="A52" s="229">
         <v>18</v>
       </c>
-      <c r="B52" s="249">
+      <c r="B52" s="229">
         <v>7.2800000000000004E-2</v>
       </c>
-      <c r="C52" s="249">
+      <c r="C52" s="229">
         <v>0.1227</v>
       </c>
-      <c r="D52" s="249">
+      <c r="D52" s="229">
         <v>1E-4</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="249">
+      <c r="A53" s="229">
         <v>20</v>
       </c>
-      <c r="B53" s="249">
+      <c r="B53" s="229">
         <v>5.3499999999999999E-2</v>
       </c>
-      <c r="C53" s="249">
+      <c r="C53" s="229">
         <v>9.0399999999999994E-2</v>
       </c>
-      <c r="D53" s="249"/>
+      <c r="D53" s="229"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="249">
+      <c r="A54" s="229">
         <v>25</v>
       </c>
-      <c r="B54" s="249">
+      <c r="B54" s="229">
         <v>2.47E-2</v>
       </c>
-      <c r="C54" s="249">
+      <c r="C54" s="229">
         <v>4.19E-2</v>
       </c>
-      <c r="D54" s="249"/>
+      <c r="D54" s="229"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="249">
+      <c r="A55" s="229">
         <v>30</v>
       </c>
-      <c r="B55" s="249">
+      <c r="B55" s="229">
         <v>1.14E-2</v>
       </c>
-      <c r="C55" s="249">
+      <c r="C55" s="229">
         <v>1.9400000000000001E-2</v>
       </c>
-      <c r="D55" s="249"/>
+      <c r="D55" s="229"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="249">
+      <c r="A56" s="229">
         <v>40</v>
       </c>
-      <c r="B56" s="249">
+      <c r="B56" s="229">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="C56" s="249">
+      <c r="C56" s="229">
         <v>4.1999999999999997E-3</v>
       </c>
-      <c r="D56" s="249"/>
+      <c r="D56" s="229"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="249">
+      <c r="A57" s="229">
         <v>50</v>
       </c>
-      <c r="B57" s="249">
+      <c r="B57" s="229">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="C57" s="249">
+      <c r="C57" s="229">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D57" s="249"/>
+      <c r="D57" s="229"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="248" t="s">
+      <c r="A59" s="228" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="249" t="s">
+      <c r="A60" s="229" t="s">
         <v>358</v>
       </c>
-      <c r="B60" s="259" t="s">
+      <c r="B60" s="232" t="s">
         <v>41</v>
       </c>
-      <c r="C60" s="259" t="s">
+      <c r="C60" s="232" t="s">
         <v>42</v>
       </c>
-      <c r="D60" s="259" t="s">
+      <c r="D60" s="232" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="249" t="s">
+      <c r="A61" s="229" t="s">
         <v>49</v>
       </c>
-      <c r="B61" s="249">
+      <c r="B61" s="229">
         <v>0.15429999999999999</v>
       </c>
-      <c r="C61" s="249">
+      <c r="C61" s="229">
         <v>-0.44080000000000003</v>
       </c>
-      <c r="D61" s="249">
+      <c r="D61" s="229">
         <v>2.1360000000000001</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="249" t="s">
+      <c r="A62" s="229" t="s">
         <v>51</v>
       </c>
-      <c r="B62" s="249">
+      <c r="B62" s="229">
         <v>0.15390000000000001</v>
       </c>
-      <c r="C62" s="249">
+      <c r="C62" s="229">
         <v>-0.11609999999999999</v>
       </c>
-      <c r="D62" s="249">
+      <c r="D62" s="229">
         <v>2.0752000000000002</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="249" t="s">
+      <c r="A63" s="229" t="s">
         <v>355</v>
       </c>
-      <c r="B63" s="249">
+      <c r="B63" s="229">
         <v>0.57040000000000002</v>
       </c>
-      <c r="C63" s="249">
+      <c r="C63" s="229">
         <v>-0.30630000000000002</v>
       </c>
-      <c r="D63" s="249">
+      <c r="D63" s="229">
         <v>0.63260000000000005</v>
       </c>
     </row>
@@ -23574,11 +23629,6 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C10:C11"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
@@ -23586,10 +23636,399 @@
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DE8792-DD2B-477A-AF5C-DCF89AF48366}">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" style="227"/>
+    <col min="2" max="4" width="15.83203125" style="227" customWidth="1"/>
+    <col min="5" max="16384" width="9.33203125" style="227"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="233" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="233" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="233" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="233" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="234" t="s">
+        <v>323</v>
+      </c>
+      <c r="B6" s="230" t="s">
+        <v>362</v>
+      </c>
+      <c r="C6" s="230" t="s">
+        <v>363</v>
+      </c>
+      <c r="D6" s="230" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="234" t="s">
+        <v>365</v>
+      </c>
+      <c r="B7" s="235">
+        <v>20.85</v>
+      </c>
+      <c r="C7" s="235">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="D7" s="235">
+        <v>17.739999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="234" t="s">
+        <v>366</v>
+      </c>
+      <c r="B8" s="235">
+        <v>41.57</v>
+      </c>
+      <c r="C8" s="235">
+        <v>1.23</v>
+      </c>
+      <c r="D8" s="235">
+        <v>12.58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="234" t="s">
+        <v>367</v>
+      </c>
+      <c r="B9" s="235">
+        <v>57.44</v>
+      </c>
+      <c r="C9" s="235">
+        <v>10.28</v>
+      </c>
+      <c r="D9" s="235">
+        <v>21.23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="234" t="s">
+        <v>368</v>
+      </c>
+      <c r="B10" s="235">
+        <v>83.14</v>
+      </c>
+      <c r="C10" s="235">
+        <v>2.33</v>
+      </c>
+      <c r="D10" s="235">
+        <v>15.17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="234" t="s">
+        <v>369</v>
+      </c>
+      <c r="B11" s="235">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C11" s="235">
+        <v>1.08</v>
+      </c>
+      <c r="D11" s="235">
+        <v>14.32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="234" t="s">
+        <v>370</v>
+      </c>
+      <c r="B12" s="235">
+        <v>11.29</v>
+      </c>
+      <c r="C12" s="235">
+        <v>0.89</v>
+      </c>
+      <c r="D12" s="235">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="234" t="s">
+        <v>371</v>
+      </c>
+      <c r="B13" s="235">
+        <v>13.87</v>
+      </c>
+      <c r="C13" s="235">
+        <v>0.4</v>
+      </c>
+      <c r="D13" s="235">
+        <v>5.58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="233" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="229" t="s">
+        <v>323</v>
+      </c>
+      <c r="B16" s="232" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="232" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="232" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="234" t="s">
+        <v>365</v>
+      </c>
+      <c r="B17" s="229">
+        <v>4.4119999999999999E-2</v>
+      </c>
+      <c r="C17" s="229">
+        <v>0.73260000000000003</v>
+      </c>
+      <c r="D17" s="229">
+        <v>0.38690000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="234" t="s">
+        <v>366</v>
+      </c>
+      <c r="B18" s="229">
+        <v>0.13220000000000001</v>
+      </c>
+      <c r="C18" s="229">
+        <v>14.85</v>
+      </c>
+      <c r="D18" s="229">
+        <v>1.488</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="234" t="s">
+        <v>367</v>
+      </c>
+      <c r="B19" s="229">
+        <v>0.10780000000000001</v>
+      </c>
+      <c r="C19" s="229">
+        <v>0.20030000000000001</v>
+      </c>
+      <c r="D19" s="229">
+        <v>0.49569999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="234" t="s">
+        <v>368</v>
+      </c>
+      <c r="B20" s="229">
+        <v>0.70940000000000003</v>
+      </c>
+      <c r="C20" s="229">
+        <v>30.63</v>
+      </c>
+      <c r="D20" s="229">
+        <v>5.9790000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="234" t="s">
+        <v>369</v>
+      </c>
+      <c r="B21" s="229">
+        <v>2.4790000000000001</v>
+      </c>
+      <c r="C21" s="229">
+        <v>-1.093</v>
+      </c>
+      <c r="D21" s="229">
+        <v>1.3759999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="234" t="s">
+        <v>370</v>
+      </c>
+      <c r="B22" s="229">
+        <v>1.67</v>
+      </c>
+      <c r="C22" s="229">
+        <v>1.3580000000000001</v>
+      </c>
+      <c r="D22" s="229">
+        <v>0.36919999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="234" t="s">
+        <v>371</v>
+      </c>
+      <c r="B23" s="229">
+        <v>2.66</v>
+      </c>
+      <c r="C23" s="229">
+        <v>55.84</v>
+      </c>
+      <c r="D23" s="229">
+        <v>2.419</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="233" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="229" t="s">
+        <v>323</v>
+      </c>
+      <c r="B26" s="232" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="232" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="232" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="234" t="s">
+        <v>365</v>
+      </c>
+      <c r="B27" s="229">
+        <v>0.1865</v>
+      </c>
+      <c r="C27" s="229">
+        <v>-0.15290000000000001</v>
+      </c>
+      <c r="D27" s="229">
+        <v>1.6830000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="234" t="s">
+        <v>366</v>
+      </c>
+      <c r="B28" s="229">
+        <v>0.18659999999999999</v>
+      </c>
+      <c r="C28" s="229">
+        <v>1253</v>
+      </c>
+      <c r="D28" s="229">
+        <v>74.930000000000007</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="234" t="s">
+        <v>367</v>
+      </c>
+      <c r="B29" s="229">
+        <v>0.17050000000000001</v>
+      </c>
+      <c r="C29" s="229">
+        <v>-0.1308</v>
+      </c>
+      <c r="D29" s="229">
+        <v>1.038</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="234" t="s">
+        <v>368</v>
+      </c>
+      <c r="B30" s="229">
+        <v>0.2339</v>
+      </c>
+      <c r="C30" s="229">
+        <v>-0.1265</v>
+      </c>
+      <c r="D30" s="229">
+        <v>0.46179999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="234" t="s">
+        <v>369</v>
+      </c>
+      <c r="B31" s="229">
+        <v>0.28129999999999999</v>
+      </c>
+      <c r="C31" s="229">
+        <v>-0.2349</v>
+      </c>
+      <c r="D31" s="229">
+        <v>0.96530000000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="234" t="s">
+        <v>370</v>
+      </c>
+      <c r="B32" s="229">
+        <v>0.26069999999999999</v>
+      </c>
+      <c r="C32" s="229">
+        <v>-0.26069999999999999</v>
+      </c>
+      <c r="D32" s="229">
+        <v>20.99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="234" t="s">
+        <v>371</v>
+      </c>
+      <c r="B33" s="229">
+        <v>0.36969999999999997</v>
+      </c>
+      <c r="C33" s="229">
+        <v>2.8370000000000002</v>
+      </c>
+      <c r="D33" s="229">
+        <v>7.149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -23609,22 +24048,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1" s="236" t="s">
+      <c r="B1" s="245" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236" t="s">
+      <c r="C1" s="245"/>
+      <c r="D1" s="245" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="H1" s="237" t="s">
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="H1" s="246" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="237"/>
-      <c r="J1" s="237"/>
-      <c r="K1" s="237"/>
-      <c r="L1" s="237"/>
+      <c r="I1" s="246"/>
+      <c r="J1" s="246"/>
+      <c r="K1" s="246"/>
+      <c r="L1" s="246"/>
       <c r="M1" s="98"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -23719,13 +24158,13 @@
       <c r="D5" s="101"/>
       <c r="E5" s="101"/>
       <c r="F5" s="101"/>
-      <c r="H5" s="238" t="s">
+      <c r="H5" s="247" t="s">
         <v>103</v>
       </c>
-      <c r="I5" s="238"/>
-      <c r="J5" s="238"/>
-      <c r="K5" s="238"/>
-      <c r="L5" s="238"/>
+      <c r="I5" s="247"/>
+      <c r="J5" s="247"/>
+      <c r="K5" s="247"/>
+      <c r="L5" s="247"/>
       <c r="M5" s="98"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -25009,16 +25448,16 @@
         <v>172</v>
       </c>
       <c r="N19" s="122"/>
-      <c r="P19" s="228" t="s">
+      <c r="P19" s="237" t="s">
         <v>95</v>
       </c>
-      <c r="Q19" s="228"/>
-      <c r="R19" s="228"/>
-      <c r="S19" s="228" t="s">
+      <c r="Q19" s="237"/>
+      <c r="R19" s="237"/>
+      <c r="S19" s="237" t="s">
         <v>96</v>
       </c>
-      <c r="T19" s="228"/>
-      <c r="U19" s="228"/>
+      <c r="T19" s="237"/>
+      <c r="U19" s="237"/>
       <c r="V19"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
@@ -25239,7 +25678,7 @@
       <c r="H27" s="154" t="s">
         <v>49</v>
       </c>
-      <c r="J27" s="239" t="s">
+      <c r="J27" s="248" t="s">
         <v>191</v>
       </c>
       <c r="K27" s="115" t="s">
@@ -25281,7 +25720,7 @@
       <c r="H28" s="158" t="s">
         <v>199</v>
       </c>
-      <c r="J28" s="239"/>
+      <c r="J28" s="248"/>
       <c r="K28" s="115" t="s">
         <v>200</v>
       </c>
@@ -26608,7 +27047,7 @@
       <c r="E18" s="169" t="s">
         <v>224</v>
       </c>
-      <c r="F18" s="240" t="s">
+      <c r="F18" s="249" t="s">
         <v>225</v>
       </c>
       <c r="L18" s="188" t="s">
@@ -26654,7 +27093,7 @@
       <c r="E19" s="169" t="s">
         <v>187</v>
       </c>
-      <c r="F19" s="240"/>
+      <c r="F19" s="249"/>
       <c r="G19" s="169" t="s">
         <v>49</v>
       </c>
@@ -26687,22 +27126,22 @@
       <c r="E20" s="191" t="s">
         <v>226</v>
       </c>
-      <c r="F20" s="240"/>
+      <c r="F20" s="249"/>
       <c r="G20" s="191" t="s">
         <v>199</v>
       </c>
       <c r="H20" s="191" t="s">
         <v>227</v>
       </c>
-      <c r="L20" s="241" t="s">
+      <c r="L20" s="250" t="s">
         <v>228</v>
       </c>
-      <c r="M20" s="241"/>
-      <c r="N20" s="241"/>
-      <c r="O20" s="241"/>
-      <c r="P20" s="241"/>
-      <c r="Q20" s="241"/>
-      <c r="R20" s="241"/>
+      <c r="M20" s="250"/>
+      <c r="N20" s="250"/>
+      <c r="O20" s="250"/>
+      <c r="P20" s="250"/>
+      <c r="Q20" s="250"/>
+      <c r="R20" s="250"/>
       <c r="T20" s="169">
         <v>1.1906250009999999</v>
       </c>
@@ -27589,42 +28028,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A1" s="242" t="s">
+      <c r="A1" s="251" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="242"/>
-      <c r="I1" s="242"/>
-      <c r="J1" s="242"/>
-      <c r="K1" s="242"/>
-      <c r="L1" s="242"/>
-      <c r="M1" s="242"/>
-      <c r="N1" s="242"/>
-      <c r="O1" s="242"/>
-      <c r="P1" s="242"/>
-      <c r="Q1" s="243" t="s">
+      <c r="B1" s="251"/>
+      <c r="C1" s="251"/>
+      <c r="D1" s="251"/>
+      <c r="E1" s="251"/>
+      <c r="F1" s="251"/>
+      <c r="G1" s="251"/>
+      <c r="H1" s="251"/>
+      <c r="I1" s="251"/>
+      <c r="J1" s="251"/>
+      <c r="K1" s="251"/>
+      <c r="L1" s="251"/>
+      <c r="M1" s="251"/>
+      <c r="N1" s="251"/>
+      <c r="O1" s="251"/>
+      <c r="P1" s="251"/>
+      <c r="Q1" s="252" t="s">
         <v>90</v>
       </c>
-      <c r="R1" s="243"/>
-      <c r="S1" s="243"/>
-      <c r="T1" s="243"/>
-      <c r="U1" s="243"/>
-      <c r="V1" s="243"/>
-      <c r="W1" s="243"/>
-      <c r="X1" s="243"/>
-      <c r="Y1" s="243"/>
-      <c r="Z1" s="243"/>
-      <c r="AA1" s="243"/>
-      <c r="AB1" s="243"/>
-      <c r="AC1" s="243"/>
-      <c r="AD1" s="243"/>
-      <c r="AE1" s="243"/>
-      <c r="AF1" s="243"/>
+      <c r="R1" s="252"/>
+      <c r="S1" s="252"/>
+      <c r="T1" s="252"/>
+      <c r="U1" s="252"/>
+      <c r="V1" s="252"/>
+      <c r="W1" s="252"/>
+      <c r="X1" s="252"/>
+      <c r="Y1" s="252"/>
+      <c r="Z1" s="252"/>
+      <c r="AA1" s="252"/>
+      <c r="AB1" s="252"/>
+      <c r="AC1" s="252"/>
+      <c r="AD1" s="252"/>
+      <c r="AE1" s="252"/>
+      <c r="AF1" s="252"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="199"/>
@@ -27639,46 +28078,46 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="204"/>
-      <c r="B3" s="244" t="s">
+      <c r="B3" s="253" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="244"/>
-      <c r="D3" s="244"/>
+      <c r="C3" s="253"/>
+      <c r="D3" s="253"/>
       <c r="E3" s="205"/>
       <c r="F3" s="205"/>
-      <c r="G3" s="244" t="s">
+      <c r="G3" s="253" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="244"/>
-      <c r="I3" s="244"/>
+      <c r="H3" s="253"/>
+      <c r="I3" s="253"/>
       <c r="J3" s="205"/>
       <c r="K3" s="205"/>
-      <c r="L3" s="244" t="s">
+      <c r="L3" s="253" t="s">
         <v>53</v>
       </c>
-      <c r="M3" s="244"/>
-      <c r="N3" s="244"/>
+      <c r="M3" s="253"/>
+      <c r="N3" s="253"/>
       <c r="O3" s="205"/>
       <c r="P3" s="205"/>
-      <c r="Q3" s="245" t="s">
+      <c r="Q3" s="254" t="s">
         <v>55</v>
       </c>
-      <c r="R3" s="245"/>
-      <c r="S3" s="245"/>
+      <c r="R3" s="254"/>
+      <c r="S3" s="254"/>
       <c r="T3" s="205"/>
       <c r="U3" s="205"/>
-      <c r="V3" s="244" t="s">
+      <c r="V3" s="253" t="s">
         <v>97</v>
       </c>
-      <c r="W3" s="244"/>
-      <c r="X3" s="244"/>
+      <c r="W3" s="253"/>
+      <c r="X3" s="253"/>
       <c r="Y3" s="205"/>
       <c r="Z3" s="205"/>
-      <c r="AA3" s="244" t="s">
+      <c r="AA3" s="253" t="s">
         <v>59</v>
       </c>
-      <c r="AB3" s="244"/>
-      <c r="AC3" s="244"/>
+      <c r="AB3" s="253"/>
+      <c r="AC3" s="253"/>
       <c r="AD3" s="205"/>
       <c r="AE3" s="205"/>
       <c r="AF3" s="206"/>
@@ -30757,16 +31196,16 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="228" t="s">
+      <c r="B3" s="237" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="228"/>
-      <c r="D3" s="228"/>
-      <c r="E3" s="228" t="s">
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237" t="s">
         <v>242</v>
       </c>
-      <c r="F3" s="228"/>
-      <c r="G3" s="228"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
     </row>
     <row r="4" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="222" t="s">
@@ -31613,11 +32052,11 @@
       <c r="A30" t="s">
         <v>253</v>
       </c>
-      <c r="B30" s="228">
+      <c r="B30" s="237">
         <v>110</v>
       </c>
-      <c r="C30" s="228"/>
-      <c r="D30" s="228"/>
+      <c r="C30" s="237"/>
+      <c r="D30" s="237"/>
       <c r="E30">
         <v>18</v>
       </c>
@@ -31673,14 +32112,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="246" t="s">
+      <c r="C3" s="255" t="s">
         <v>256</v>
       </c>
-      <c r="D3" s="246"/>
-      <c r="E3" s="246" t="s">
+      <c r="D3" s="255"/>
+      <c r="E3" s="255" t="s">
         <v>257</v>
       </c>
-      <c r="F3" s="246"/>
+      <c r="F3" s="255"/>
     </row>
     <row r="4" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="222" t="s">

</xml_diff>